<commit_message>
remove hub from default list
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C365976E-3E83-4B64-BF57-19E4B0A5E277}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CD9F0D-A1D9-4997-B80C-80DA951C0604}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="90">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -729,8 +729,8 @@
   <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1014,12 +1014,8 @@
       <c r="A24" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="6" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
add inkscape to choco
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A33834-45FD-45E4-A517-446A7B376E92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACF761D-E893-4F80-B139-7835CEC4B9C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$E$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$E$88</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="99">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -319,6 +319,9 @@
   </si>
   <si>
     <t>Insbesondere für vim</t>
+  </si>
+  <si>
+    <t>inkscape</t>
   </si>
 </sst>
 </file>
@@ -753,11 +756,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E87"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E74" sqref="E74"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,82 +1115,82 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="B32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" s="3"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B33" s="3"/>
       <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
+      <c r="D33" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="B35" s="3"/>
+      <c r="C35" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="B36" s="3"/>
       <c r="C36" s="3"/>
-      <c r="D36" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="D36" s="3"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D37" s="3"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>56</v>
@@ -1199,61 +1202,63 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D39" s="3"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="B40" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D40" s="3"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
+      <c r="B41" s="3"/>
+      <c r="C41" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="B42" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C43" s="3"/>
+      <c r="C43" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D43" s="3"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>56</v>
@@ -1263,7 +1268,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>56</v>
@@ -1272,8 +1277,8 @@
       <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>78</v>
+      <c r="A46" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>56</v>
@@ -1283,7 +1288,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>56</v>
@@ -1292,8 +1297,8 @@
       <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>27</v>
+      <c r="A48" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>56</v>
@@ -1302,20 +1307,18 @@
       <c r="D48" s="3"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>64</v>
+      <c r="A49" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="C49" s="3"/>
       <c r="D49" s="3"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>56</v>
@@ -1323,31 +1326,35 @@
       <c r="C50" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D50" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="D50" s="3"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
+      <c r="D52" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -1355,7 +1362,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -1363,35 +1370,33 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B55" s="3"/>
-      <c r="C55" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="C55" s="3"/>
       <c r="D55" s="3"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
+      <c r="C56" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D56" s="3"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>56</v>
@@ -1400,45 +1405,45 @@
       <c r="D58" s="3"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B59" s="3"/>
+      <c r="A59" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B60" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D60" s="3"/>
-      <c r="E60" s="8" t="s">
+      <c r="B61" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D61" s="3"/>
+      <c r="E61" s="8" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D61" s="3"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B62" s="3"/>
+        <v>87</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C62" s="3" t="s">
         <v>56</v>
       </c>
@@ -1446,7 +1451,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
       <c r="B63" s="3"/>
       <c r="C63" s="3" t="s">
@@ -1456,43 +1461,43 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
+      <c r="C64" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D64" s="3"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B66" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>56</v>
@@ -1502,77 +1507,77 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C69" s="3"/>
-      <c r="D69" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="D69" s="3"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C72" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="C72" s="3"/>
       <c r="D72" s="3"/>
-      <c r="E72" s="7" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D73" s="3"/>
+      <c r="E73" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B73" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D73" s="3"/>
-      <c r="E73" s="9" t="s">
+      <c r="B74" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D74" s="3"/>
+      <c r="E74" s="9" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>56</v>
@@ -1582,15 +1587,17 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B76" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -1598,101 +1605,99 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B78" s="3"/>
       <c r="C78" s="3"/>
-      <c r="D78" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="D78" s="3"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B79" s="3"/>
-      <c r="C79" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D79" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D80" s="3"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="B81" s="3"/>
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>50</v>
+      <c r="A82" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C82" s="3"/>
-      <c r="D82" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="D82" s="3"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C83" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D84" s="3"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B84" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C84" s="3"/>
-      <c r="D84" s="3"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="4" t="s">
+      <c r="B85" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B85" s="3"/>
-      <c r="C85" s="3"/>
-      <c r="D85" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="B86" s="3"/>
       <c r="C86" s="3"/>
-      <c r="D86" s="3"/>
+      <c r="D86" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>56</v>
@@ -1700,8 +1705,18 @@
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
     </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E87" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E88" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
migrate to windows terminal 0.11
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CD249B-1175-4004-AD9F-5F6AEA8CBD37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65139A02-EA5A-4C78-9C7E-51DA42E8ACA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="255" windowWidth="38640" windowHeight="20865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3990" yWindow="1350" windowWidth="28800" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="106">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -297,9 +297,6 @@
     <t>GitHub</t>
   </si>
   <si>
-    <t>adoptopenjdk12</t>
-  </si>
-  <si>
     <t>adoptopenjdk11</t>
   </si>
   <si>
@@ -340,6 +337,12 @@
   </si>
   <si>
     <t>insomnia-rest-api-client</t>
+  </si>
+  <si>
+    <t>Gute Alternative: qview</t>
+  </si>
+  <si>
+    <t>adoptopenjdk14</t>
   </si>
 </sst>
 </file>
@@ -413,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -435,6 +438,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -774,11 +780,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E94"/>
+  <dimension ref="A1:F94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,7 +852,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
@@ -856,20 +862,24 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -884,7 +894,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -894,7 +904,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -904,7 +914,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -966,7 +976,7 @@
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>82</v>
       </c>
@@ -978,7 +988,7 @@
       </c>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -990,7 +1000,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -998,7 +1008,7 @@
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -1008,7 +1018,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
@@ -1020,7 +1030,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
@@ -1034,7 +1044,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>68</v>
       </c>
@@ -1048,8 +1058,11 @@
       <c r="E23" s="6" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>57</v>
       </c>
@@ -1060,7 +1073,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>62</v>
       </c>
@@ -1072,7 +1085,7 @@
       </c>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>11</v>
       </c>
@@ -1080,9 +1093,9 @@
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>56</v>
@@ -1090,10 +1103,10 @@
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>12</v>
       </c>
@@ -1107,7 +1120,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>13</v>
       </c>
@@ -1117,7 +1130,7 @@
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>14</v>
       </c>
@@ -1129,7 +1142,7 @@
       </c>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>88</v>
       </c>
@@ -1140,7 +1153,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>15</v>
       </c>
@@ -1164,7 +1177,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>56</v>
@@ -1176,7 +1189,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3" t="s">
@@ -1272,7 +1285,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>56</v>
@@ -1420,7 +1433,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>56</v>
@@ -1494,7 +1507,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>56</v>
@@ -1644,7 +1657,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>56</v>
@@ -1654,7 +1667,7 @@
       </c>
       <c r="D80" s="3"/>
       <c r="E80" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update choco and remap key to AltGr
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D7854C-9198-47CA-82A8-15B6FDE68AFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06534203-93D3-4609-A7A2-1CEB0EBB22D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="106">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -783,8 +783,8 @@
   <dimension ref="A1:F94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,7 +1193,9 @@
       <c r="A35" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B35" s="3"/>
+      <c r="B35" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C35" s="3" t="s">
         <v>56</v>
       </c>

</xml_diff>

<commit_message>
update packages available for winget
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06534203-93D3-4609-A7A2-1CEB0EBB22D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E834C6B-B674-4751-9D52-356DDEF1D2F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$E$94</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$F$106</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="123">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -234,9 +234,6 @@
     <t>fsviewer</t>
   </si>
   <si>
-    <t>FastStone Image Viewer</t>
-  </si>
-  <si>
     <t>twitch</t>
   </si>
   <si>
@@ -342,7 +339,84 @@
     <t>adoptopenjdk14</t>
   </si>
   <si>
-    <t>Gute Alternative: qView</t>
+    <r>
+      <t xml:space="preserve">FastStone Image Viewer (alternativ: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>qView</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>!)</t>
+    </r>
+  </si>
+  <si>
+    <t>Bemerkungen</t>
+  </si>
+  <si>
+    <t>gh/microsoft/winget-pkgs</t>
+  </si>
+  <si>
+    <t>etcher</t>
+  </si>
+  <si>
+    <t>Balena Etcher</t>
+  </si>
+  <si>
+    <t>awscli</t>
+  </si>
+  <si>
+    <t>cryptomator</t>
+  </si>
+  <si>
+    <t>epicgameslauncher</t>
+  </si>
+  <si>
+    <t>gh</t>
+  </si>
+  <si>
+    <t>GitHub CLI, offizieller Nachfolger von hub</t>
+  </si>
+  <si>
+    <t>meld</t>
+  </si>
+  <si>
+    <t>Visual Diff</t>
+  </si>
+  <si>
+    <t>powertoys</t>
+  </si>
+  <si>
+    <t>microsoft-teams</t>
+  </si>
+  <si>
+    <t>microsoft-windows-terminal</t>
+  </si>
+  <si>
+    <t>vnc-viewer</t>
+  </si>
+  <si>
+    <t>franz</t>
+  </si>
+  <si>
+    <t>winscp</t>
+  </si>
+  <si>
+    <t>zoom</t>
   </si>
 </sst>
 </file>
@@ -366,7 +440,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -379,8 +453,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -403,20 +483,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -430,17 +501,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -780,37 +854,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F94"/>
+  <dimension ref="A1:F107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>59</v>
       </c>
@@ -823,8 +904,12 @@
       <c r="D2" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -835,8 +920,10 @@
       <c r="D3" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="7"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>60</v>
       </c>
@@ -849,30 +936,40 @@
       <c r="D4" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="7"/>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
         <v>56</v>
       </c>
       <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
         <v>56</v>
       </c>
       <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>56</v>
@@ -881,8 +978,12 @@
         <v>56</v>
       </c>
       <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
@@ -891,38 +992,46 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="7"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="7"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="7"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="7"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>61</v>
       </c>
@@ -933,206 +1042,250 @@
         <v>56</v>
       </c>
       <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>2</v>
+      <c r="E12" s="7"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
         <v>56</v>
       </c>
       <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="B15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="B16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
       <c r="D17" s="3"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18" s="11" t="s">
         <v>56</v>
       </c>
       <c r="C18" s="3"/>
-      <c r="D18" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
+      <c r="A19" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D19" s="3"/>
+      <c r="E19" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22" s="8"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23" s="3" t="s">
+      <c r="A23" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>56</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>105</v>
+      <c r="D23" s="3"/>
+      <c r="E23" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24" s="3"/>
+      <c r="A24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="6" t="s">
-        <v>58</v>
-      </c>
+      <c r="E24" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>62</v>
+      <c r="A25" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="8"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="8"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>93</v>
+      <c r="A27" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="6" t="s">
-        <v>94</v>
+      <c r="D27" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="8" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>56</v>
+      <c r="A28" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="3"/>
+      <c r="A29" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D29" s="3"/>
+      <c r="E29" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>14</v>
+      <c r="A30" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>56</v>
@@ -1141,227 +1294,286 @@
         <v>56</v>
       </c>
       <c r="D30" s="3"/>
+      <c r="E30" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="8"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>88</v>
+        <v>11</v>
       </c>
       <c r="B31" s="3"/>
-      <c r="C31" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="C31" s="3"/>
       <c r="D31" s="3"/>
-      <c r="E31" s="6" t="s">
-        <v>89</v>
-      </c>
+      <c r="E31" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F31" s="8"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F33" s="8"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="8"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="8"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="8"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+      <c r="B38" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E38" s="7"/>
+      <c r="F38" s="8"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" s="3"/>
+      <c r="E39" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F39" s="8"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F40" s="8"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="8"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E42" s="7"/>
+      <c r="F42" s="8"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="8"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="8"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D39" s="3"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="8"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+      <c r="B46" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E46" s="7"/>
+      <c r="F46" s="8"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D42" s="3"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="B47" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D47" s="3"/>
+      <c r="E47" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F47" s="8"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D43" s="3"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D44" s="3"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="B48" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D48" s="3"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="8"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D49" s="3"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="8"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D45" s="3"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D47" s="3"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D50" s="3"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" s="7"/>
+      <c r="F50" s="8"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>78</v>
       </c>
@@ -1370,30 +1582,40 @@
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="7"/>
+      <c r="F51" s="8"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B52" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B52" s="11" t="s">
         <v>56</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F52" s="8"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C53" s="3"/>
+      <c r="C53" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D53" s="3"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
-        <v>64</v>
+      <c r="E53" s="7"/>
+      <c r="F53" s="8"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>56</v>
@@ -1402,129 +1624,179 @@
         <v>56</v>
       </c>
       <c r="D54" s="3"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>65</v>
+      <c r="E54" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C55" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>71</v>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="8"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
-      <c r="D56" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="3"/>
+      <c r="E56" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F56" s="8"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B57" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" s="7"/>
+      <c r="F57" s="8"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="B58" s="3"/>
       <c r="C58" s="3" t="s">
         <v>56</v>
       </c>
       <c r="D58" s="3"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F58" s="8"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
+        <v>118</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D59" s="3"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B60" s="3"/>
+      <c r="E59" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F59" s="8"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="E60" s="7"/>
+      <c r="F60" s="8"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C61" s="3"/>
       <c r="D61" s="3"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F61" s="8"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B62" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>33</v>
+      <c r="E62" s="7"/>
+      <c r="F62" s="8"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C63" s="3"/>
+      <c r="C63" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D63" s="3"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>34</v>
+      <c r="E63" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F63" s="8"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C64" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E64" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F64" s="8"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
+      <c r="D65" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F65" s="8"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="7"/>
+      <c r="F66" s="8"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B66" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D66" s="3"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="B67" s="3" t="s">
         <v>56</v>
       </c>
@@ -1532,241 +1804,294 @@
         <v>56</v>
       </c>
       <c r="D67" s="3"/>
-      <c r="E67" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E67" s="7"/>
+      <c r="F67" s="8"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
       <c r="D68" s="3"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E68" s="7"/>
+      <c r="F68" s="8"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="B69" s="3"/>
-      <c r="C69" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="C69" s="3"/>
       <c r="D69" s="3"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E69" s="7"/>
+      <c r="F69" s="8"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B70" s="3"/>
       <c r="C70" s="3" t="s">
         <v>56</v>
       </c>
       <c r="D70" s="3"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E70" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F70" s="8"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E71" s="7"/>
+      <c r="F71" s="8"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>37</v>
+        <v>116</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C72" s="3"/>
+      <c r="C72" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D72" s="3"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E72" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F72" s="8"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B73" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E73" s="7"/>
+      <c r="F73" s="8"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="E74" s="7"/>
+      <c r="F74" s="8"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>41</v>
+      <c r="E75" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F75" s="8"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>100</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C76" s="3"/>
-      <c r="D76" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B77" s="3"/>
-      <c r="C77" s="3"/>
+      <c r="C76" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D76" s="3"/>
+      <c r="E76" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F76" s="8"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D77" s="3"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
-        <v>70</v>
+      <c r="E77" s="7"/>
+      <c r="F77" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C78" s="3"/>
+      <c r="C78" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D78" s="3"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="E78" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F78" s="8"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B79" s="3"/>
       <c r="C79" s="3" t="s">
         <v>56</v>
       </c>
       <c r="D79" s="3"/>
-      <c r="E79" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="E79" s="7"/>
+      <c r="F79" s="8"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B80" s="3"/>
       <c r="C80" s="3" t="s">
         <v>56</v>
       </c>
       <c r="D80" s="3"/>
-      <c r="E80" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F80" s="8"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B81" s="3"/>
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81" s="7"/>
+      <c r="F81" s="8"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F82" s="8"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
       <c r="D83" s="3"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F83" s="8"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B84" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C84" s="3"/>
       <c r="D84" s="3"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84" s="7"/>
+      <c r="F84" s="8"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C85" s="3"/>
-      <c r="D85" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D85" s="3"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="8"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D86" s="3"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E86" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F86" s="8"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87" s="7"/>
+      <c r="F87" s="8"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C88" s="3"/>
       <c r="D88" s="3"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>50</v>
+      <c r="E88" s="7"/>
+      <c r="F88" s="8"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C89" s="3"/>
-      <c r="D89" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
-        <v>51</v>
+      <c r="C89" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D89" s="3"/>
+      <c r="E89" s="7"/>
+      <c r="F89" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
+        <v>94</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>56</v>
@@ -1775,51 +2100,238 @@
         <v>56</v>
       </c>
       <c r="D90" s="3"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90" s="7"/>
+      <c r="F90" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B92" s="3"/>
+      <c r="E91" s="7"/>
+      <c r="F91" s="8"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C92" s="3"/>
-      <c r="D92" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D92" s="3"/>
+      <c r="E92" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F92" s="8"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B93" s="3"/>
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93" s="7"/>
+      <c r="F93" s="8"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B94" s="3"/>
       <c r="C94" s="3"/>
       <c r="D94" s="3"/>
+      <c r="E94" s="7"/>
+      <c r="F94" s="8"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E95" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F95" s="8"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B96" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F96" s="8"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D97" s="3"/>
+      <c r="E97" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F97" s="8"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B98" s="3"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
+      <c r="E98" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F98" s="8"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="7"/>
+      <c r="F99" s="8"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C100" s="3"/>
+      <c r="D100" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E100" s="7"/>
+      <c r="F100" s="8"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D101" s="3"/>
+      <c r="E101" s="7"/>
+      <c r="F101" s="8"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C102" s="3"/>
+      <c r="D102" s="3"/>
+      <c r="E102" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F102" s="8"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B103" s="3"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
+      <c r="E103" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F103" s="8"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B104" s="3"/>
+      <c r="C104" s="3"/>
+      <c r="D104" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E104" s="7"/>
+      <c r="F104" s="8"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C105" s="3"/>
+      <c r="D105" s="3"/>
+      <c r="E105" s="7"/>
+      <c r="F105" s="8"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
+      <c r="E106" s="7"/>
+      <c r="F106" s="8"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B107" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C107" s="3"/>
+      <c r="D107" s="3"/>
+      <c r="E107" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F107" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E94" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:F106" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <hyperlinks>
+    <hyperlink ref="E1" r:id="rId1" display="https://github.com/microsoft/winget-pkgs" xr:uid="{2C434A13-8B1C-492F-95C8-B89737A54984}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add tooling & add fzf bindings
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12FAE8B-960A-47EA-8D6F-CD5C9969F307}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE88875F-8144-41A4-BFA4-D22B4D40FB77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,14 +18,14 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$F$107</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$F$111</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="131">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -418,12 +418,36 @@
   <si>
     <t>zoom</t>
   </si>
+  <si>
+    <t>bat</t>
+  </si>
+  <si>
+    <t>Better cat, https://github.com/sharkdp/bat</t>
+  </si>
+  <si>
+    <t>fd</t>
+  </si>
+  <si>
+    <t>https://github.com/sharkdp/fd</t>
+  </si>
+  <si>
+    <t>ripgrep</t>
+  </si>
+  <si>
+    <t>https://github.com/BurntSushi/ripgrep</t>
+  </si>
+  <si>
+    <t>starship</t>
+  </si>
+  <si>
+    <t>https://starship.rs/</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -454,8 +478,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -471,6 +502,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -498,11 +534,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -534,8 +571,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Gut" xfId="2" builtinId="26"/>
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -873,11 +912,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F107"/>
+  <dimension ref="A1:F111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F87" sqref="F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1091,67 +1130,67 @@
       <c r="F14" s="8"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>3</v>
+      <c r="A15" s="13" t="s">
+        <v>123</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="C15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="3"/>
       <c r="E15" s="7"/>
-      <c r="F15" s="8"/>
+      <c r="F15" s="8" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E16" s="7"/>
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D17" s="3"/>
       <c r="E17" s="7"/>
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>56</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="E18" s="7"/>
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="A19" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="7" t="s">
         <v>56</v>
@@ -1159,46 +1198,48 @@
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>6</v>
+      <c r="A20" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="7"/>
+      <c r="C20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E21" s="7"/>
       <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>56</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="E22" s="7"/>
       <c r="F22" s="8"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>56</v>
@@ -1208,15 +1249,13 @@
       <c r="E23" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F23" s="8" t="s">
-        <v>108</v>
-      </c>
+      <c r="F23" s="8"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B24" s="11" t="s">
         <v>56</v>
       </c>
       <c r="C24" s="3"/>
@@ -1224,43 +1263,43 @@
       <c r="E24" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F24" s="8"/>
+      <c r="F24" s="8" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="8"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F26" s="8"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>56</v>
@@ -1270,95 +1309,97 @@
         <v>56</v>
       </c>
       <c r="E27" s="7"/>
-      <c r="F27" s="8" t="s">
-        <v>104</v>
-      </c>
+      <c r="F27" s="8"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="8" t="s">
-        <v>58</v>
-      </c>
+      <c r="A28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" s="8"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29" s="7"/>
+      <c r="F29" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F30" s="8"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
+      <c r="C31" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D31" s="3"/>
       <c r="E31" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F31" s="8"/>
+      <c r="F31" s="8" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>92</v>
+      <c r="A32" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C32" s="3"/>
+      <c r="C32" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D32" s="3"/>
       <c r="E32" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F32" s="8" t="s">
-        <v>93</v>
-      </c>
+      <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
       <c r="E33" s="7" t="s">
         <v>56</v>
       </c>
@@ -1366,19 +1407,23 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="8"/>
+      <c r="E34" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>56</v>
@@ -1386,85 +1431,83 @@
       <c r="C35" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="7"/>
+      <c r="D35" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F35" s="8"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="7"/>
-      <c r="F36" s="8" t="s">
-        <v>88</v>
-      </c>
+      <c r="F36" s="8"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C37" s="3"/>
+      <c r="C37" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D37" s="3"/>
       <c r="E37" s="7"/>
       <c r="F37" s="8"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38" s="3"/>
       <c r="E38" s="7"/>
-      <c r="F38" s="8"/>
+      <c r="F38" s="8" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>96</v>
+        <v>15</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="C39" s="3"/>
       <c r="D39" s="3"/>
-      <c r="E39" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="E39" s="7"/>
       <c r="F39" s="8"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>102</v>
+        <v>16</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D40" s="3"/>
-      <c r="E40" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E40" s="7"/>
       <c r="F40" s="8"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>82</v>
+      <c r="A41" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>56</v>
@@ -1473,50 +1516,60 @@
         <v>56</v>
       </c>
       <c r="D41" s="3"/>
-      <c r="E41" s="7"/>
+      <c r="E41" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F41" s="8"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E42" s="7"/>
+        <v>102</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D42" s="3"/>
+      <c r="E42" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F42" s="8"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>18</v>
+      <c r="A43" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C43" s="3"/>
+      <c r="C43" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D43" s="3"/>
       <c r="E43" s="7"/>
       <c r="F43" s="8"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B44" s="3"/>
-      <c r="C44" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E44" s="7"/>
       <c r="F44" s="8"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B45" s="3"/>
+      <c r="A45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="7"/>
@@ -1524,51 +1577,43 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D46" s="3"/>
       <c r="E46" s="7"/>
       <c r="F46" s="8"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
       <c r="D47" s="3"/>
-      <c r="E47" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="E47" s="7"/>
       <c r="F47" s="8"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E48" s="7"/>
       <c r="F48" s="8"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>56</v>
@@ -1577,14 +1622,18 @@
         <v>56</v>
       </c>
       <c r="D49" s="3"/>
-      <c r="E49" s="7"/>
+      <c r="E49" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F49" s="8"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B50" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C50" s="3" t="s">
         <v>56</v>
       </c>
@@ -1594,89 +1643,91 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C51" s="3"/>
+      <c r="C51" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D51" s="3"/>
       <c r="E51" s="7"/>
       <c r="F51" s="8"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C52" s="3"/>
+      <c r="A52" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D52" s="3"/>
-      <c r="E52" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="E52" s="7"/>
       <c r="F52" s="8"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>23</v>
+      <c r="A53" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C53" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="7"/>
       <c r="F53" s="8"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="A54" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F54" s="8" t="s">
-        <v>115</v>
-      </c>
+      <c r="F54" s="8"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C55" s="3"/>
+      <c r="C55" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D55" s="3"/>
       <c r="E55" s="7"/>
       <c r="F55" s="8"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
+        <v>114</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D56" s="3"/>
       <c r="E56" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F56" s="8"/>
+      <c r="F56" s="8" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>56</v>
@@ -1688,12 +1739,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>117</v>
+        <v>25</v>
       </c>
       <c r="B58" s="3"/>
-      <c r="C58" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="7" t="s">
         <v>56</v>
@@ -1702,40 +1751,40 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="8"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D60" s="3"/>
+      <c r="E60" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F60" s="8"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D59" s="3"/>
-      <c r="E59" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F59" s="8"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="8"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>84</v>
-      </c>
       <c r="B61" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C61" s="3"/>
+      <c r="C61" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D61" s="3"/>
       <c r="E61" s="7" t="s">
         <v>56</v>
@@ -1743,8 +1792,8 @@
       <c r="F61" s="8"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>27</v>
+      <c r="A62" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>56</v>
@@ -1756,14 +1805,12 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C63" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="C63" s="3"/>
       <c r="D63" s="3"/>
       <c r="E63" s="7" t="s">
         <v>56</v>
@@ -1771,64 +1818,68 @@
       <c r="F63" s="8"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
-        <v>65</v>
+      <c r="A64" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C64" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E64" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="7"/>
       <c r="F64" s="8"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D65" s="3"/>
+      <c r="E65" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F65" s="8"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E66" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F66" s="8"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E65" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F65" s="8"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="7"/>
-      <c r="F66" s="8"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D67" s="3"/>
-      <c r="E67" s="7"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F67" s="8"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -1838,31 +1889,31 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B69" s="3"/>
-      <c r="C69" s="3"/>
+        <v>101</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D69" s="3"/>
       <c r="E69" s="7"/>
       <c r="F69" s="8"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B70" s="3"/>
-      <c r="C70" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="C70" s="3"/>
       <c r="D70" s="3"/>
-      <c r="E70" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="E70" s="7"/>
       <c r="F70" s="8"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -1872,11 +1923,9 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B72" s="3"/>
       <c r="C72" s="3" t="s">
         <v>56</v>
       </c>
@@ -1888,11 +1937,9 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
       <c r="E73" s="7"/>
@@ -1900,63 +1947,59 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>34</v>
+        <v>116</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C74" s="3"/>
+      <c r="C74" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D74" s="3"/>
-      <c r="E74" s="7"/>
+      <c r="E74" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F74" s="8"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B75" s="3"/>
+      <c r="A75" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
-      <c r="E75" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="E75" s="7"/>
       <c r="F75" s="8"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
-        <v>100</v>
+      <c r="A76" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C76" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="C76" s="3"/>
       <c r="D76" s="3"/>
-      <c r="E76" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="E76" s="7"/>
       <c r="F76" s="8"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
       <c r="D77" s="3"/>
-      <c r="E77" s="7"/>
-      <c r="F77" s="9" t="s">
-        <v>80</v>
-      </c>
+      <c r="E77" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F77" s="8"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>86</v>
+      <c r="A78" s="4" t="s">
+        <v>100</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>56</v>
@@ -1971,61 +2014,73 @@
       <c r="F78" s="8"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B79" s="3"/>
+      <c r="A79" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C79" s="3" t="s">
         <v>56</v>
       </c>
       <c r="D79" s="3"/>
       <c r="E79" s="7"/>
-      <c r="F79" s="8"/>
+      <c r="F79" s="8" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B80" s="3"/>
+      <c r="A80" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C80" s="3" t="s">
         <v>56</v>
       </c>
       <c r="D80" s="3"/>
-      <c r="E80" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F80" s="8"/>
+      <c r="E80" s="7"/>
+      <c r="F80" s="9" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B81" s="3"/>
-      <c r="C81" s="3"/>
+        <v>86</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D81" s="3"/>
-      <c r="E81" s="7"/>
+      <c r="E81" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F81" s="8"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C82" s="3"/>
+        <v>85</v>
+      </c>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D82" s="3"/>
-      <c r="E82" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="E82" s="7"/>
       <c r="F82" s="8"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
+      <c r="C83" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D83" s="3"/>
       <c r="E83" s="7" t="s">
         <v>56</v>
@@ -2034,11 +2089,9 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B84" s="3"/>
       <c r="C84" s="3"/>
       <c r="D84" s="3"/>
       <c r="E84" s="7"/>
@@ -2046,43 +2099,49 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C85" s="3"/>
       <c r="D85" s="3"/>
-      <c r="E85" s="7"/>
+      <c r="E85" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F85" s="8"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
-      <c r="D86" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="D86" s="3"/>
       <c r="E86" s="7" t="s">
         <v>56</v>
       </c>
       <c r="F86" s="8"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B87" s="3"/>
-      <c r="C87" s="3"/>
+      <c r="A87" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D87" s="3"/>
       <c r="E87" s="7"/>
-      <c r="F87" s="8"/>
+      <c r="F87" s="8" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="4" t="s">
-        <v>69</v>
+      <c r="A88" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>56</v>
@@ -2093,104 +2152,102 @@
       <c r="F88" s="8"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="4" t="s">
-        <v>75</v>
+      <c r="A89" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C89" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="C89" s="3"/>
       <c r="D89" s="3"/>
       <c r="E89" s="7"/>
-      <c r="F89" s="10" t="s">
-        <v>76</v>
-      </c>
+      <c r="F89" s="8"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D90" s="3"/>
-      <c r="E90" s="7"/>
-      <c r="F90" s="10" t="s">
-        <v>95</v>
-      </c>
+      <c r="A90" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E90" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F90" s="8"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B91" s="3"/>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
       <c r="E91" s="7"/>
       <c r="F91" s="8"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>44</v>
+      <c r="A92" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="3"/>
-      <c r="E92" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="E92" s="7"/>
       <c r="F92" s="8"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B93" s="3"/>
-      <c r="C93" s="3"/>
+      <c r="A93" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D93" s="3"/>
       <c r="E93" s="7"/>
-      <c r="F93" s="8"/>
+      <c r="F93" s="10" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B94" s="3"/>
-      <c r="C94" s="3"/>
+      <c r="A94" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D94" s="3"/>
       <c r="E94" s="7"/>
-      <c r="F94" s="8"/>
+      <c r="F94" s="10" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C95" s="3"/>
-      <c r="D95" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E95" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="D95" s="3"/>
+      <c r="E95" s="7"/>
       <c r="F95" s="8"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B96" s="11" t="s">
+      <c r="A96" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B96" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C96" s="3"/>
@@ -2202,61 +2259,57 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B97" s="3"/>
+      <c r="C97" s="3"/>
       <c r="D97" s="3"/>
-      <c r="E97" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="E97" s="7"/>
       <c r="F97" s="8"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
       <c r="D98" s="3"/>
-      <c r="E98" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="E98" s="7"/>
       <c r="F98" s="8"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="4" t="s">
-        <v>74</v>
+      <c r="A99" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C99" s="3"/>
-      <c r="D99" s="3"/>
-      <c r="E99" s="7"/>
+      <c r="D99" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E99" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F99" s="8"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B100" s="3" t="s">
+      <c r="A100" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B100" s="11" t="s">
         <v>56</v>
       </c>
       <c r="C100" s="3"/>
-      <c r="D100" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E100" s="7"/>
+      <c r="D100" s="3"/>
+      <c r="E100" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F100" s="8"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>56</v>
@@ -2265,16 +2318,16 @@
         <v>56</v>
       </c>
       <c r="D101" s="3"/>
-      <c r="E101" s="7"/>
+      <c r="E101" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F101" s="8"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="B102" s="3"/>
       <c r="C102" s="3"/>
       <c r="D102" s="3"/>
       <c r="E102" s="7" t="s">
@@ -2283,22 +2336,24 @@
       <c r="F102" s="8"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B103" s="3"/>
+      <c r="A103" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C103" s="3"/>
       <c r="D103" s="3"/>
-      <c r="E103" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="E103" s="7"/>
       <c r="F103" s="8"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B104" s="3"/>
+      <c r="A104" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C104" s="3"/>
       <c r="D104" s="3" t="s">
         <v>56</v>
@@ -2308,35 +2363,37 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C105" s="3"/>
+      <c r="C105" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D105" s="3"/>
       <c r="E105" s="7"/>
       <c r="F105" s="8"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C106" s="3"/>
       <c r="D106" s="3"/>
-      <c r="E106" s="7"/>
+      <c r="E106" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F106" s="8"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B107" s="11" t="s">
-        <v>56</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="B107" s="3"/>
       <c r="C107" s="3"/>
       <c r="D107" s="3"/>
       <c r="E107" s="7" t="s">
@@ -2344,8 +2401,58 @@
       </c>
       <c r="F107" s="8"/>
     </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B108" s="3"/>
+      <c r="C108" s="3"/>
+      <c r="D108" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E108" s="7"/>
+      <c r="F108" s="8"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C109" s="3"/>
+      <c r="D109" s="3"/>
+      <c r="E109" s="7"/>
+      <c r="F109" s="8"/>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C110" s="3"/>
+      <c r="D110" s="3"/>
+      <c r="E110" s="7"/>
+      <c r="F110" s="8"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B111" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C111" s="3"/>
+      <c r="D111" s="3"/>
+      <c r="E111" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F111" s="8"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F107" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:F111" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="E1" r:id="rId1" display="https://github.com/microsoft/winget-pkgs" xr:uid="{2C434A13-8B1C-492F-95C8-B89737A54984}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
migrate to CaskaydiaCove NF installed from chocolatey
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\ubuntu\projects\wiki\Settings\Chocolatey\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FCC2E1-2BEB-48BA-A170-71E80E6D10C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A7CA1E-F49A-42EE-BE0E-4C34BD0366B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="140">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -966,8 +966,8 @@
   <dimension ref="A1:F120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,21 +1195,17 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="7"/>
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="4" t="s">
         <v>134</v>
       </c>
       <c r="B17" s="3" t="s">

</xml_diff>

<commit_message>
update available winget packages
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\wiki\Settings\Chocolatey\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\ubuntu\projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3AB2BB8-54CB-476F-A7F3-059C33474C27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C45F5A-A8A8-4360-8634-324C6CB1CD8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="141">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -625,10 +625,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Gut" xfId="1" builtinId="26"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
-    <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -649,7 +649,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -972,11 +972,11 @@
   <dimension ref="A1:F120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E116" sqref="E116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
@@ -1051,7 +1051,9 @@
       <c r="D4" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1117,7 +1119,9 @@
       <c r="D9" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1155,7 +1159,9 @@
         <v>56</v>
       </c>
       <c r="D12" s="3"/>
-      <c r="E12" s="7"/>
+      <c r="E12" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1235,7 +1241,9 @@
       <c r="D18" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="7"/>
+      <c r="E18" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1415,7 +1423,9 @@
       <c r="D31" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E31" s="7"/>
+      <c r="E31" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F31" s="8" t="s">
         <v>104</v>
       </c>
@@ -1523,7 +1533,9 @@
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
-      <c r="E38" s="7"/>
+      <c r="E38" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F38" s="8"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1563,7 +1575,9 @@
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
-      <c r="E41" s="7"/>
+      <c r="E41" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F41" s="8"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1637,7 +1651,9 @@
       <c r="D46" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E46" s="7"/>
+      <c r="E46" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F46" s="8"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1685,7 +1701,9 @@
       <c r="D50" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E50" s="7"/>
+      <c r="E50" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F50" s="8"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1715,7 +1733,9 @@
         <v>56</v>
       </c>
       <c r="D52" s="3"/>
-      <c r="E52" s="7"/>
+      <c r="E52" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F52" s="8"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1751,7 +1771,9 @@
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
-      <c r="E55" s="7"/>
+      <c r="E55" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F55" s="8" t="s">
         <v>132</v>
       </c>
@@ -1847,7 +1869,9 @@
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
-      <c r="E62" s="7"/>
+      <c r="E62" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F62" s="8"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -1913,7 +1937,9 @@
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
-      <c r="E67" s="7"/>
+      <c r="E67" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F67" s="8"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -1971,7 +1997,9 @@
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
-      <c r="E71" s="7"/>
+      <c r="E71" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F71" s="8"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -2005,7 +2033,9 @@
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
-      <c r="E74" s="7"/>
+      <c r="E74" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F74" s="8"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2181,7 +2211,9 @@
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
-      <c r="E87" s="7"/>
+      <c r="E87" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F87" s="8"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2247,7 +2279,9 @@
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="3"/>
-      <c r="E92" s="7"/>
+      <c r="E92" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F92" s="8"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -2271,7 +2305,9 @@
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
       <c r="D94" s="3"/>
-      <c r="E94" s="7"/>
+      <c r="E94" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F94" s="8"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2283,7 +2319,9 @@
       </c>
       <c r="C95" s="3"/>
       <c r="D95" s="3"/>
-      <c r="E95" s="7"/>
+      <c r="E95" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F95" s="8"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2293,7 +2331,9 @@
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
       <c r="D96" s="3"/>
-      <c r="E96" s="7"/>
+      <c r="E96" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F96" s="8"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -2361,7 +2401,9 @@
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
       <c r="D101" s="3"/>
-      <c r="E101" s="7"/>
+      <c r="E101" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F101" s="8"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -2441,7 +2483,9 @@
       </c>
       <c r="C107" s="3"/>
       <c r="D107" s="3"/>
-      <c r="E107" s="7"/>
+      <c r="E107" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F107" s="8"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -2455,7 +2499,9 @@
       <c r="D108" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E108" s="7"/>
+      <c r="E108" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F108" s="8"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
@@ -2469,7 +2515,9 @@
         <v>56</v>
       </c>
       <c r="D109" s="3"/>
-      <c r="E109" s="7"/>
+      <c r="E109" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F109" s="8"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -2517,7 +2565,9 @@
       <c r="D113" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E113" s="7"/>
+      <c r="E113" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="F113" s="8"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -2589,7 +2639,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2601,7 +2651,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add choco list for seconday Computer
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\ubuntu\projects\wiki\Settings\Chocolatey\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C45F5A-A8A8-4360-8634-324C6CB1CD8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E2825F-01BC-4789-8AC8-09F4126A12BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3465" yWindow="3630" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$F$116</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$G$116</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="142">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -471,6 +471,9 @@
   </si>
   <si>
     <t>Not working. Installs to postman's location.</t>
+  </si>
+  <si>
+    <t>Secondary</t>
   </si>
 </sst>
 </file>
@@ -625,10 +628,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Gut" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -649,7 +652,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -969,24 +972,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F120"/>
+  <dimension ref="A1:G120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E116" sqref="E116"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>55</v>
       </c>
@@ -994,19 +998,22 @@
         <v>71</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>59</v>
       </c>
@@ -1019,12 +1026,15 @@
       <c r="D2" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1032,13 +1042,14 @@
         <v>56</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="8"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>60</v>
       </c>
@@ -1051,104 +1062,114 @@
       <c r="D4" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="8"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>90</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>89</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>103</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="3"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="8"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="8"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>61</v>
       </c>
@@ -1158,115 +1179,128 @@
       <c r="C12" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>109</v>
       </c>
       <c r="B13" s="3"/>
-      <c r="C13" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="8"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="3"/>
-      <c r="C14" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>123</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="8" t="s">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="8" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>133</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="8"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E16" s="3"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>134</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="8"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="8"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="8"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E19" s="3"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="8"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="8"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E20" s="3"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="8"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>110</v>
       </c>
@@ -1275,28 +1309,30 @@
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" s="8"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E21" s="3"/>
+      <c r="F21" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>81</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>6</v>
       </c>
@@ -1304,97 +1340,110 @@
         <v>56</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="8"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D23" s="3"/>
+      <c r="E23" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="8"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E24" s="3"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="8"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>111</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="3"/>
+      <c r="C25" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="D25" s="3"/>
-      <c r="E25" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F25" s="8"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E25" s="3"/>
+      <c r="F25" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="3"/>
+      <c r="C26" s="11"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F26" s="8" t="s">
+      <c r="E26" s="3"/>
+      <c r="F26" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G26" s="8" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="3"/>
+      <c r="C27" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D27" s="3"/>
-      <c r="E27" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F27" s="8"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E27" s="3"/>
+      <c r="F27" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27" s="8"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>125</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="8" t="s">
+      <c r="C28" s="3"/>
+      <c r="D28" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="8"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C29" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29" s="7"/>
+      <c r="G29" s="8"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
@@ -1407,106 +1456,119 @@
       <c r="D30" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E30" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F30" s="8"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E30" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" s="8"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>68</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F31" s="8" t="s">
+      <c r="C31" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" s="8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>57</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="8" t="s">
+      <c r="C32" s="3"/>
+      <c r="D32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E32" s="3"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>112</v>
       </c>
       <c r="B33" s="3"/>
-      <c r="C33" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F33" s="8" t="s">
+      <c r="C33" s="3"/>
+      <c r="D33" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E33" s="3"/>
+      <c r="F33" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G33" s="8" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>62</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D34" s="3"/>
-      <c r="E34" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F34" s="8"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C34" s="3"/>
+      <c r="D34" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E34" s="3"/>
+      <c r="F34" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G34" s="8"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
-      <c r="E35" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F35" s="8"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E35" s="3"/>
+      <c r="F35" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G35" s="8"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C36" s="3"/>
+      <c r="C36" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D36" s="3"/>
-      <c r="E36" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F36" s="8" t="s">
+      <c r="E36" s="3"/>
+      <c r="F36" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G36" s="8" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>12</v>
       </c>
@@ -1519,54 +1581,62 @@
       <c r="D37" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E37" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F37" s="8"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E37" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G37" s="8"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C38" s="3"/>
+      <c r="C38" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D38" s="3"/>
-      <c r="E38" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F38" s="8"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E38" s="3"/>
+      <c r="F38" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G38" s="8"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D39" s="3"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="8"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C39" s="3"/>
+      <c r="D39" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E39" s="3"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="8"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
         <v>87</v>
       </c>
       <c r="B40" s="3"/>
-      <c r="C40" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D40" s="3"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="8" t="s">
+      <c r="C40" s="3"/>
+      <c r="D40" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E40" s="3"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>15</v>
       </c>
@@ -1575,26 +1645,30 @@
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
-      <c r="E41" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F41" s="8"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E41" s="3"/>
+      <c r="F41" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G41" s="8"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E42" s="7"/>
-      <c r="F42" s="8"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C42" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F42" s="7"/>
+      <c r="G42" s="8"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>96</v>
       </c>
@@ -1604,109 +1678,123 @@
       <c r="C43" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D43" s="3"/>
-      <c r="E43" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F43" s="8"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D43" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E43" s="3"/>
+      <c r="F43" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G43" s="8"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>102</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F44" s="15" t="s">
+      <c r="C44" s="3"/>
+      <c r="D44" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E44" s="3"/>
+      <c r="F44" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G44" s="15" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>82</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D45" s="3"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="8"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C45" s="3"/>
+      <c r="D45" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E45" s="3"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="8"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
-      <c r="D46" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F46" s="8"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D46" s="3"/>
+      <c r="E46" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G46" s="8"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C47" s="3"/>
+      <c r="C47" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D47" s="3"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="8"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E47" s="3"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="8"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B48" s="3"/>
-      <c r="C48" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D48" s="3"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="8"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C48" s="3"/>
+      <c r="D48" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E48" s="3"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="8"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>83</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="8"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E49" s="3"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="8"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F50" s="8"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C50" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G50" s="8"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>63</v>
       </c>
@@ -1716,13 +1804,16 @@
       <c r="C51" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D51" s="3"/>
-      <c r="E51" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F51" s="8"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D51" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E51" s="3"/>
+      <c r="F51" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G51" s="8"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>21</v>
       </c>
@@ -1732,111 +1823,119 @@
       <c r="C52" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D52" s="3"/>
-      <c r="E52" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F52" s="8"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D52" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E52" s="3"/>
+      <c r="F52" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G52" s="8"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>91</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C53" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D53" s="3"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="8"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C53" s="3"/>
+      <c r="D53" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E53" s="3"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="8"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
         <v>22</v>
       </c>
       <c r="B54" s="3"/>
-      <c r="C54" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D54" s="3"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="8"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C54" s="3"/>
+      <c r="D54" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E54" s="3"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="8"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>131</v>
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
-      <c r="E55" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F55" s="8" t="s">
+      <c r="E55" s="3"/>
+      <c r="F55" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G55" s="8" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>78</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C56" s="3"/>
+      <c r="C56" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D56" s="3"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="8"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E56" s="3"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="8"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>120</v>
       </c>
       <c r="B57" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C57" s="3"/>
+      <c r="C57" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="D57" s="3"/>
-      <c r="E57" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F57" s="8"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E57" s="3"/>
+      <c r="F57" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G57" s="8"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C58" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D58" s="3"/>
-      <c r="E58" s="7"/>
-      <c r="F58" s="8"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C58" s="3"/>
+      <c r="D58" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E58" s="3"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="8"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
       <c r="D59" s="3"/>
-      <c r="E59" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F59" s="8" t="s">
+      <c r="E59" s="3"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="8" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>24</v>
       </c>
@@ -1845,120 +1944,135 @@
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="8"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E60" s="3"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="8"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
-      <c r="E61" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F61" s="8"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E61" s="3"/>
+      <c r="F61" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G61" s="8"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C62" s="3"/>
+      <c r="C62" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D62" s="3"/>
-      <c r="E62" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F62" s="8"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E62" s="3"/>
+      <c r="F62" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G62" s="8"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B63" s="3"/>
-      <c r="C63" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D63" s="3"/>
-      <c r="E63" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F63" s="8"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C63" s="3"/>
+      <c r="D63" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E63" s="3"/>
+      <c r="F63" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G63" s="8"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C64" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D64" s="3"/>
-      <c r="E64" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F64" s="8"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C64" s="3"/>
+      <c r="D64" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E64" s="3"/>
+      <c r="F64" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G64" s="8"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>77</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C65" s="3"/>
+      <c r="C65" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D65" s="3"/>
-      <c r="E65" s="7"/>
-      <c r="F65" s="8"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E65" s="3"/>
+      <c r="F65" s="7"/>
+      <c r="G65" s="8"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>84</v>
       </c>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
-      <c r="E66" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F66" s="8"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E66" s="3"/>
+      <c r="F66" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G66" s="8"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C67" s="3"/>
+      <c r="C67" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D67" s="3"/>
-      <c r="E67" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F67" s="8"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E67" s="3"/>
+      <c r="F67" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G67" s="8"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>64</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C68" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D68" s="3"/>
-      <c r="E68" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F68" s="8"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C68" s="3"/>
+      <c r="D68" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E68" s="3"/>
+      <c r="F68" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G68" s="8"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>65</v>
       </c>
@@ -1971,98 +2085,108 @@
       <c r="D69" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E69" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F69" s="8"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E69" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G69" s="8"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>70</v>
       </c>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
-      <c r="D70" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E70" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F70" s="8"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D70" s="3"/>
+      <c r="E70" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G70" s="8"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
-      <c r="E71" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F71" s="8"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E71" s="3"/>
+      <c r="F71" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G71" s="8"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C72" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D72" s="3"/>
-      <c r="E72" s="7"/>
-      <c r="F72" s="8"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C72" s="3"/>
+      <c r="D72" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E72" s="3"/>
+      <c r="F72" s="7"/>
+      <c r="G72" s="8"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
-      <c r="E73" s="7"/>
-      <c r="F73" s="8"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E73" s="3"/>
+      <c r="F73" s="7"/>
+      <c r="G73" s="8"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
-      <c r="E74" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F74" s="8"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E74" s="3"/>
+      <c r="F74" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G74" s="8"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B75" s="3"/>
-      <c r="C75" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D75" s="3"/>
-      <c r="E75" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F75" s="8"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C75" s="3"/>
+      <c r="D75" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E75" s="3"/>
+      <c r="F75" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G75" s="8"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
-      <c r="E76" s="7"/>
-      <c r="F76" s="8"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E76" s="3"/>
+      <c r="F76" s="7"/>
+      <c r="G76" s="8"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>116</v>
       </c>
@@ -2072,97 +2196,110 @@
       <c r="C77" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D77" s="3"/>
-      <c r="E77" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F77" s="8"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D77" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E77" s="3"/>
+      <c r="F77" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G77" s="8"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C78" s="3"/>
+      <c r="C78" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D78" s="3"/>
-      <c r="E78" s="7"/>
-      <c r="F78" s="8"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E78" s="3"/>
+      <c r="F78" s="7"/>
+      <c r="G78" s="8"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C79" s="3"/>
+      <c r="C79" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D79" s="3"/>
-      <c r="E79" s="7"/>
-      <c r="F79" s="8"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E79" s="3"/>
+      <c r="F79" s="7"/>
+      <c r="G79" s="8"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>66</v>
       </c>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
-      <c r="E80" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F80" s="8"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E80" s="3"/>
+      <c r="F80" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G80" s="8"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>100</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C81" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D81" s="3"/>
-      <c r="E81" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F81" s="8"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C81" s="3"/>
+      <c r="D81" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E81" s="3"/>
+      <c r="F81" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G81" s="8"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
         <v>127</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C82" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D82" s="3"/>
-      <c r="E82" s="7"/>
-      <c r="F82" s="8" t="s">
+      <c r="C82" s="3"/>
+      <c r="D82" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E82" s="3"/>
+      <c r="F82" s="7"/>
+      <c r="G82" s="8" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>79</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C83" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D83" s="3"/>
-      <c r="E83" s="7"/>
-      <c r="F83" s="9" t="s">
+      <c r="C83" s="3"/>
+      <c r="D83" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E83" s="3"/>
+      <c r="F83" s="7"/>
+      <c r="G83" s="9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>86</v>
       </c>
@@ -2172,171 +2309,194 @@
       <c r="C84" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D84" s="3"/>
-      <c r="E84" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F84" s="8"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D84" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E84" s="3"/>
+      <c r="F84" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G84" s="8"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B85" s="3"/>
-      <c r="C85" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D85" s="3"/>
-      <c r="E85" s="7"/>
-      <c r="F85" s="8"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C85" s="3"/>
+      <c r="D85" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E85" s="3"/>
+      <c r="F85" s="7"/>
+      <c r="G85" s="8"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B86" s="3"/>
-      <c r="C86" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D86" s="3"/>
-      <c r="E86" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F86" s="8"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C86" s="3"/>
+      <c r="D86" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E86" s="3"/>
+      <c r="F86" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G86" s="8"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
-      <c r="E87" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F87" s="8"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E87" s="3"/>
+      <c r="F87" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G87" s="8"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C88" s="3"/>
+      <c r="C88" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D88" s="3"/>
-      <c r="E88" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F88" s="8"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E88" s="3"/>
+      <c r="F88" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G88" s="8"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
-      <c r="E89" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F89" s="8"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E89" s="3"/>
+      <c r="F89" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G89" s="8"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
         <v>129</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C90" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D90" s="3"/>
-      <c r="E90" s="7"/>
-      <c r="F90" s="8" t="s">
+      <c r="C90" s="3"/>
+      <c r="D90" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E90" s="3"/>
+      <c r="F90" s="7"/>
+      <c r="G90" s="8" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C91" s="3"/>
+      <c r="C91" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D91" s="3"/>
-      <c r="E91" s="7"/>
-      <c r="F91" s="8"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E91" s="3"/>
+      <c r="F91" s="7"/>
+      <c r="G91" s="8"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C92" s="3"/>
+      <c r="C92" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D92" s="3"/>
-      <c r="E92" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F92" s="8"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E92" s="3"/>
+      <c r="F92" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G92" s="8"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
-      <c r="D93" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E93" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F93" s="8"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D93" s="3"/>
+      <c r="E93" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F93" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G93" s="8"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
       <c r="D94" s="3"/>
-      <c r="E94" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F94" s="8"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E94" s="3"/>
+      <c r="F94" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G94" s="8"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>69</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C95" s="3"/>
+      <c r="C95" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D95" s="3"/>
-      <c r="E95" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F95" s="8"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E95" s="3"/>
+      <c r="F95" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G95" s="8"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="s">
         <v>137</v>
       </c>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
       <c r="D96" s="3"/>
-      <c r="E96" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F96" s="8"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E96" s="3"/>
+      <c r="F96" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G96" s="8"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>75</v>
       </c>
@@ -2346,165 +2506,189 @@
       <c r="C97" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D97" s="3"/>
-      <c r="E97" s="7"/>
-      <c r="F97" s="10" t="s">
+      <c r="D97" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E97" s="3"/>
+      <c r="F97" s="7"/>
+      <c r="G97" s="10" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="14" t="s">
         <v>94</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C98" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D98" s="3"/>
-      <c r="E98" s="7"/>
-      <c r="F98" s="10" t="s">
+      <c r="C98" s="3"/>
+      <c r="D98" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E98" s="3"/>
+      <c r="F98" s="7"/>
+      <c r="G98" s="10" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C99" s="3"/>
+      <c r="C99" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D99" s="3"/>
-      <c r="E99" s="7"/>
-      <c r="F99" s="8"/>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E99" s="3"/>
+      <c r="F99" s="7"/>
+      <c r="G99" s="8"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C100" s="3"/>
+      <c r="C100" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D100" s="3"/>
-      <c r="E100" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F100" s="8"/>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E100" s="3"/>
+      <c r="F100" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G100" s="8"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
       <c r="D101" s="3"/>
-      <c r="E101" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F101" s="8"/>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E101" s="3"/>
+      <c r="F101" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G101" s="8"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
       <c r="D102" s="3"/>
-      <c r="E102" s="7"/>
-      <c r="F102" s="8"/>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E102" s="3"/>
+      <c r="F102" s="7"/>
+      <c r="G102" s="8"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C103" s="3"/>
-      <c r="D103" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E103" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F103" s="8"/>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C103" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D103" s="3"/>
+      <c r="E103" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F103" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G103" s="8"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>119</v>
       </c>
       <c r="B104" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C104" s="3"/>
+      <c r="C104" s="11"/>
       <c r="D104" s="3"/>
-      <c r="E104" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F104" s="8"/>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E104" s="3"/>
+      <c r="F104" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G104" s="8"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C105" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D105" s="3"/>
-      <c r="E105" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F105" s="8"/>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C105" s="3"/>
+      <c r="D105" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E105" s="3"/>
+      <c r="F105" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G105" s="8"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
       <c r="D106" s="3"/>
-      <c r="E106" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F106" s="8"/>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E106" s="3"/>
+      <c r="F106" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G106" s="8"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C107" s="3"/>
+      <c r="C107" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D107" s="3"/>
-      <c r="E107" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F107" s="8"/>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E107" s="3"/>
+      <c r="F107" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G107" s="8"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C108" s="3"/>
-      <c r="D108" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E108" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F108" s="8"/>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C108" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D108" s="3"/>
+      <c r="E108" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F108" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G108" s="8"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>51</v>
       </c>
@@ -2514,119 +2698,137 @@
       <c r="C109" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D109" s="3"/>
-      <c r="E109" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F109" s="8"/>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D109" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E109" s="3"/>
+      <c r="F109" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G109" s="8"/>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C110" s="3"/>
+      <c r="C110" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D110" s="3"/>
-      <c r="E110" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F110" s="8"/>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E110" s="3"/>
+      <c r="F110" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G110" s="8"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>121</v>
       </c>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
       <c r="D111" s="3"/>
-      <c r="E111" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F111" s="8"/>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E111" s="3"/>
+      <c r="F111" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G111" s="8"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="12" t="s">
         <v>136</v>
       </c>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
       <c r="D112" s="3"/>
-      <c r="E112" s="7"/>
-      <c r="F112" s="8"/>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E112" s="3"/>
+      <c r="F112" s="7"/>
+      <c r="G112" s="8"/>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
-      <c r="D113" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E113" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F113" s="8"/>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D113" s="3"/>
+      <c r="E113" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F113" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G113" s="8"/>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C114" s="3"/>
+      <c r="C114" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D114" s="3"/>
-      <c r="E114" s="7"/>
-      <c r="F114" s="8"/>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E114" s="3"/>
+      <c r="F114" s="7"/>
+      <c r="G114" s="8"/>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="14" t="s">
         <v>54</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C115" s="3"/>
+      <c r="C115" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D115" s="3"/>
-      <c r="E115" s="7"/>
-      <c r="F115" s="8"/>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E115" s="3"/>
+      <c r="F115" s="7"/>
+      <c r="G115" s="8"/>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B116" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C116" s="3"/>
+      <c r="C116" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="D116" s="3"/>
-      <c r="E116" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F116" s="8"/>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E116" s="3"/>
+      <c r="F116" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G116" s="8"/>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="14" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="12" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="13" t="s">
         <v>138</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F116" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G116" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
-    <hyperlink ref="E1" r:id="rId1" display="https://github.com/microsoft/winget-pkgs" xr:uid="{2C434A13-8B1C-492F-95C8-B89737A54984}"/>
+    <hyperlink ref="F1" r:id="rId1" display="https://github.com/microsoft/winget-pkgs" xr:uid="{2C434A13-8B1C-492F-95C8-B89737A54984}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -2639,7 +2841,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2651,7 +2853,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
remove goggalaxy from recommendation
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E2825F-01BC-4789-8AC8-09F4126A12BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC298A8-B6B6-4207-86A7-BB1A5DF4E4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3465" yWindow="3630" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -304,9 +304,6 @@
   </si>
   <si>
     <t>goggalaxy</t>
-  </si>
-  <si>
-    <t>GOG Game Launcher</t>
   </si>
   <si>
     <t>universal-ctags</t>
@@ -474,6 +471,9 @@
   </si>
   <si>
     <t>Secondary</t>
+  </si>
+  <si>
+    <t>GOG Game Launcher; do not use via choco, as it does not install silently</t>
   </si>
 </sst>
 </file>
@@ -975,8 +975,8 @@
   <dimension ref="A1:G120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,7 +987,7 @@
     <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="64.85546875" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -998,7 +998,7 @@
         <v>71</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>73</v>
@@ -1007,10 +1007,10 @@
         <v>72</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1102,7 +1102,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>56</v>
@@ -1130,7 +1130,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1145,7 +1145,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1158,7 +1158,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1190,7 +1190,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1218,7 +1218,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>56</v>
@@ -1230,12 +1230,12 @@
       <c r="E15" s="3"/>
       <c r="F15" s="7"/>
       <c r="G15" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1246,7 +1246,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>56</v>
@@ -1302,7 +1302,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>56</v>
@@ -1360,7 +1360,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>56</v>
@@ -1377,7 +1377,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>56</v>
@@ -1389,7 +1389,7 @@
         <v>56</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1411,7 +1411,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>56</v>
@@ -1423,7 +1423,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="7"/>
       <c r="G28" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1482,7 +1482,7 @@
         <v>56</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1504,7 +1504,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1516,7 +1516,7 @@
         <v>56</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1550,7 +1550,7 @@
       <c r="G35" s="8"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="13" t="s">
         <v>92</v>
       </c>
       <c r="B36" s="3" t="s">
@@ -1564,8 +1564,8 @@
       <c r="F36" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G36" s="8" t="s">
-        <v>93</v>
+      <c r="G36" s="15" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1670,7 +1670,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>56</v>
@@ -1689,7 +1689,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>56</v>
@@ -1703,7 +1703,7 @@
         <v>56</v>
       </c>
       <c r="G44" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1862,7 +1862,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -1872,7 +1872,7 @@
         <v>56</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -1892,7 +1892,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B57" s="11" t="s">
         <v>56</v>
@@ -1924,7 +1924,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -1932,7 +1932,7 @@
       <c r="E59" s="3"/>
       <c r="F59" s="7"/>
       <c r="G59" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -1980,7 +1980,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -1995,7 +1995,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>56</v>
@@ -2123,7 +2123,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>56</v>
@@ -2188,7 +2188,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>56</v>
@@ -2250,7 +2250,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>56</v>
@@ -2267,7 +2267,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>56</v>
@@ -2279,7 +2279,7 @@
       <c r="E82" s="3"/>
       <c r="F82" s="7"/>
       <c r="G82" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -2391,7 +2391,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>56</v>
@@ -2403,7 +2403,7 @@
       <c r="E90" s="3"/>
       <c r="F90" s="7"/>
       <c r="G90" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -2485,7 +2485,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
@@ -2517,7 +2517,7 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>56</v>
@@ -2529,7 +2529,7 @@
       <c r="E98" s="3"/>
       <c r="F98" s="7"/>
       <c r="G98" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -2609,7 +2609,7 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B104" s="11" t="s">
         <v>56</v>
@@ -2726,7 +2726,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
@@ -2739,7 +2739,7 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
@@ -2795,7 +2795,7 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B116" s="11" t="s">
         <v>56</v>
@@ -2812,17 +2812,17 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add discord to package manager
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3720CA38-A144-46D3-AE02-758ED1CC5C02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78FBE4B6-5D94-4EAE-A618-5A337E63125F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$G$116</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$G$117</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="143">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -474,6 +474,9 @@
   </si>
   <si>
     <t>GOG Game Launcher; do not use via choco, as it does not install silently</t>
+  </si>
+  <si>
+    <t>discord</t>
   </si>
 </sst>
 </file>
@@ -972,11 +975,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G120"/>
+  <dimension ref="A1:G121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1318,16 +1321,14 @@
       <c r="G21" s="8"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>81</v>
+      <c r="A22" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C22" s="3"/>
-      <c r="D22" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="7" t="s">
         <v>56</v>
@@ -1335,202 +1336,198 @@
       <c r="G22" s="8"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="8"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="3"/>
+      <c r="B24" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="E24" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="F24" s="7"/>
       <c r="G24" s="8"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>56</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="F25" s="7"/>
       <c r="G25" s="8"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="11"/>
+      <c r="C26" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G26" s="8" t="s">
-        <v>107</v>
-      </c>
+      <c r="G26" s="8"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="11"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G27" s="8"/>
+      <c r="G27" s="8" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G28" s="8"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E28" s="3"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="8" t="s">
+      <c r="B29" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29" s="3"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="8" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F29" s="7"/>
-      <c r="G29" s="8"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="7"/>
+      <c r="G30" s="8"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G30" s="8"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="B31" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" s="8"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G31" s="8" t="s">
+      <c r="B32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G32" s="8" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E32" s="3"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="8" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="B33" s="3"/>
+        <v>57</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
         <v>56</v>
       </c>
       <c r="E33" s="3"/>
-      <c r="F33" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="F33" s="7"/>
       <c r="G33" s="8" t="s">
-        <v>112</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="A34" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
         <v>56</v>
       </c>
@@ -1538,15 +1535,23 @@
       <c r="F34" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G34" s="8"/>
+      <c r="G34" s="8" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
+      <c r="A35" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E35" s="3"/>
       <c r="F35" s="7" t="s">
         <v>56</v>
@@ -1554,48 +1559,40 @@
       <c r="G35" s="8"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="A36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G36" s="15" t="s">
+      <c r="G36" s="8"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G37" s="15" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G37" s="8"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>56</v>
@@ -1603,8 +1600,12 @@
       <c r="C38" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
+      <c r="D38" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="F38" s="7" t="s">
         <v>56</v>
       </c>
@@ -1612,93 +1613,93 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G39" s="8"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E39" s="3"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="8"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B40" s="3"/>
+      <c r="B40" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3" t="s">
         <v>56</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="7"/>
-      <c r="G40" s="8" t="s">
+      <c r="G40" s="8"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E41" s="3"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="8" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G41" s="8"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="C42" s="3"/>
       <c r="D42" s="3"/>
-      <c r="E42" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F42" s="7"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="G42" s="8"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F43" s="7"/>
+      <c r="G43" s="8"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E43" s="3"/>
-      <c r="F43" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G43" s="8"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="s">
-        <v>101</v>
-      </c>
       <c r="B44" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C44" s="3"/>
+      <c r="C44" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D44" s="3" t="s">
         <v>56</v>
       </c>
@@ -1706,13 +1707,11 @@
       <c r="F44" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G44" s="15" t="s">
-        <v>139</v>
-      </c>
+      <c r="G44" s="8"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>82</v>
+      <c r="A45" s="13" t="s">
+        <v>101</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>56</v>
@@ -1722,104 +1721,104 @@
         <v>56</v>
       </c>
       <c r="E45" s="3"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="8"/>
+      <c r="F45" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G45" s="15" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B46" s="3"/>
+      <c r="A46" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="D46" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E46" s="3"/>
+      <c r="F46" s="7"/>
       <c r="G46" s="8"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G47" s="8"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="8"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="B48" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="7"/>
       <c r="G48" s="8"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>83</v>
+      <c r="A49" s="14" t="s">
+        <v>19</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
+      <c r="D49" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E49" s="3"/>
       <c r="F49" s="7"/>
       <c r="G49" s="8"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="8"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B50" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G50" s="8"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+      <c r="B51" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G51" s="8"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E51" s="3"/>
-      <c r="F51" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G51" s="8"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>56</v>
@@ -1837,25 +1836,31 @@
       <c r="G52" s="8"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E53" s="3"/>
+      <c r="F53" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G53" s="8"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B53" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E53" s="3"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="8"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B54" s="3"/>
+      <c r="B54" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3" t="s">
         <v>56</v>
@@ -1865,116 +1870,112 @@
       <c r="G54" s="8"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>130</v>
+      <c r="A55" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
+      <c r="D55" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E55" s="3"/>
-      <c r="F55" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G55" s="8" t="s">
-        <v>131</v>
-      </c>
+      <c r="F55" s="7"/>
+      <c r="G55" s="8"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="A56" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
-      <c r="F56" s="7"/>
-      <c r="G56" s="8"/>
+      <c r="F56" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G56" s="8" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B57" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C57" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>56</v>
       </c>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
-      <c r="F57" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="F57" s="7"/>
       <c r="G57" s="8"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="A58" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D58" s="3"/>
       <c r="E58" s="3"/>
-      <c r="F58" s="7"/>
+      <c r="F58" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="G58" s="8"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B59" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
+      <c r="D59" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E59" s="3"/>
       <c r="F59" s="7"/>
-      <c r="G59" s="8" t="s">
-        <v>114</v>
-      </c>
+      <c r="G59" s="8"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="7"/>
-      <c r="G60" s="8"/>
+      <c r="G60" s="8" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B61" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
-      <c r="F61" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="F61" s="7"/>
       <c r="G61" s="8"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
       <c r="F62" s="7" t="s">
@@ -1984,13 +1985,15 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D63" s="3"/>
       <c r="E63" s="3"/>
       <c r="F63" s="7" t="s">
         <v>56</v>
@@ -1999,11 +2002,9 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3" t="s">
         <v>56</v>
@@ -2015,43 +2016,43 @@
       <c r="G64" s="8"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
-        <v>77</v>
+      <c r="A65" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C65" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E65" s="3"/>
-      <c r="F65" s="7"/>
+      <c r="F65" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="G65" s="8"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
+        <v>77</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
-      <c r="F66" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="F66" s="7"/>
       <c r="G66" s="8"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="A67" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
       <c r="F67" s="7" t="s">
@@ -2060,16 +2061,16 @@
       <c r="G67" s="8"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
-        <v>64</v>
+      <c r="A68" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="C68" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D68" s="3"/>
       <c r="E68" s="3"/>
       <c r="F68" s="7" t="s">
         <v>56</v>
@@ -2078,20 +2079,16 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C69" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="C69" s="3"/>
       <c r="D69" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E69" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="E69" s="3"/>
       <c r="F69" s="7" t="s">
         <v>56</v>
       </c>
@@ -2099,27 +2096,35 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G70" s="8"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F70" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G70" s="8"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
-      <c r="E71" s="3"/>
+      <c r="E71" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="F71" s="7" t="s">
         <v>56</v>
       </c>
@@ -2127,52 +2132,50 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B72" s="3"/>
       <c r="C72" s="3"/>
-      <c r="D72" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="D72" s="3"/>
       <c r="E72" s="3"/>
-      <c r="F72" s="7"/>
+      <c r="F72" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="G72" s="8"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B73" s="3"/>
+        <v>100</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
+      <c r="D73" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E73" s="3"/>
       <c r="F73" s="7"/>
       <c r="G73" s="8"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
-      <c r="F74" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="F74" s="7"/>
       <c r="G74" s="8"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
-      <c r="D75" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="D75" s="3"/>
       <c r="E75" s="3"/>
       <c r="F75" s="7" t="s">
         <v>56</v>
@@ -2181,37 +2184,33 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
+      <c r="D76" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E76" s="3"/>
-      <c r="F76" s="7"/>
+      <c r="F76" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="G76" s="8"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
       <c r="E77" s="3"/>
-      <c r="F77" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="F77" s="7"/>
       <c r="G77" s="8"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>33</v>
+        <v>115</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>56</v>
@@ -2219,14 +2218,18 @@
       <c r="C78" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D78" s="3"/>
+      <c r="D78" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E78" s="3"/>
-      <c r="F78" s="7"/>
+      <c r="F78" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="G78" s="8"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>56</v>
@@ -2240,29 +2243,27 @@
       <c r="G79" s="8"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
+      <c r="A80" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
-      <c r="F80" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="F80" s="7"/>
       <c r="G80" s="8"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="B81" s="3"/>
       <c r="C81" s="3"/>
-      <c r="D81" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="D81" s="3"/>
       <c r="E81" s="3"/>
       <c r="F81" s="7" t="s">
         <v>56</v>
@@ -2270,8 +2271,8 @@
       <c r="G81" s="8"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="14" t="s">
-        <v>126</v>
+      <c r="A82" s="4" t="s">
+        <v>99</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>56</v>
@@ -2281,14 +2282,14 @@
         <v>56</v>
       </c>
       <c r="E82" s="3"/>
-      <c r="F82" s="7"/>
-      <c r="G82" s="8" t="s">
-        <v>127</v>
-      </c>
+      <c r="F82" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G82" s="8"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="4" t="s">
-        <v>79</v>
+      <c r="A83" s="14" t="s">
+        <v>126</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>56</v>
@@ -2299,45 +2300,49 @@
       </c>
       <c r="E83" s="3"/>
       <c r="F83" s="7"/>
-      <c r="G83" s="9" t="s">
+      <c r="G83" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E84" s="3"/>
+      <c r="F84" s="7"/>
+      <c r="G84" s="9" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E84" s="3"/>
-      <c r="F84" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G84" s="8"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B85" s="3"/>
-      <c r="C85" s="3"/>
+        <v>86</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D85" s="3" t="s">
         <v>56</v>
       </c>
       <c r="E85" s="3"/>
-      <c r="F85" s="7"/>
+      <c r="F85" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="G85" s="8"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
@@ -2345,18 +2350,18 @@
         <v>56</v>
       </c>
       <c r="E86" s="3"/>
-      <c r="F86" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="F86" s="7"/>
       <c r="G86" s="8"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
+      <c r="D87" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E87" s="3"/>
       <c r="F87" s="7" t="s">
         <v>56</v>
@@ -2365,14 +2370,10 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
       <c r="F88" s="7" t="s">
@@ -2382,10 +2383,14 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B89" s="3"/>
-      <c r="C89" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
       <c r="F89" s="7" t="s">
@@ -2394,40 +2399,38 @@
       <c r="G89" s="8"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="14" t="s">
+      <c r="A90" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G90" s="8"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="B90" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C90" s="3"/>
-      <c r="D90" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E90" s="3"/>
-      <c r="F90" s="7"/>
-      <c r="G90" s="8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="B91" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C91" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E91" s="3"/>
       <c r="F91" s="7"/>
-      <c r="G91" s="8"/>
+      <c r="G91" s="8" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>56</v>
@@ -2437,21 +2440,21 @@
       </c>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
-      <c r="F92" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="F92" s="7"/>
       <c r="G92" s="8"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B93" s="3"/>
-      <c r="C93" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D93" s="3"/>
-      <c r="E93" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="E93" s="3"/>
       <c r="F93" s="7" t="s">
         <v>56</v>
       </c>
@@ -2459,27 +2462,25 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
       <c r="D94" s="3"/>
-      <c r="E94" s="3"/>
+      <c r="E94" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="F94" s="7" t="s">
         <v>56</v>
       </c>
       <c r="G94" s="8"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="A95" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
       <c r="F95" s="7" t="s">
@@ -2488,11 +2489,15 @@
       <c r="G95" s="8"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="B96" s="3"/>
-      <c r="C96" s="3"/>
+      <c r="A96" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
       <c r="F96" s="7" t="s">
@@ -2501,59 +2506,57 @@
       <c r="G96" s="8"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="4" t="s">
+      <c r="A97" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B97" s="3"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G97" s="8"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B97" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D97" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E97" s="3"/>
-      <c r="F97" s="7"/>
-      <c r="G97" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="14" t="s">
-        <v>93</v>
-      </c>
       <c r="B98" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C98" s="3"/>
+      <c r="C98" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D98" s="3" t="s">
         <v>56</v>
       </c>
       <c r="E98" s="3"/>
       <c r="F98" s="7"/>
       <c r="G98" s="10" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
-        <v>43</v>
+      <c r="A99" s="14" t="s">
+        <v>93</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C99" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D99" s="3"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E99" s="3"/>
       <c r="F99" s="7"/>
-      <c r="G99" s="8"/>
+      <c r="G99" s="10" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>56</v>
@@ -2563,17 +2566,19 @@
       </c>
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
-      <c r="F100" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="F100" s="7"/>
       <c r="G100" s="8"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B101" s="3"/>
-      <c r="C101" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
       <c r="F101" s="7" t="s">
@@ -2583,62 +2588,56 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
       <c r="D102" s="3"/>
       <c r="E102" s="3"/>
-      <c r="F102" s="7"/>
+      <c r="F102" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="G102" s="8"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B103" s="3"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
+      <c r="E103" s="3"/>
+      <c r="F103" s="7"/>
+      <c r="G103" s="8"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B103" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D103" s="3"/>
-      <c r="E103" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F103" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G103" s="8"/>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="4" t="s">
+      <c r="B104" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D104" s="3"/>
+      <c r="E104" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F104" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G104" s="8"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B104" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C104" s="11"/>
-      <c r="D104" s="3"/>
-      <c r="E104" s="3"/>
-      <c r="F104" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G104" s="8"/>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="B105" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C105" s="11"/>
+      <c r="D105" s="3"/>
       <c r="E105" s="3"/>
       <c r="F105" s="7" t="s">
         <v>56</v>
@@ -2647,11 +2646,17 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B106" s="3"/>
-      <c r="C106" s="3"/>
-      <c r="D106" s="3"/>
+        <v>48</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E106" s="3"/>
       <c r="F106" s="7" t="s">
         <v>56</v>
@@ -2659,15 +2664,11 @@
       <c r="G106" s="8"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="A107" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B107" s="3"/>
+      <c r="C107" s="3"/>
       <c r="D107" s="3"/>
       <c r="E107" s="3"/>
       <c r="F107" s="7" t="s">
@@ -2676,8 +2677,8 @@
       <c r="G107" s="8"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
-        <v>50</v>
+      <c r="A108" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>56</v>
@@ -2686,9 +2687,7 @@
         <v>56</v>
       </c>
       <c r="D108" s="3"/>
-      <c r="E108" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="E108" s="3"/>
       <c r="F108" s="7" t="s">
         <v>56</v>
       </c>
@@ -2696,7 +2695,7 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>56</v>
@@ -2704,10 +2703,10 @@
       <c r="C109" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D109" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E109" s="3"/>
+      <c r="D109" s="3"/>
+      <c r="E109" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="F109" s="7" t="s">
         <v>56</v>
       </c>
@@ -2715,7 +2714,7 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>56</v>
@@ -2723,7 +2722,9 @@
       <c r="C110" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D110" s="3"/>
+      <c r="D110" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E110" s="3"/>
       <c r="F110" s="7" t="s">
         <v>56</v>
@@ -2732,10 +2733,14 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B111" s="3"/>
-      <c r="C111" s="3"/>
+        <v>52</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D111" s="3"/>
       <c r="E111" s="3"/>
       <c r="F111" s="7" t="s">
@@ -2744,49 +2749,47 @@
       <c r="G111" s="8"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="12" t="s">
-        <v>135</v>
+      <c r="A112" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
       <c r="D112" s="3"/>
       <c r="E112" s="3"/>
-      <c r="F112" s="7"/>
+      <c r="F112" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="G112" s="8"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" s="4" t="s">
-        <v>67</v>
+      <c r="A113" s="12" t="s">
+        <v>135</v>
       </c>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
       <c r="D113" s="3"/>
-      <c r="E113" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F113" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="E113" s="3"/>
+      <c r="F113" s="7"/>
       <c r="G113" s="8"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
+      <c r="A114" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B114" s="3"/>
+      <c r="C114" s="3"/>
+      <c r="D114" s="3"/>
+      <c r="E114" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F114" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G114" s="8"/>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D114" s="3"/>
-      <c r="E114" s="3"/>
-      <c r="F114" s="7"/>
-      <c r="G114" s="8"/>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A115" s="14" t="s">
-        <v>54</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>56</v>
@@ -2800,39 +2803,54 @@
       <c r="G115" s="8"/>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B116" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C116" s="11" t="s">
+      <c r="A116" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C116" s="3" t="s">
         <v>56</v>
       </c>
       <c r="D116" s="3"/>
       <c r="E116" s="3"/>
-      <c r="F116" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="F116" s="7"/>
       <c r="G116" s="8"/>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A118" s="14" t="s">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B117" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C117" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D117" s="3"/>
+      <c r="E117" s="3"/>
+      <c r="F117" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G117" s="8"/>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="14" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A119" s="12" t="s">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" s="12" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120" s="13" t="s">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" s="13" t="s">
         <v>137</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G116" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G117" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="F1" r:id="rId1" display="https://github.com/microsoft/winget-pkgs" xr:uid="{2C434A13-8B1C-492F-95C8-B89737A54984}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
add handbrake to choco
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78FBE4B6-5D94-4EAE-A618-5A337E63125F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C92634-FAFF-4118-A308-D385FAD8E6D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="900" yWindow="2385" windowWidth="20925" windowHeight="14205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$G$117</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$G$119</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="147">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -477,6 +477,18 @@
   </si>
   <si>
     <t>discord</t>
+  </si>
+  <si>
+    <t>handbrake</t>
+  </si>
+  <si>
+    <t>DVD Ripper; anschließend libdvdcss-2 installieren</t>
+  </si>
+  <si>
+    <t>libdvdcss-2</t>
+  </si>
+  <si>
+    <t>DVD Decryption; zuerst handbrake installieren</t>
   </si>
 </sst>
 </file>
@@ -975,11 +987,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G121"/>
+  <dimension ref="A1:G123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1644,79 +1656,81 @@
       <c r="G40" s="8"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
+      <c r="A41" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E41" s="3"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="8" t="s">
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E42" s="3"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="8" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G42" s="8"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="C43" s="3"/>
       <c r="D43" s="3"/>
-      <c r="E43" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F43" s="7"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="G43" s="8"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F44" s="7"/>
+      <c r="G44" s="8"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E44" s="3"/>
-      <c r="F44" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G44" s="8"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="s">
-        <v>101</v>
-      </c>
       <c r="B45" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C45" s="3"/>
+      <c r="C45" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D45" s="3" t="s">
         <v>56</v>
       </c>
@@ -1724,13 +1738,11 @@
       <c r="F45" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G45" s="15" t="s">
-        <v>139</v>
-      </c>
+      <c r="G45" s="8"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>82</v>
+      <c r="A46" s="13" t="s">
+        <v>101</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>56</v>
@@ -1740,104 +1752,104 @@
         <v>56</v>
       </c>
       <c r="E46" s="3"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="8"/>
+      <c r="F46" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G46" s="15" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B47" s="3"/>
+      <c r="A47" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="D47" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E47" s="3"/>
+      <c r="F47" s="7"/>
       <c r="G47" s="8"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G48" s="8"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="8"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="B49" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D49" s="3"/>
       <c r="E49" s="3"/>
       <c r="F49" s="7"/>
       <c r="G49" s="8"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>83</v>
+      <c r="A50" s="14" t="s">
+        <v>19</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
+      <c r="D50" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E50" s="3"/>
       <c r="F50" s="7"/>
       <c r="G50" s="8"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="8"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G51" s="8"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
+      <c r="B52" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G52" s="8"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E52" s="3"/>
-      <c r="F52" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G52" s="8"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>56</v>
@@ -1855,25 +1867,31 @@
       <c r="G53" s="8"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E54" s="3"/>
+      <c r="F54" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G54" s="8"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E54" s="3"/>
-      <c r="F54" s="7"/>
-      <c r="G54" s="8"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B55" s="3"/>
+      <c r="B55" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3" t="s">
         <v>56</v>
@@ -1883,23 +1901,21 @@
       <c r="G55" s="8"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>130</v>
+      <c r="A56" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
+      <c r="D56" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E56" s="3"/>
-      <c r="F56" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G56" s="8" t="s">
-        <v>131</v>
-      </c>
+      <c r="F56" s="7"/>
+      <c r="G56" s="8"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
-        <v>78</v>
+      <c r="A57" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>56</v>
@@ -1910,105 +1926,105 @@
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
       <c r="F57" s="7"/>
-      <c r="G57" s="8"/>
+      <c r="G57" s="8" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B58" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C58" s="11" t="s">
-        <v>56</v>
-      </c>
+      <c r="A58" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
       <c r="F58" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G58" s="8"/>
+      <c r="G58" s="8" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>23</v>
+      <c r="A59" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="C59" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D59" s="3"/>
       <c r="E59" s="3"/>
       <c r="F59" s="7"/>
       <c r="G59" s="8"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
+      <c r="A60" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B60" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
-      <c r="F60" s="7"/>
-      <c r="G60" s="8" t="s">
-        <v>114</v>
-      </c>
+      <c r="F60" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G60" s="8"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
+      <c r="D61" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E61" s="3"/>
       <c r="F61" s="7"/>
       <c r="G61" s="8"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>25</v>
+        <v>113</v>
       </c>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
-      <c r="F62" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G62" s="8"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="8" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C63" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="C63" s="3"/>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
-      <c r="F63" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="F63" s="7"/>
       <c r="G63" s="8"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>116</v>
+        <v>25</v>
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
-      <c r="D64" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="D64" s="3"/>
       <c r="E64" s="3"/>
       <c r="F64" s="7" t="s">
         <v>56</v>
@@ -2017,15 +2033,15 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>117</v>
+        <v>26</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="C65" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D65" s="3"/>
       <c r="E65" s="3"/>
       <c r="F65" s="7" t="s">
         <v>56</v>
@@ -2033,27 +2049,31 @@
       <c r="G65" s="8"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D66" s="3"/>
+      <c r="A66" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E66" s="3"/>
-      <c r="F66" s="7"/>
+      <c r="F66" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="G66" s="8"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B67" s="3"/>
+      <c r="A67" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
+      <c r="D67" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E67" s="3"/>
       <c r="F67" s="7" t="s">
         <v>56</v>
@@ -2061,8 +2081,8 @@
       <c r="G67" s="8"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>27</v>
+      <c r="A68" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>56</v>
@@ -2072,22 +2092,16 @@
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
-      <c r="F68" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="F68" s="7"/>
       <c r="G68" s="8"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="B69" s="3"/>
       <c r="C69" s="3"/>
-      <c r="D69" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="D69" s="3"/>
       <c r="E69" s="3"/>
       <c r="F69" s="7" t="s">
         <v>56</v>
@@ -2095,8 +2109,8 @@
       <c r="G69" s="8"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
-        <v>65</v>
+      <c r="A70" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>56</v>
@@ -2104,12 +2118,8 @@
       <c r="C70" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D70" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
       <c r="F70" s="7" t="s">
         <v>56</v>
       </c>
@@ -2117,107 +2127,115 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E71" s="3"/>
+      <c r="F71" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G71" s="8"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F72" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G72" s="8"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
-      <c r="E71" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F71" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G71" s="8"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
-      <c r="E72" s="3"/>
-      <c r="F72" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G72" s="8"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="B73" s="3"/>
       <c r="C73" s="3"/>
-      <c r="D73" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E73" s="3"/>
-      <c r="F73" s="7"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="G73" s="8"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
-      <c r="F74" s="7"/>
+      <c r="F74" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="G74" s="8"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B75" s="3"/>
+        <v>100</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
+      <c r="D75" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E75" s="3"/>
-      <c r="F75" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="F75" s="7"/>
       <c r="G75" s="8"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
-      <c r="D76" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="D76" s="3"/>
       <c r="E76" s="3"/>
-      <c r="F76" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="F76" s="7"/>
       <c r="G76" s="8"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
-      <c r="F77" s="7"/>
+      <c r="F77" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="G77" s="8"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
       <c r="D78" s="3" t="s">
         <v>56</v>
       </c>
@@ -2229,14 +2247,10 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
       <c r="F79" s="7"/>
@@ -2244,7 +2258,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>56</v>
@@ -2252,61 +2266,61 @@
       <c r="C80" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D80" s="3"/>
+      <c r="D80" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E80" s="3"/>
-      <c r="F80" s="7"/>
+      <c r="F80" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="G80" s="8"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B81" s="3"/>
-      <c r="C81" s="3"/>
+      <c r="A81" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
-      <c r="F81" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="F81" s="7"/>
       <c r="G81" s="8"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
-        <v>99</v>
+      <c r="A82" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="C82" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D82" s="3"/>
       <c r="E82" s="3"/>
-      <c r="F82" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="F82" s="7"/>
       <c r="G82" s="8"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="A83" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B83" s="3"/>
       <c r="C83" s="3"/>
-      <c r="D83" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="D83" s="3"/>
       <c r="E83" s="3"/>
-      <c r="F83" s="7"/>
-      <c r="G83" s="8" t="s">
-        <v>127</v>
-      </c>
+      <c r="F83" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G83" s="8"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>56</v>
@@ -2316,49 +2330,55 @@
         <v>56</v>
       </c>
       <c r="E84" s="3"/>
-      <c r="F84" s="7"/>
-      <c r="G84" s="9" t="s">
-        <v>80</v>
-      </c>
+      <c r="F84" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G84" s="8"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>86</v>
+      <c r="A85" s="14" t="s">
+        <v>126</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C85" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="C85" s="3"/>
       <c r="D85" s="3" t="s">
         <v>56</v>
       </c>
       <c r="E85" s="3"/>
-      <c r="F85" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G85" s="8"/>
+      <c r="F85" s="7"/>
+      <c r="G85" s="8" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B86" s="3"/>
+      <c r="A86" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C86" s="3"/>
       <c r="D86" s="3" t="s">
         <v>56</v>
       </c>
       <c r="E86" s="3"/>
       <c r="F86" s="7"/>
-      <c r="G86" s="8"/>
+      <c r="G86" s="9" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B87" s="3"/>
-      <c r="C87" s="3"/>
+        <v>86</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D87" s="3" t="s">
         <v>56</v>
       </c>
@@ -2370,28 +2390,26 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
-      <c r="D88" s="3"/>
+      <c r="D88" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E88" s="3"/>
-      <c r="F88" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="F88" s="7"/>
       <c r="G88" s="8"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D89" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E89" s="3"/>
       <c r="F89" s="7" t="s">
         <v>56</v>
@@ -2400,7 +2418,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -2412,75 +2430,77 @@
       <c r="G90" s="8"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="14" t="s">
-        <v>128</v>
+      <c r="A91" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C91" s="3"/>
-      <c r="D91" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="C91" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D91" s="3"/>
       <c r="E91" s="3"/>
-      <c r="F91" s="7"/>
-      <c r="G91" s="8" t="s">
-        <v>129</v>
-      </c>
+      <c r="F91" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G91" s="8"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
-      <c r="F92" s="7"/>
+      <c r="F92" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="G92" s="8"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>40</v>
+      <c r="A93" s="14" t="s">
+        <v>128</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C93" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D93" s="3"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E93" s="3"/>
-      <c r="F93" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G93" s="8"/>
+      <c r="F93" s="7"/>
+      <c r="G93" s="8" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B94" s="3"/>
-      <c r="C94" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D94" s="3"/>
-      <c r="E94" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F94" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="E94" s="3"/>
+      <c r="F94" s="7"/>
       <c r="G94" s="8"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B95" s="3"/>
-      <c r="C95" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
       <c r="F95" s="7" t="s">
@@ -2489,25 +2509,23 @@
       <c r="G95" s="8"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="A96" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
       <c r="D96" s="3"/>
-      <c r="E96" s="3"/>
+      <c r="E96" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="F96" s="7" t="s">
         <v>56</v>
       </c>
       <c r="G96" s="8"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="13" t="s">
-        <v>136</v>
+      <c r="A97" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
@@ -2520,133 +2538,129 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D98" s="3"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G98" s="8"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B99" s="3"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G99" s="8"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B98" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D98" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E98" s="3"/>
-      <c r="F98" s="7"/>
-      <c r="G98" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C99" s="3"/>
-      <c r="D99" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E99" s="3"/>
-      <c r="F99" s="7"/>
-      <c r="G99" s="10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="B100" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D100" s="3"/>
+      <c r="D100" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E100" s="3"/>
       <c r="F100" s="7"/>
-      <c r="G100" s="8"/>
+      <c r="G100" s="10" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>44</v>
+      <c r="A101" s="14" t="s">
+        <v>93</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C101" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D101" s="3"/>
+      <c r="C101" s="3"/>
+      <c r="D101" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E101" s="3"/>
-      <c r="F101" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G101" s="8"/>
+      <c r="F101" s="7"/>
+      <c r="G101" s="10" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B102" s="3"/>
-      <c r="C102" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D102" s="3"/>
       <c r="E102" s="3"/>
-      <c r="F102" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="F102" s="7"/>
       <c r="G102" s="8"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B103" s="3"/>
-      <c r="C103" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D103" s="3"/>
       <c r="E103" s="3"/>
-      <c r="F103" s="7"/>
+      <c r="F103" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="G103" s="8"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B104" s="3"/>
+      <c r="C104" s="3"/>
       <c r="D104" s="3"/>
-      <c r="E104" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="E104" s="3"/>
       <c r="F104" s="7" t="s">
         <v>56</v>
       </c>
       <c r="G104" s="8"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B105" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C105" s="11"/>
+      <c r="A105" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B105" s="3"/>
+      <c r="C105" s="3"/>
       <c r="D105" s="3"/>
       <c r="E105" s="3"/>
-      <c r="F105" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="F105" s="7"/>
       <c r="G105" s="8"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>56</v>
@@ -2654,21 +2668,23 @@
       <c r="C106" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D106" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E106" s="3"/>
+      <c r="D106" s="3"/>
+      <c r="E106" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="F106" s="7" t="s">
         <v>56</v>
       </c>
       <c r="G106" s="8"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B107" s="3"/>
-      <c r="C107" s="3"/>
+      <c r="A107" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B107" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C107" s="11"/>
       <c r="D107" s="3"/>
       <c r="E107" s="3"/>
       <c r="F107" s="7" t="s">
@@ -2677,8 +2693,8 @@
       <c r="G107" s="8"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="4" t="s">
-        <v>74</v>
+      <c r="A108" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>56</v>
@@ -2686,7 +2702,9 @@
       <c r="C108" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D108" s="3"/>
+      <c r="D108" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E108" s="3"/>
       <c r="F108" s="7" t="s">
         <v>56</v>
@@ -2695,26 +2713,20 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="B109" s="3"/>
+      <c r="C109" s="3"/>
       <c r="D109" s="3"/>
-      <c r="E109" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="E109" s="3"/>
       <c r="F109" s="7" t="s">
         <v>56</v>
       </c>
       <c r="G109" s="8"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
-        <v>51</v>
+      <c r="A110" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>56</v>
@@ -2722,9 +2734,7 @@
       <c r="C110" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D110" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="D110" s="3"/>
       <c r="E110" s="3"/>
       <c r="F110" s="7" t="s">
         <v>56</v>
@@ -2733,7 +2743,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>56</v>
@@ -2742,7 +2752,9 @@
         <v>56</v>
       </c>
       <c r="D111" s="3"/>
-      <c r="E111" s="3"/>
+      <c r="E111" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="F111" s="7" t="s">
         <v>56</v>
       </c>
@@ -2750,11 +2762,17 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B112" s="3"/>
-      <c r="C112" s="3"/>
-      <c r="D112" s="3"/>
+        <v>51</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E112" s="3"/>
       <c r="F112" s="7" t="s">
         <v>56</v>
@@ -2762,95 +2780,125 @@
       <c r="G112" s="8"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="B113" s="3"/>
-      <c r="C113" s="3"/>
+      <c r="A113" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D113" s="3"/>
       <c r="E113" s="3"/>
-      <c r="F113" s="7"/>
+      <c r="F113" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="G113" s="8"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="4" t="s">
-        <v>67</v>
+      <c r="A114" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
       <c r="D114" s="3"/>
-      <c r="E114" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="E114" s="3"/>
       <c r="F114" s="7" t="s">
         <v>56</v>
       </c>
       <c r="G114" s="8"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B115" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="A115" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B115" s="3"/>
+      <c r="C115" s="3"/>
       <c r="D115" s="3"/>
       <c r="E115" s="3"/>
       <c r="F115" s="7"/>
       <c r="G115" s="8"/>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C116" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="A116" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B116" s="3"/>
+      <c r="C116" s="3"/>
       <c r="D116" s="3"/>
-      <c r="E116" s="3"/>
-      <c r="F116" s="7"/>
+      <c r="E116" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F116" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="G116" s="8"/>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B117" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C117" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C117" s="3" t="s">
         <v>56</v>
       </c>
       <c r="D117" s="3"/>
       <c r="E117" s="3"/>
-      <c r="F117" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="F117" s="7"/>
       <c r="G117" s="8"/>
     </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D118" s="3"/>
+      <c r="E118" s="3"/>
+      <c r="F118" s="7"/>
+      <c r="G118" s="8"/>
+    </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A119" s="14" t="s">
+      <c r="A119" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B119" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C119" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D119" s="3"/>
+      <c r="E119" s="3"/>
+      <c r="F119" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G119" s="8"/>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" s="14" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120" s="12" t="s">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" s="12" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A121" s="13" t="s">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" s="13" t="s">
         <v>137</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G117" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G119" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="F1" r:id="rId1" display="https://github.com/microsoft/winget-pkgs" xr:uid="{2C434A13-8B1C-492F-95C8-B89737A54984}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
add info for windirstat
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\wiki\Settings\Chocolatey\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\ubuntu\projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CE8750-C005-4567-A993-1901898AE356}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D882C94-977B-4CF4-B9E4-CC82F2C37E1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="156">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -513,6 +513,9 @@
   </si>
   <si>
     <t>Balena Etcher, format &amp; flash bootable USB</t>
+  </si>
+  <si>
+    <t>Disk Space</t>
   </si>
 </sst>
 </file>
@@ -667,10 +670,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Gut" xfId="1" builtinId="26"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
-    <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -691,7 +694,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1014,11 +1017,11 @@
   <dimension ref="A1:G127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G114" sqref="G114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
@@ -2850,7 +2853,9 @@
       <c r="F115" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G115" s="8"/>
+      <c r="G115" s="8" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
@@ -3005,7 +3010,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3017,7 +3022,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
replace pgadmin3 by pgadmin4, finally
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\ubuntu\projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D882C94-977B-4CF4-B9E4-CC82F2C37E1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5AAEDD-9A57-4368-8A42-3960305C84CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="156">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -112,9 +112,6 @@
   </si>
   <si>
     <t>owncloud-client</t>
-  </si>
-  <si>
-    <t>pgadmin3</t>
   </si>
   <si>
     <t>postgresql</t>
@@ -516,6 +513,9 @@
   </si>
   <si>
     <t>Disk Space</t>
+  </si>
+  <si>
+    <t>pgadmin4</t>
   </si>
 </sst>
 </file>
@@ -1017,8 +1017,8 @@
   <dimension ref="A1:G127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G114" sqref="G114"/>
+      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,45 +1034,45 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G2" s="8"/>
     </row>
@@ -1081,81 +1081,81 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G7" s="8"/>
     </row>
@@ -1172,76 +1172,76 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G12" s="8"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G13" s="8"/>
     </row>
@@ -1252,7 +1252,7 @@
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="7"/>
@@ -1260,24 +1260,24 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="7"/>
       <c r="G15" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1288,16 +1288,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="7"/>
@@ -1308,33 +1308,33 @@
         <v>3</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G18" s="8"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="7"/>
       <c r="G19" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1361,65 +1361,65 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G22" s="8"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G23" s="8"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G24" s="8"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G25" s="8"/>
     </row>
@@ -1428,12 +1428,12 @@
         <v>6</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="8"/>
@@ -1451,36 +1451,36 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G28" s="8"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1488,33 +1488,33 @@
         <v>8</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G30" s="8"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="7"/>
       <c r="G31" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1522,14 +1522,14 @@
         <v>9</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="8"/>
@@ -1539,93 +1539,93 @@
         <v>10</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G33" s="8"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="7"/>
       <c r="G35" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G37" s="8"/>
     </row>
@@ -1638,27 +1638,27 @@
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G38" s="8"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1666,19 +1666,19 @@
         <v>12</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G40" s="8"/>
     </row>
@@ -1687,15 +1687,15 @@
         <v>13</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G41" s="8"/>
     </row>
@@ -1704,11 +1704,11 @@
         <v>14</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="7"/>
@@ -1716,36 +1716,36 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="7"/>
       <c r="G44" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1753,13 +1753,13 @@
         <v>15</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G45" s="8"/>
     </row>
@@ -1768,66 +1768,66 @@
         <v>16</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F46" s="7"/>
       <c r="G46" s="8"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G47" s="8"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G48" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="7"/>
@@ -1841,10 +1841,10 @@
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G50" s="8"/>
     </row>
@@ -1853,10 +1853,10 @@
         <v>18</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
@@ -1870,7 +1870,7 @@
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="7"/>
@@ -1878,7 +1878,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -1892,38 +1892,38 @@
         <v>20</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D54" s="3"/>
       <c r="E54" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G55" s="8"/>
     </row>
@@ -1932,30 +1932,30 @@
         <v>21</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G56" s="8"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C57" s="3"/>
       <c r="D57" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="7"/>
@@ -1968,7 +1968,7 @@
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="7"/>
@@ -1976,45 +1976,45 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
       <c r="F59" s="7"/>
       <c r="G59" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
@@ -2023,18 +2023,18 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
       <c r="F62" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G62" s="8"/>
     </row>
@@ -2043,11 +2043,11 @@
         <v>23</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E63" s="3"/>
       <c r="F63" s="7"/>
@@ -2055,7 +2055,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -2063,24 +2063,24 @@
       <c r="E64" s="3"/>
       <c r="F64" s="7"/>
       <c r="G64" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
       <c r="F65" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -2088,7 +2088,7 @@
         <v>24</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
@@ -2105,7 +2105,7 @@
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
       <c r="F67" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G67" s="8"/>
     </row>
@@ -2114,59 +2114,59 @@
         <v>26</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
       <c r="F68" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G68" s="8"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E69" s="3"/>
       <c r="F69" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G69" s="8"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C70" s="3"/>
       <c r="D70" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E70" s="3"/>
       <c r="F70" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G70" s="8"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
@@ -2175,14 +2175,14 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
       <c r="F72" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G72" s="8"/>
     </row>
@@ -2191,68 +2191,68 @@
         <v>27</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G73" s="8"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C74" s="3"/>
       <c r="D74" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E74" s="3"/>
       <c r="F74" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G74" s="8"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G75" s="8"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
       <c r="E76" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G76" s="8"/>
     </row>
@@ -2265,20 +2265,20 @@
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
       <c r="F77" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G77" s="8"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C78" s="3"/>
       <c r="D78" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E78" s="3"/>
       <c r="F78" s="7"/>
@@ -2286,46 +2286,50 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>29</v>
+        <v>155</v>
       </c>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
+      <c r="D79" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E79" s="3"/>
-      <c r="F79" s="7"/>
+      <c r="F79" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="G79" s="8"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
       <c r="F80" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G80" s="8"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
       <c r="D81" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E81" s="3"/>
       <c r="F81" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G81" s="8"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
@@ -2336,32 +2340,32 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E83" s="3"/>
       <c r="F83" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G83" s="8"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
@@ -2370,13 +2374,13 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
@@ -2385,112 +2389,112 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
       <c r="F86" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G86" s="8"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E87" s="3"/>
       <c r="F87" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G87" s="8"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C88" s="3"/>
       <c r="D88" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E88" s="3"/>
       <c r="F88" s="7"/>
       <c r="G88" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
       <c r="F89" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G89" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C90" s="3"/>
       <c r="D90" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E90" s="3"/>
       <c r="F90" s="7"/>
       <c r="G90" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E91" s="3"/>
       <c r="F91" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G91" s="8"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
       <c r="D92" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E92" s="3"/>
       <c r="F92" s="7"/>
@@ -2498,88 +2502,88 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
       <c r="D93" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E93" s="3"/>
       <c r="F93" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G93" s="8"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
       <c r="F94" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G94" s="8"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
       <c r="F95" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G95" s="8"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
       <c r="F96" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G96" s="8"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C97" s="3"/>
       <c r="D97" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E97" s="3"/>
       <c r="F97" s="7"/>
       <c r="G97" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D98" s="3"/>
       <c r="E98" s="3"/>
@@ -2588,124 +2592,124 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
       <c r="F99" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G99" s="8"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
       <c r="E100" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G100" s="8"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
       <c r="F101" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G101" s="8"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D102" s="3"/>
       <c r="E102" s="3"/>
       <c r="F102" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G102" s="8"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
       <c r="D103" s="3"/>
       <c r="E103" s="3"/>
       <c r="F103" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G103" s="8"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E104" s="3"/>
       <c r="F104" s="7"/>
       <c r="G104" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C105" s="3"/>
       <c r="D105" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E105" s="3"/>
       <c r="F105" s="7"/>
       <c r="G105" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D106" s="3"/>
       <c r="E106" s="3"/>
@@ -2714,37 +2718,37 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D107" s="3"/>
       <c r="E107" s="3"/>
       <c r="F107" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G107" s="8"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
       <c r="D108" s="3"/>
       <c r="E108" s="3"/>
       <c r="F108" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G108" s="8"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
@@ -2755,160 +2759,160 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D110" s="3"/>
       <c r="E110" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F110" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G110" s="8"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B111" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C111" s="11"/>
       <c r="D111" s="3"/>
       <c r="E111" s="3"/>
       <c r="F111" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G111" s="8"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E112" s="3"/>
       <c r="F112" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G112" s="8"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
       <c r="D113" s="3"/>
       <c r="E113" s="3"/>
       <c r="F113" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G113" s="8"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D114" s="3"/>
       <c r="E114" s="3"/>
       <c r="F114" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G114" s="8"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D115" s="3"/>
       <c r="E115" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F115" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G115" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E116" s="3"/>
       <c r="F116" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G116" s="8"/>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D117" s="3"/>
       <c r="E117" s="3"/>
       <c r="F117" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G117" s="8"/>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
       <c r="D118" s="3"/>
       <c r="E118" s="3"/>
       <c r="F118" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G118" s="8"/>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
@@ -2919,28 +2923,28 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
       <c r="D120" s="3"/>
       <c r="E120" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F120" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G120" s="8"/>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D121" s="3"/>
       <c r="E121" s="3"/>
@@ -2949,13 +2953,13 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D122" s="3"/>
       <c r="E122" s="3"/>
@@ -2964,34 +2968,34 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B123" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C123" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D123" s="3"/>
       <c r="E123" s="3"/>
       <c r="F123" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G123" s="8"/>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove mobaxterm as default install from chocolatey
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\ubuntu\projects\wiki\Settings\Chocolatey\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ubuntu\projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5AAEDD-9A57-4368-8A42-3960305C84CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A92C09-040B-4225-B744-449E063E0F27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39180" yWindow="780" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="156">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -670,10 +670,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Gut" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -694,7 +694,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1018,10 +1018,10 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G79" sqref="G79"/>
+      <selection pane="bottomLeft" activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
@@ -2087,9 +2087,7 @@
       <c r="A66" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B66" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
@@ -3014,7 +3012,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3026,7 +3024,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add Sweet Home 3D to choco
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ubuntu\projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986E8DAB-F33F-425C-86CA-0AB8ACE4627D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CDCBFB-3413-4351-8EAB-653A3FCE155F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43890" yWindow="2355" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$G$125</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$G$126</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="165">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -537,6 +537,12 @@
   </si>
   <si>
     <t>CD Emulator for ISO Images</t>
+  </si>
+  <si>
+    <t>sweet-home-3d</t>
+  </si>
+  <si>
+    <t>Grundriss, Raumplaner</t>
   </si>
 </sst>
 </file>
@@ -1046,11 +1052,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G129"/>
+  <dimension ref="A1:G130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G48" sqref="G48"/>
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F96" sqref="F96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2643,22 +2649,20 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="B100" s="3"/>
+      <c r="C100" s="3"/>
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
       <c r="F100" s="7"/>
-      <c r="G100" s="8"/>
+      <c r="G100" s="8" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>55</v>
@@ -2668,21 +2672,21 @@
       </c>
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
-      <c r="F101" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="F101" s="7"/>
       <c r="G101" s="8"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B102" s="3"/>
-      <c r="C102" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D102" s="3"/>
-      <c r="E102" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="E102" s="3"/>
       <c r="F102" s="7" t="s">
         <v>55</v>
       </c>
@@ -2690,27 +2694,25 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
       <c r="D103" s="3"/>
-      <c r="E103" s="3"/>
+      <c r="E103" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F103" s="7" t="s">
         <v>55</v>
       </c>
       <c r="G103" s="8"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A104" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B104" s="3"/>
+      <c r="C104" s="3"/>
       <c r="D104" s="3"/>
       <c r="E104" s="3"/>
       <c r="F104" s="7" t="s">
@@ -2719,11 +2721,15 @@
       <c r="G104" s="8"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="B105" s="3"/>
-      <c r="C105" s="3"/>
+      <c r="A105" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D105" s="3"/>
       <c r="E105" s="3"/>
       <c r="F105" s="7" t="s">
@@ -2732,59 +2738,57 @@
       <c r="G105" s="8"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="4" t="s">
+      <c r="A106" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B106" s="3"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
+      <c r="E106" s="3"/>
+      <c r="F106" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G106" s="8"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B106" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D106" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E106" s="3"/>
-      <c r="F106" s="7"/>
-      <c r="G106" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="14" t="s">
-        <v>92</v>
-      </c>
       <c r="B107" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C107" s="3"/>
+      <c r="C107" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D107" s="3" t="s">
         <v>55</v>
       </c>
       <c r="E107" s="3"/>
       <c r="F107" s="7"/>
       <c r="G107" s="10" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
-        <v>42</v>
+      <c r="A108" s="14" t="s">
+        <v>92</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C108" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D108" s="3"/>
+      <c r="C108" s="3"/>
+      <c r="D108" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E108" s="3"/>
       <c r="F108" s="7"/>
-      <c r="G108" s="8"/>
+      <c r="G108" s="10" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>55</v>
@@ -2794,17 +2798,19 @@
       </c>
       <c r="D109" s="3"/>
       <c r="E109" s="3"/>
-      <c r="F109" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="F109" s="7"/>
       <c r="G109" s="8"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B110" s="3"/>
-      <c r="C110" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D110" s="3"/>
       <c r="E110" s="3"/>
       <c r="F110" s="7" t="s">
@@ -2814,62 +2820,56 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
       <c r="D111" s="3"/>
       <c r="E111" s="3"/>
-      <c r="F111" s="7"/>
+      <c r="F111" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="G111" s="8"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B112" s="3"/>
+      <c r="C112" s="3"/>
+      <c r="D112" s="3"/>
+      <c r="E112" s="3"/>
+      <c r="F112" s="7"/>
+      <c r="G112" s="8"/>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B112" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C112" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D112" s="3"/>
-      <c r="E112" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F112" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G112" s="8"/>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" s="4" t="s">
+      <c r="B113" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D113" s="3"/>
+      <c r="E113" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F113" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G113" s="8"/>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B113" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C113" s="11"/>
-      <c r="D113" s="3"/>
-      <c r="E113" s="3"/>
-      <c r="F113" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G113" s="8"/>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D114" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="B114" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C114" s="11"/>
+      <c r="D114" s="3"/>
       <c r="E114" s="3"/>
       <c r="F114" s="7" t="s">
         <v>55</v>
@@ -2878,11 +2878,17 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B115" s="3"/>
-      <c r="C115" s="3"/>
-      <c r="D115" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E115" s="3"/>
       <c r="F115" s="7" t="s">
         <v>55</v>
@@ -2890,48 +2896,40 @@
       <c r="G115" s="8"/>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C116" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A116" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B116" s="3"/>
+      <c r="C116" s="3"/>
       <c r="D116" s="3"/>
       <c r="E116" s="3"/>
       <c r="F116" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="G116" s="8" t="s">
+      <c r="G116" s="8"/>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D117" s="3"/>
+      <c r="E117" s="3"/>
+      <c r="F117" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G117" s="8" t="s">
         <v>162</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B117" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C117" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D117" s="3"/>
-      <c r="E117" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F117" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G117" s="8" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>55</v>
@@ -2939,18 +2937,20 @@
       <c r="C118" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D118" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E118" s="3"/>
+      <c r="D118" s="3"/>
+      <c r="E118" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F118" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="G118" s="8"/>
+      <c r="G118" s="8" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>55</v>
@@ -2958,7 +2958,9 @@
       <c r="C119" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D119" s="3"/>
+      <c r="D119" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E119" s="3"/>
       <c r="F119" s="7" t="s">
         <v>55</v>
@@ -2967,10 +2969,14 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B120" s="3"/>
-      <c r="C120" s="3"/>
+        <v>51</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D120" s="3"/>
       <c r="E120" s="3"/>
       <c r="F120" s="7" t="s">
@@ -2979,49 +2985,47 @@
       <c r="G120" s="8"/>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A121" s="12" t="s">
-        <v>133</v>
+      <c r="A121" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
       <c r="D121" s="3"/>
       <c r="E121" s="3"/>
-      <c r="F121" s="7"/>
+      <c r="F121" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="G121" s="8"/>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A122" s="4" t="s">
-        <v>66</v>
+      <c r="A122" s="12" t="s">
+        <v>133</v>
       </c>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
       <c r="D122" s="3"/>
-      <c r="E122" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F122" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="E122" s="3"/>
+      <c r="F122" s="7"/>
       <c r="G122" s="8"/>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
+      <c r="A123" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B123" s="3"/>
+      <c r="C123" s="3"/>
+      <c r="D123" s="3"/>
+      <c r="E123" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F123" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G123" s="8"/>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B123" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C123" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D123" s="3"/>
-      <c r="E123" s="3"/>
-      <c r="F123" s="7"/>
-      <c r="G123" s="8"/>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A124" s="14" t="s">
-        <v>53</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>55</v>
@@ -3035,39 +3039,54 @@
       <c r="G124" s="8"/>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A125" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B125" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C125" s="11" t="s">
+      <c r="A125" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C125" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D125" s="3"/>
       <c r="E125" s="3"/>
-      <c r="F125" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="F125" s="7"/>
       <c r="G125" s="8"/>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A127" s="14" t="s">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B126" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C126" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D126" s="3"/>
+      <c r="E126" s="3"/>
+      <c r="F126" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G126" s="8"/>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" s="14" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A128" s="12" t="s">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="12" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="13" t="s">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="13" t="s">
         <v>135</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G125" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G126" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="F1" r:id="rId1" display="https://github.com/microsoft/winget-pkgs" xr:uid="{2C434A13-8B1C-492F-95C8-B89737A54984}"/>
     <hyperlink ref="A47" r:id="rId2" xr:uid="{5AAD9A6E-C562-4737-9662-CEC2B195962E}"/>

</xml_diff>

<commit_message>
add keystore installation note
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ubuntu\projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A3858D-A3C1-4660-ABAF-ECE4363FCE24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9195492-9DDB-4A84-8A0B-AD65534D5DAB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="255" windowWidth="38640" windowHeight="20865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="167">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -546,6 +546,9 @@
       </rPr>
       <t>!)</t>
     </r>
+  </si>
+  <si>
+    <t>Only compatible with Java 8. Place jre dir of Java 8 into Keystore Install dir.</t>
   </si>
 </sst>
 </file>
@@ -1058,8 +1061,8 @@
   <dimension ref="A1:I130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H35" sqref="H35"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2103,7 +2106,9 @@
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
       <c r="G59" s="7"/>
-      <c r="H59" s="8"/>
+      <c r="H59" s="8" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">

</xml_diff>

<commit_message>
update chocolatey for work
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ubuntu\projects\wiki\Settings\Chocolatey\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\ubuntu\projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9195492-9DDB-4A84-8A0B-AD65534D5DAB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03AE1921-1945-4631-9FD0-E934A5ED6906}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="255" windowWidth="38640" windowHeight="20865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="168">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -328,9 +328,6 @@
   </si>
   <si>
     <t>insomnia-rest-api-client</t>
-  </si>
-  <si>
-    <t>adoptopenjdk14</t>
   </si>
   <si>
     <t>Bemerkungen</t>
@@ -549,6 +546,12 @@
   </si>
   <si>
     <t>Only compatible with Java 8. Place jre dir of Java 8 into Keystore Install dir.</t>
+  </si>
+  <si>
+    <t>adoptopenjdk16</t>
+  </si>
+  <si>
+    <t>Use JetBrains Toolbox for work</t>
   </si>
 </sst>
 </file>
@@ -1061,8 +1064,8 @@
   <dimension ref="A1:I130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H59" sqref="H59"/>
+      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,7 +1088,7 @@
         <v>70</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>72</v>
@@ -1094,13 +1097,13 @@
         <v>71</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1202,7 +1205,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>101</v>
+        <v>166</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>55</v>
@@ -1296,7 +1299,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1316,9 +1319,7 @@
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="7"/>
@@ -1326,25 +1327,23 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="7"/>
       <c r="H15" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1356,7 +1355,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>55</v>
@@ -1391,12 +1390,12 @@
         <v>55</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>55</v>
@@ -1407,7 +1406,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="7"/>
       <c r="H19" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1436,7 +1435,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>55</v>
@@ -1452,7 +1451,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>55</v>
@@ -1470,7 +1469,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>55</v>
@@ -1532,7 +1531,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>55</v>
@@ -1550,7 +1549,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>55</v>
@@ -1563,7 +1562,7 @@
         <v>55</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1588,38 +1587,38 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
+      <c r="D31" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3" t="s">
         <v>55</v>
       </c>
       <c r="G31" s="7"/>
       <c r="H31" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C32" s="3"/>
-      <c r="D32" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="7"/>
       <c r="H32" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1673,7 +1672,7 @@
       <c r="F35" s="3"/>
       <c r="G35" s="7"/>
       <c r="H35" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1684,9 +1683,7 @@
         <v>55</v>
       </c>
       <c r="C36" s="3"/>
-      <c r="D36" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="7"/>
@@ -1696,7 +1693,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1709,7 +1706,7 @@
         <v>55</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -1763,7 +1760,7 @@
         <v>55</v>
       </c>
       <c r="H40" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -1814,9 +1811,7 @@
         <v>55</v>
       </c>
       <c r="C43" s="3"/>
-      <c r="D43" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="7"/>
@@ -1824,7 +1819,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>55</v>
@@ -1839,7 +1834,7 @@
         <v>55</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -1848,9 +1843,7 @@
       </c>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
-      <c r="D45" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="7"/>
@@ -1876,11 +1869,13 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
+      <c r="D47" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3" t="s">
         <v>55</v>
@@ -1889,7 +1884,7 @@
         <v>55</v>
       </c>
       <c r="H47" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -1909,7 +1904,7 @@
       <c r="F48" s="3"/>
       <c r="G48" s="7"/>
       <c r="H48" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -1940,16 +1935,14 @@
         <v>55</v>
       </c>
       <c r="C50" s="3"/>
-      <c r="D50" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D50" s="3"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
       <c r="G50" s="7" t="s">
         <v>55</v>
       </c>
       <c r="H50" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -1960,13 +1953,13 @@
         <v>55</v>
       </c>
       <c r="C51" s="3"/>
-      <c r="D51" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D51" s="3"/>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="7"/>
-      <c r="H51" s="8"/>
+      <c r="H51" s="8" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
@@ -2045,7 +2038,7 @@
         <v>55</v>
       </c>
       <c r="H56" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -2107,7 +2100,7 @@
       <c r="F59" s="3"/>
       <c r="G59" s="7"/>
       <c r="H59" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -2116,9 +2109,7 @@
       </c>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
-      <c r="D60" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
       <c r="G60" s="7"/>
@@ -2126,7 +2117,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>55</v>
@@ -2139,12 +2130,12 @@
       <c r="F61" s="3"/>
       <c r="G61" s="7"/>
       <c r="H61" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -2155,7 +2146,7 @@
         <v>55</v>
       </c>
       <c r="H62" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -2168,7 +2159,9 @@
       <c r="C63" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D63" s="3"/>
+      <c r="D63" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
       <c r="G63" s="7"/>
@@ -2176,7 +2169,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B64" s="11" t="s">
         <v>55</v>
@@ -2212,7 +2205,7 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -2221,12 +2214,12 @@
       <c r="F66" s="3"/>
       <c r="G66" s="7"/>
       <c r="H66" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>55</v>
@@ -2239,7 +2232,7 @@
         <v>55</v>
       </c>
       <c r="H67" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -2288,7 +2281,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -2304,7 +2297,7 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>55</v>
@@ -2427,7 +2420,7 @@
         <v>55</v>
       </c>
       <c r="H78" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -2452,9 +2445,7 @@
         <v>55</v>
       </c>
       <c r="C80" s="3"/>
-      <c r="D80" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D80" s="3"/>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
       <c r="G80" s="7"/>
@@ -2462,13 +2453,11 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
-      <c r="D81" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D81" s="3"/>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
       <c r="G81" s="7" t="s">
@@ -2520,7 +2509,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>55</v>
@@ -2594,9 +2583,7 @@
         <v>55</v>
       </c>
       <c r="C89" s="3"/>
-      <c r="D89" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D89" s="3"/>
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
       <c r="G89" s="7" t="s">
@@ -2606,25 +2593,23 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C90" s="3"/>
-      <c r="D90" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D90" s="3"/>
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
       <c r="G90" s="7"/>
       <c r="H90" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>55</v>
@@ -2637,7 +2622,7 @@
         <v>55</v>
       </c>
       <c r="H91" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -2648,9 +2633,7 @@
         <v>55</v>
       </c>
       <c r="C92" s="3"/>
-      <c r="D92" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D92" s="3"/>
       <c r="E92" s="3"/>
       <c r="F92" s="3"/>
       <c r="G92" s="7"/>
@@ -2668,9 +2651,7 @@
       <c r="C93" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D93" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D93" s="3"/>
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
       <c r="G93" s="7" t="s">
@@ -2684,9 +2665,7 @@
       </c>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
-      <c r="D94" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D94" s="3"/>
       <c r="E94" s="3"/>
       <c r="F94" s="3"/>
       <c r="G94" s="7"/>
@@ -2756,25 +2735,23 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C99" s="3"/>
-      <c r="D99" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D99" s="3"/>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
       <c r="G99" s="7"/>
       <c r="H99" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
@@ -2783,7 +2760,7 @@
       <c r="F100" s="3"/>
       <c r="G100" s="7"/>
       <c r="H100" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -2870,7 +2847,7 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
@@ -2892,9 +2869,7 @@
       <c r="C107" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D107" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D107" s="3"/>
       <c r="E107" s="3"/>
       <c r="F107" s="3"/>
       <c r="G107" s="7"/>
@@ -2910,9 +2885,7 @@
         <v>55</v>
       </c>
       <c r="C108" s="3"/>
-      <c r="D108" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D108" s="3"/>
       <c r="E108" s="3"/>
       <c r="F108" s="3"/>
       <c r="G108" s="7"/>
@@ -3004,7 +2977,7 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B114" s="11" t="s">
         <v>55</v>
@@ -3069,7 +3042,7 @@
         <v>55</v>
       </c>
       <c r="H117" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -3082,7 +3055,9 @@
       <c r="C118" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D118" s="3"/>
+      <c r="D118" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E118" s="3" t="s">
         <v>55</v>
       </c>
@@ -3091,7 +3066,7 @@
         <v>55</v>
       </c>
       <c r="H118" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -3134,7 +3109,7 @@
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
@@ -3148,7 +3123,7 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
@@ -3208,7 +3183,7 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B126" s="11" t="s">
         <v>55</v>
@@ -3228,17 +3203,17 @@
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
install bat as a requirement for git-bash
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\ubuntu\projects\wiki\Settings\Chocolatey\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A408CBF4-C1E6-4073-A248-496BAA92380A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBAD50E6-45A6-4608-8001-DC76A51E641D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="169">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -1067,8 +1067,8 @@
   <dimension ref="A1:I131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,7 +1336,9 @@
         <v>55</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="7"/>

</xml_diff>

<commit_message>
add fd to work installation
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\wiki\Settings\Chocolatey\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\ubuntu\projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBAD50E6-45A6-4608-8001-DC76A51E641D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83BA0BF-7326-42A2-870D-72FE02C6554A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="169">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -1068,7 +1068,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1618,7 +1618,9 @@
         <v>55</v>
       </c>
       <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
+      <c r="D32" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="7"/>

</xml_diff>

<commit_message>
upgrade to win 10
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\ubuntu\projects\wiki\Settings\Chocolatey\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ubuntu\projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730A0175-FC4D-45C6-9D19-FC3C86335C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C64644B-7DD2-481C-80E8-5840BD5838B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$128</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$129</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="172">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -558,6 +558,12 @@
   </si>
   <si>
     <t>keepassxc</t>
+  </si>
+  <si>
+    <t>shexview</t>
+  </si>
+  <si>
+    <t>ShellExView, disable broken context menu entries (e.g. for Win 11)</t>
   </si>
 </sst>
 </file>
@@ -1067,11 +1073,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I132"/>
+  <dimension ref="A1:I133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H95" sqref="H95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2712,58 +2718,60 @@
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>85</v>
+      <c r="A95" s="4" t="s">
+        <v>170</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C95" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C95" s="3"/>
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
       <c r="F95" s="3"/>
-      <c r="G95" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H95" s="8"/>
+      <c r="G95" s="7"/>
+      <c r="H95" s="9" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B96" s="3"/>
-      <c r="C96" s="3"/>
+        <v>85</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
       <c r="F96" s="3"/>
-      <c r="G96" s="7"/>
+      <c r="G96" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="H96" s="8"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
-      <c r="D97" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D97" s="3"/>
       <c r="E97" s="3"/>
       <c r="F97" s="3"/>
-      <c r="G97" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="G97" s="7"/>
       <c r="H97" s="8"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
-      <c r="D98" s="3"/>
+      <c r="D98" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E98" s="3"/>
       <c r="F98" s="3"/>
       <c r="G98" s="7" t="s">
@@ -2773,14 +2781,10 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B99" s="3"/>
+      <c r="C99" s="3"/>
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
@@ -2791,10 +2795,14 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B100" s="3"/>
-      <c r="C100" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
@@ -2804,54 +2812,52 @@
       <c r="H100" s="8"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A101" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B101" s="3"/>
       <c r="C101" s="3"/>
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
       <c r="F101" s="3"/>
-      <c r="G101" s="7"/>
-      <c r="H101" s="8" t="s">
-        <v>125</v>
-      </c>
+      <c r="G101" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H101" s="8"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B102" s="3"/>
+      <c r="A102" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C102" s="3"/>
       <c r="D102" s="3"/>
       <c r="E102" s="3"/>
       <c r="F102" s="3"/>
       <c r="G102" s="7"/>
       <c r="H102" s="8" t="s">
-        <v>162</v>
+        <v>125</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="B103" s="3"/>
+      <c r="C103" s="3"/>
       <c r="D103" s="3"/>
       <c r="E103" s="3"/>
       <c r="F103" s="3"/>
       <c r="G103" s="7"/>
-      <c r="H103" s="8"/>
+      <c r="H103" s="8" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>55</v>
@@ -2862,21 +2868,21 @@
       <c r="D104" s="3"/>
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
-      <c r="G104" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="G104" s="7"/>
       <c r="H104" s="8"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B105" s="3"/>
-      <c r="C105" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D105" s="3"/>
-      <c r="E105" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="E105" s="3"/>
       <c r="F105" s="3"/>
       <c r="G105" s="7" t="s">
         <v>55</v>
@@ -2885,12 +2891,14 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
       <c r="D106" s="3"/>
-      <c r="E106" s="3"/>
+      <c r="E106" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F106" s="3"/>
       <c r="G106" s="7" t="s">
         <v>55</v>
@@ -2898,15 +2906,11 @@
       <c r="H106" s="8"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A107" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A107" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B107" s="3"/>
+      <c r="C107" s="3"/>
       <c r="D107" s="3"/>
       <c r="E107" s="3"/>
       <c r="F107" s="3"/>
@@ -2916,11 +2920,15 @@
       <c r="H107" s="8"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A108" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="B108" s="3"/>
-      <c r="C108" s="3"/>
+      <c r="A108" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D108" s="3"/>
       <c r="E108" s="3"/>
       <c r="F108" s="3"/>
@@ -2930,60 +2938,58 @@
       <c r="H108" s="8"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A109" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A109" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B109" s="3"/>
+      <c r="C109" s="3"/>
       <c r="D109" s="3"/>
       <c r="E109" s="3"/>
       <c r="F109" s="3"/>
       <c r="G109" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H109" s="10" t="s">
-        <v>75</v>
-      </c>
+      <c r="H109" s="8"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A110" s="14" t="s">
-        <v>92</v>
+      <c r="A110" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C110" s="3"/>
+      <c r="C110" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D110" s="3"/>
       <c r="E110" s="3"/>
       <c r="F110" s="3"/>
-      <c r="G110" s="7"/>
+      <c r="G110" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="H110" s="10" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
-        <v>42</v>
+      <c r="A111" s="14" t="s">
+        <v>92</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C111" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C111" s="3"/>
       <c r="D111" s="3"/>
       <c r="E111" s="3"/>
       <c r="F111" s="3"/>
       <c r="G111" s="7"/>
-      <c r="H111" s="8"/>
+      <c r="H111" s="10" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>55</v>
@@ -2994,17 +3000,19 @@
       <c r="D112" s="3"/>
       <c r="E112" s="3"/>
       <c r="F112" s="3"/>
-      <c r="G112" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="G112" s="7"/>
       <c r="H112" s="8"/>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B113" s="3"/>
-      <c r="C113" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D113" s="3"/>
       <c r="E113" s="3"/>
       <c r="F113" s="3"/>
@@ -3015,7 +3023,7 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
@@ -3029,55 +3037,49 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B115" s="3"/>
+      <c r="C115" s="3"/>
+      <c r="D115" s="3"/>
+      <c r="E115" s="3"/>
+      <c r="F115" s="3"/>
+      <c r="G115" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H115" s="8"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B115" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D115" s="3"/>
-      <c r="E115" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F115" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G115" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H115" s="8"/>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A116" s="4" t="s">
+      <c r="B116" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D116" s="3"/>
+      <c r="E116" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G116" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H116" s="8"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A117" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B116" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C116" s="11"/>
-      <c r="D116" s="3"/>
-      <c r="E116" s="3"/>
-      <c r="F116" s="3"/>
-      <c r="G116" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H116" s="8"/>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B117" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C117" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D117" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="B117" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C117" s="11"/>
+      <c r="D117" s="3"/>
       <c r="E117" s="3"/>
       <c r="F117" s="3"/>
       <c r="G117" s="7" t="s">
@@ -3087,11 +3089,17 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B118" s="3"/>
-      <c r="C118" s="3"/>
-      <c r="D118" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E118" s="3"/>
       <c r="F118" s="3"/>
       <c r="G118" s="7" t="s">
@@ -3100,28 +3108,22 @@
       <c r="H118" s="8"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A119" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B119" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C119" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A119" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B119" s="3"/>
+      <c r="C119" s="3"/>
       <c r="D119" s="3"/>
       <c r="E119" s="3"/>
       <c r="F119" s="3"/>
       <c r="G119" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H119" s="8" t="s">
-        <v>160</v>
-      </c>
+      <c r="H119" s="8"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
-        <v>49</v>
+      <c r="A120" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>55</v>
@@ -3129,23 +3131,19 @@
       <c r="C120" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D120" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E120" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D120" s="3"/>
+      <c r="E120" s="3"/>
       <c r="F120" s="3"/>
       <c r="G120" s="7" t="s">
         <v>55</v>
       </c>
       <c r="H120" s="8" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>55</v>
@@ -3156,16 +3154,20 @@
       <c r="D121" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E121" s="3"/>
+      <c r="E121" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F121" s="3"/>
       <c r="G121" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H121" s="8"/>
+      <c r="H121" s="8" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>55</v>
@@ -3173,7 +3175,9 @@
       <c r="C122" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D122" s="3"/>
+      <c r="D122" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E122" s="3"/>
       <c r="F122" s="3"/>
       <c r="G122" s="7" t="s">
@@ -3183,10 +3187,14 @@
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B123" s="3"/>
-      <c r="C123" s="3"/>
+        <v>51</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D123" s="3"/>
       <c r="E123" s="3"/>
       <c r="F123" s="3"/>
@@ -3196,52 +3204,50 @@
       <c r="H123" s="8"/>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A124" s="12" t="s">
-        <v>131</v>
+      <c r="A124" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
       <c r="D124" s="3"/>
       <c r="E124" s="3"/>
       <c r="F124" s="3"/>
-      <c r="G124" s="7"/>
+      <c r="G124" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="H124" s="8"/>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A125" s="4" t="s">
-        <v>66</v>
+      <c r="A125" s="12" t="s">
+        <v>131</v>
       </c>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
       <c r="D125" s="3"/>
-      <c r="E125" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="E125" s="3"/>
       <c r="F125" s="3"/>
-      <c r="G125" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="G125" s="7"/>
       <c r="H125" s="8"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
+      <c r="A126" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B126" s="3"/>
+      <c r="C126" s="3"/>
+      <c r="D126" s="3"/>
+      <c r="E126" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F126" s="3"/>
+      <c r="G126" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H126" s="8"/>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C126" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D126" s="3"/>
-      <c r="E126" s="3"/>
-      <c r="F126" s="3"/>
-      <c r="G126" s="7"/>
-      <c r="H126" s="8"/>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A127" s="14" t="s">
-        <v>53</v>
       </c>
       <c r="B127" s="3" t="s">
         <v>55</v>
@@ -3256,42 +3262,58 @@
       <c r="H127" s="8"/>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A128" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B128" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C128" s="11" t="s">
+      <c r="A128" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C128" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D128" s="3"/>
       <c r="E128" s="3"/>
-      <c r="F128" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G128" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="F128" s="3"/>
+      <c r="G128" s="7"/>
       <c r="H128" s="8"/>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="14" t="s">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B129" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C129" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D129" s="3"/>
+      <c r="E129" s="3"/>
+      <c r="F129" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G129" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H129" s="8"/>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A131" s="14" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="12" t="s">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A132" s="12" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="13" t="s">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A133" s="13" t="s">
         <v>133</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H128" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H129" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="G1" r:id="rId1" display="https://github.com/microsoft/winget-pkgs" xr:uid="{2C434A13-8B1C-492F-95C8-B89737A54984}"/>
     <hyperlink ref="A47" r:id="rId2" xr:uid="{5AAD9A6E-C562-4737-9662-CEC2B195962E}"/>

</xml_diff>

<commit_message>
add WinAuth to choco
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ubuntu\projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C64644B-7DD2-481C-80E8-5840BD5838B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15786AC1-4DC6-45FF-9DA1-E0C268998F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$129</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$130</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="174">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -564,6 +564,12 @@
   </si>
   <si>
     <t>ShellExView, disable broken context menu entries (e.g. for Win 11)</t>
+  </si>
+  <si>
+    <t>WinAuth</t>
+  </si>
+  <si>
+    <t>Authenticator</t>
   </si>
 </sst>
 </file>
@@ -1073,11 +1079,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I133"/>
+  <dimension ref="A1:I134"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H95" sqref="H95"/>
+      <selection pane="bottomLeft" activeCell="A120" sqref="A120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3122,28 +3128,24 @@
       <c r="H119" s="8"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A120" s="4" t="s">
-        <v>73</v>
+      <c r="A120" s="1" t="s">
+        <v>172</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C120" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C120" s="3"/>
       <c r="D120" s="3"/>
       <c r="E120" s="3"/>
       <c r="F120" s="3"/>
-      <c r="G120" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="G120" s="7"/>
       <c r="H120" s="8" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
-        <v>49</v>
+      <c r="A121" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>55</v>
@@ -3151,23 +3153,19 @@
       <c r="C121" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D121" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E121" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D121" s="3"/>
+      <c r="E121" s="3"/>
       <c r="F121" s="3"/>
       <c r="G121" s="7" t="s">
         <v>55</v>
       </c>
       <c r="H121" s="8" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>55</v>
@@ -3178,16 +3176,20 @@
       <c r="D122" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E122" s="3"/>
+      <c r="E122" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F122" s="3"/>
       <c r="G122" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H122" s="8"/>
+      <c r="H122" s="8" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>55</v>
@@ -3195,7 +3197,9 @@
       <c r="C123" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D123" s="3"/>
+      <c r="D123" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E123" s="3"/>
       <c r="F123" s="3"/>
       <c r="G123" s="7" t="s">
@@ -3205,10 +3209,14 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B124" s="3"/>
-      <c r="C124" s="3"/>
+        <v>51</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D124" s="3"/>
       <c r="E124" s="3"/>
       <c r="F124" s="3"/>
@@ -3218,52 +3226,50 @@
       <c r="H124" s="8"/>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A125" s="12" t="s">
-        <v>131</v>
+      <c r="A125" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
       <c r="D125" s="3"/>
       <c r="E125" s="3"/>
       <c r="F125" s="3"/>
-      <c r="G125" s="7"/>
+      <c r="G125" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="H125" s="8"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A126" s="4" t="s">
-        <v>66</v>
+      <c r="A126" s="12" t="s">
+        <v>131</v>
       </c>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
       <c r="D126" s="3"/>
-      <c r="E126" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="E126" s="3"/>
       <c r="F126" s="3"/>
-      <c r="G126" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="G126" s="7"/>
       <c r="H126" s="8"/>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
+      <c r="A127" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B127" s="3"/>
+      <c r="C127" s="3"/>
+      <c r="D127" s="3"/>
+      <c r="E127" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F127" s="3"/>
+      <c r="G127" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H127" s="8"/>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C127" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D127" s="3"/>
-      <c r="E127" s="3"/>
-      <c r="F127" s="3"/>
-      <c r="G127" s="7"/>
-      <c r="H127" s="8"/>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A128" s="14" t="s">
-        <v>53</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>55</v>
@@ -3278,42 +3284,58 @@
       <c r="H128" s="8"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A129" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B129" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C129" s="11" t="s">
+      <c r="A129" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C129" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D129" s="3"/>
       <c r="E129" s="3"/>
-      <c r="F129" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G129" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="F129" s="3"/>
+      <c r="G129" s="7"/>
       <c r="H129" s="8"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A131" s="14" t="s">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B130" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C130" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D130" s="3"/>
+      <c r="E130" s="3"/>
+      <c r="F130" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G130" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H130" s="8"/>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A132" s="14" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A132" s="12" t="s">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A133" s="12" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A133" s="13" t="s">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A134" s="13" t="s">
         <v>133</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H129" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H130" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="G1" r:id="rId1" display="https://github.com/microsoft/winget-pkgs" xr:uid="{2C434A13-8B1C-492F-95C8-B89737A54984}"/>
     <hyperlink ref="A47" r:id="rId2" xr:uid="{5AAD9A6E-C562-4737-9662-CEC2B195962E}"/>

</xml_diff>

<commit_message>
feat: migrate to Temurin
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ubuntu\projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15786AC1-4DC6-45FF-9DA1-E0C268998F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6FB9AB-3CD0-457D-BBE2-B1736EB4D95D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$130</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$129</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="176">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -273,9 +273,6 @@
     <t>intellijidea-ultimate</t>
   </si>
   <si>
-    <t>jdk8</t>
-  </si>
-  <si>
     <t>mysql</t>
   </si>
   <si>
@@ -289,12 +286,6 @@
   </si>
   <si>
     <t>GitHub</t>
-  </si>
-  <si>
-    <t>adoptopenjdk11</t>
-  </si>
-  <si>
-    <t>adoptopenjdk8</t>
   </si>
   <si>
     <t>keystore-explorer.portable</t>
@@ -548,9 +539,6 @@
     <t>Only compatible with Java 8. Place jre dir of Java 8 into Keystore Install dir.</t>
   </si>
   <si>
-    <t>adoptopenjdk16</t>
-  </si>
-  <si>
     <t>Use JetBrains Toolbox for work</t>
   </si>
   <si>
@@ -570,6 +558,24 @@
   </si>
   <si>
     <t>Authenticator</t>
+  </si>
+  <si>
+    <t>temurin17</t>
+  </si>
+  <si>
+    <t>JDK 17</t>
+  </si>
+  <si>
+    <t>JDK 8</t>
+  </si>
+  <si>
+    <t>JDK 11</t>
+  </si>
+  <si>
+    <t>temurin8</t>
+  </si>
+  <si>
+    <t>temurin11</t>
   </si>
 </sst>
 </file>
@@ -1079,11 +1085,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I134"/>
+  <dimension ref="A1:H133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A120" sqref="A120"/>
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G100" sqref="G100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,7 +1102,7 @@
     <col min="8" max="8" width="66.42578125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>54</v>
       </c>
@@ -1104,7 +1110,7 @@
         <v>70</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>72</v>
@@ -1113,16 +1119,16 @@
         <v>71</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>58</v>
       </c>
@@ -1146,7 +1152,7 @@
       </c>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1161,9 +1167,8 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="7"/>
-      <c r="I3" s="8"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>59</v>
       </c>
@@ -1187,15 +1192,13 @@
       </c>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>89</v>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="7" t="s">
@@ -1203,189 +1206,191 @@
       </c>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>88</v>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F6" s="3"/>
       <c r="G6" s="7" t="s">
         <v>55</v>
       </c>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>55</v>
-      </c>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="G7" s="7"/>
       <c r="H7" s="8"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>1</v>
+        <v>94</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="G8" s="7"/>
       <c r="H8" s="8"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3" t="s">
-        <v>55</v>
-      </c>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="7" t="s">
         <v>55</v>
       </c>
       <c r="H9" s="8"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>96</v>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>101</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="7"/>
+      <c r="G10" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="H10" s="8"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>97</v>
+        <v>2</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="7"/>
       <c r="H11" s="8"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>60</v>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>115</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
         <v>55</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>104</v>
+      <c r="G12" s="7"/>
+      <c r="H12" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="G13" s="7"/>
       <c r="H13" s="8"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="7"/>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>118</v>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F15" s="3"/>
-      <c r="G15" s="7"/>
+      <c r="G15" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="H15" s="8" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B16" s="3"/>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="7"/>
-      <c r="H16" s="8"/>
+      <c r="H16" s="8" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="7"/>
@@ -1393,29 +1398,21 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H18" s="8" t="s">
-        <v>158</v>
-      </c>
+      <c r="H18" s="8"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>143</v>
+        <v>102</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>55</v>
@@ -1424,28 +1421,36 @@
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="8" t="s">
-        <v>144</v>
-      </c>
+      <c r="G19" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="8"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="3"/>
+        <v>142</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="7"/>
+      <c r="G20" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="H20" s="8"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="3"/>
+        <v>135</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -1456,14 +1461,16 @@
       <c r="H21" s="8"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>105</v>
+      <c r="A22" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="7" t="s">
@@ -1472,50 +1479,48 @@
       <c r="H22" s="8"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>145</v>
+      <c r="A23" s="14" t="s">
+        <v>6</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F23" s="3"/>
-      <c r="G23" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="G23" s="7"/>
       <c r="H23" s="8"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>138</v>
+        <v>7</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+      <c r="D24" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="G24" s="7"/>
       <c r="H24" s="8"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A25" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="7" t="s">
@@ -1524,76 +1529,84 @@
       <c r="H25" s="8"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="3"/>
+      <c r="A26" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="11"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="E26" s="3"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="8"/>
+      <c r="G26" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C27" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="7"/>
+      <c r="F27" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="H27" s="8"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D28" s="3"/>
+        <v>152</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H28" s="8"/>
+      <c r="F28" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G28" s="7"/>
+      <c r="H28" s="8" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="11"/>
-      <c r="D29" s="3"/>
+      <c r="A29" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="G29" s="7"/>
       <c r="H29" s="8" t="s">
-        <v>151</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>55</v>
@@ -1602,146 +1615,142 @@
         <v>55</v>
       </c>
       <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="E30" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F30" s="3"/>
+      <c r="G30" s="7"/>
       <c r="H30" s="8"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>155</v>
+        <v>10</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="3"/>
+      <c r="C31" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D31" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G31" s="7"/>
-      <c r="H31" s="8" t="s">
-        <v>156</v>
-      </c>
+      <c r="E31" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H31" s="8"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A32" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="3"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="7"/>
+      <c r="G32" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="H32" s="8" t="s">
-        <v>121</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>9</v>
+      <c r="A33" s="14" t="s">
+        <v>56</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C33" s="3"/>
       <c r="D33" s="3"/>
-      <c r="E33" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="7"/>
-      <c r="H33" s="8"/>
+      <c r="H33" s="8" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A34" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H34" s="8"/>
+      <c r="H34" s="8" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
+        <v>61</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H35" s="8" t="s">
-        <v>164</v>
-      </c>
+      <c r="H35" s="8"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="8" t="s">
-        <v>57</v>
-      </c>
+      <c r="G36" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H36" s="8"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A37" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H37" s="8" t="s">
-        <v>108</v>
+      <c r="H37" s="15" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>61</v>
+      <c r="A38" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>55</v>
@@ -1752,7 +1761,9 @@
       <c r="D38" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E38" s="3"/>
+      <c r="E38" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F38" s="3"/>
       <c r="G38" s="7" t="s">
         <v>55</v>
@@ -1761,10 +1772,14 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
@@ -1774,28 +1789,22 @@
       <c r="H39" s="8"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
-        <v>91</v>
+      <c r="A40" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
-      <c r="G40" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H40" s="15" t="s">
-        <v>137</v>
-      </c>
+      <c r="G40" s="7"/>
+      <c r="H40" s="8"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>12</v>
+        <v>136</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>55</v>
@@ -1803,39 +1812,33 @@
       <c r="C41" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H41" s="8"/>
+      <c r="H41" s="8" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A42" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
-      <c r="G42" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H42" s="8"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="8" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>55</v>
@@ -1844,52 +1847,66 @@
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
-      <c r="G43" s="7"/>
+      <c r="G43" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="H43" s="8"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D44" s="3"/>
+      <c r="A44" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
+      <c r="F44" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="G44" s="7" t="s">
         <v>55</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
+      <c r="A45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
+      <c r="E45" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F45" s="3"/>
-      <c r="G45" s="7"/>
+      <c r="G45" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="H45" s="8" t="s">
-        <v>87</v>
+        <v>155</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>15</v>
+        <v>91</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
+      <c r="C46" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
       <c r="G46" s="7" t="s">
@@ -1898,61 +1915,51 @@
       <c r="H46" s="8"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="B47" s="3"/>
+      <c r="A47" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C47" s="3"/>
-      <c r="D47" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D47" s="3"/>
       <c r="E47" s="3"/>
-      <c r="F47" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="F47" s="3"/>
       <c r="G47" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H47" s="8" t="s">
-        <v>157</v>
+      <c r="H47" s="15" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>16</v>
+      <c r="A48" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C48" s="3"/>
       <c r="D48" s="3"/>
-      <c r="E48" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="E48" s="3"/>
       <c r="F48" s="3"/>
       <c r="G48" s="7" t="s">
         <v>55</v>
       </c>
       <c r="H48" s="8" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E49" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F49" s="3"/>
       <c r="G49" s="7" t="s">
         <v>55</v>
@@ -1960,60 +1967,56 @@
       <c r="H49" s="8"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="13" t="s">
-        <v>100</v>
+      <c r="A50" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C50" s="3"/>
+      <c r="C50" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
-      <c r="G50" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H50" s="15" t="s">
-        <v>135</v>
-      </c>
+      <c r="G50" s="7"/>
+      <c r="H50" s="8"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>81</v>
+      <c r="A51" s="1" t="s">
+        <v>164</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
+      <c r="D51" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H51" s="8" t="s">
-        <v>167</v>
-      </c>
+      <c r="H51" s="8"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>17</v>
+      <c r="A52" s="14" t="s">
+        <v>19</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D52" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E52" s="3"/>
       <c r="F52" s="3"/>
-      <c r="G52" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="G52" s="7"/>
       <c r="H52" s="8"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>55</v>
@@ -2022,102 +2025,118 @@
         <v>55</v>
       </c>
       <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
+      <c r="E53" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F53" s="3"/>
-      <c r="G53" s="7"/>
-      <c r="H53" s="8"/>
+      <c r="G53" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H53" s="8" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>168</v>
+      <c r="A54" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C54" s="3"/>
+      <c r="C54" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D54" s="3" t="s">
         <v>55</v>
       </c>
       <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
+      <c r="F54" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="G54" s="7" t="s">
         <v>55</v>
       </c>
       <c r="H54" s="8"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
+      <c r="A55" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D55" s="3" t="s">
         <v>55</v>
       </c>
       <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="7"/>
+      <c r="F55" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="H55" s="8"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
+      <c r="A56" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="7"/>
+      <c r="F56" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="H56" s="8"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>20</v>
+      <c r="A57" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E57" s="3"/>
       <c r="F57" s="3"/>
       <c r="G57" s="7" t="s">
         <v>55</v>
       </c>
       <c r="H57" s="8" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A58" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
       <c r="E58" s="3"/>
-      <c r="F58" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G58" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="F58" s="3"/>
+      <c r="G58" s="7"/>
       <c r="H58" s="8"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
-        <v>169</v>
+      <c r="A59" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>55</v>
@@ -2125,93 +2144,89 @@
       <c r="C59" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D59" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D59" s="3"/>
       <c r="E59" s="3"/>
-      <c r="F59" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G59" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H59" s="8"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="7"/>
+      <c r="H59" s="8" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
       <c r="E60" s="3"/>
-      <c r="F60" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="F60" s="3"/>
       <c r="G60" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H60" s="8"/>
+      <c r="H60" s="8" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C61" s="3"/>
+      <c r="C61" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D61" s="3" t="s">
         <v>55</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
-      <c r="G61" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H61" s="8" t="s">
-        <v>165</v>
-      </c>
+      <c r="G61" s="7"/>
+      <c r="H61" s="8"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
+      <c r="A62" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>55</v>
+      </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="7"/>
+      <c r="F62" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G62" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="H62" s="8"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>141</v>
+        <v>23</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C63" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
-      <c r="G63" s="7"/>
-      <c r="H63" s="8" t="s">
-        <v>142</v>
-      </c>
+      <c r="G63" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H63" s="8"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -2222,58 +2237,46 @@
         <v>55</v>
       </c>
       <c r="H64" s="8" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
-        <v>77</v>
+      <c r="A65" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C65" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
-      <c r="G65" s="7"/>
-      <c r="H65" s="8"/>
+      <c r="G65" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H65" s="8" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B66" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C66" s="11" t="s">
-        <v>55</v>
-      </c>
+      <c r="A66" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
-      <c r="F66" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G66" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="F66" s="3"/>
+      <c r="G66" s="7"/>
       <c r="H66" s="8"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B67" s="3"/>
       <c r="C67" s="3"/>
-      <c r="D67" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D67" s="3"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
       <c r="G67" s="7" t="s">
@@ -2283,74 +2286,80 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
       <c r="G68" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H68" s="8" t="s">
-        <v>110</v>
-      </c>
+      <c r="H68" s="8"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="B69" s="3"/>
       <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
+      <c r="D69" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
       <c r="G69" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H69" s="8" t="s">
-        <v>148</v>
-      </c>
+      <c r="H69" s="8"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B70" s="3"/>
+        <v>110</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
+      <c r="D70" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
-      <c r="G70" s="7"/>
+      <c r="G70" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="H70" s="8"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
+      <c r="A71" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
-      <c r="F71" s="3"/>
-      <c r="G71" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="F71" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G71" s="7"/>
       <c r="H71" s="8"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A72" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
@@ -2361,13 +2370,15 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
       <c r="G73" s="7" t="s">
@@ -2376,8 +2387,8 @@
       <c r="H73" s="8"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>113</v>
+      <c r="A74" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>55</v>
@@ -2395,7 +2406,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>55</v>
@@ -2403,38 +2414,44 @@
       <c r="C75" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
+      <c r="D75" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F75" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G75" s="7"/>
+      <c r="G75" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="H75" s="8"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
-      <c r="E76" s="3"/>
+      <c r="E76" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F76" s="3"/>
       <c r="G76" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H76" s="8"/>
+      <c r="H76" s="8" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
@@ -2444,72 +2461,56 @@
       <c r="H77" s="8"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
-        <v>63</v>
+      <c r="A78" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C78" s="3"/>
-      <c r="D78" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D78" s="3"/>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
-      <c r="G78" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="G78" s="7"/>
       <c r="H78" s="8"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F79" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A79" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
       <c r="G79" s="7" t="s">
         <v>55</v>
       </c>
       <c r="H79" s="8"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="s">
-        <v>69</v>
+      <c r="A80" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
-      <c r="E80" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="E80" s="3"/>
       <c r="F80" s="3"/>
       <c r="G80" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H80" s="8" t="s">
-        <v>159</v>
-      </c>
+      <c r="H80" s="8"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
+      <c r="D81" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
       <c r="G81" s="7" t="s">
@@ -2519,27 +2520,35 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B82" s="3"/>
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
-      <c r="G82" s="7"/>
+      <c r="G82" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="H82" s="8"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
+        <v>108</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E83" s="3"/>
-      <c r="F83" s="3"/>
+      <c r="F83" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="G83" s="7" t="s">
         <v>55</v>
       </c>
@@ -2547,37 +2556,39 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B84" s="3"/>
-      <c r="C84" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
-      <c r="G84" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="G84" s="7"/>
       <c r="H84" s="8"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B85" s="3"/>
-      <c r="C85" s="3"/>
-      <c r="D85" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D85" s="3"/>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
-      <c r="G85" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="G85" s="7"/>
       <c r="H85" s="8"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>31</v>
+      <c r="A86" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
@@ -2590,76 +2601,74 @@
       <c r="H86" s="8"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>111</v>
+      <c r="A87" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C87" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
       <c r="E87" s="3"/>
-      <c r="F87" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="F87" s="3"/>
       <c r="G87" s="7" t="s">
         <v>55</v>
       </c>
       <c r="H87" s="8"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>32</v>
+      <c r="A88" s="14" t="s">
+        <v>119</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C88" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C88" s="3"/>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
       <c r="G88" s="7"/>
-      <c r="H88" s="8"/>
+      <c r="H88" s="8" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>33</v>
+      <c r="A89" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C89" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C89" s="3"/>
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
-      <c r="G89" s="7"/>
-      <c r="H89" s="8"/>
+      <c r="G89" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H89" s="8" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B90" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C90" s="3"/>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
-      <c r="G90" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H90" s="8"/>
+      <c r="G90" s="7"/>
+      <c r="H90" s="9" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>98</v>
+        <v>166</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>55</v>
@@ -2668,80 +2677,74 @@
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
       <c r="F91" s="3"/>
-      <c r="G91" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H91" s="8"/>
+      <c r="G91" s="7"/>
+      <c r="H91" s="9" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="14" t="s">
-        <v>122</v>
+      <c r="A92" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C92" s="3"/>
+      <c r="C92" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
       <c r="F92" s="3"/>
-      <c r="G92" s="7"/>
-      <c r="H92" s="8" t="s">
-        <v>123</v>
-      </c>
+      <c r="G92" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H92" s="8"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A93" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B93" s="3"/>
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
-      <c r="G93" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H93" s="8" t="s">
-        <v>150</v>
-      </c>
+      <c r="G93" s="7"/>
+      <c r="H93" s="8"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A94" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B94" s="3"/>
       <c r="C94" s="3"/>
-      <c r="D94" s="3"/>
+      <c r="D94" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E94" s="3"/>
       <c r="F94" s="3"/>
-      <c r="G94" s="7"/>
-      <c r="H94" s="9" t="s">
-        <v>79</v>
-      </c>
+      <c r="G94" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H94" s="8"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A95" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B95" s="3"/>
       <c r="C95" s="3"/>
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
       <c r="F95" s="3"/>
-      <c r="G95" s="7"/>
-      <c r="H95" s="9" t="s">
-        <v>171</v>
-      </c>
+      <c r="G95" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H95" s="8"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>85</v>
+        <v>36</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>55</v>
@@ -2759,49 +2762,51 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
       <c r="D97" s="3"/>
       <c r="E97" s="3"/>
       <c r="F97" s="3"/>
-      <c r="G97" s="7"/>
+      <c r="G97" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="H97" s="8"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B98" s="3"/>
+      <c r="A98" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C98" s="3"/>
-      <c r="D98" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D98" s="3"/>
       <c r="E98" s="3"/>
       <c r="F98" s="3"/>
-      <c r="G98" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H98" s="8"/>
+      <c r="G98" s="7"/>
+      <c r="H98" s="8" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>35</v>
+        <v>158</v>
       </c>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
-      <c r="G99" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H99" s="8"/>
+      <c r="G99" s="7"/>
+      <c r="H99" s="8" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>55</v>
@@ -2812,17 +2817,19 @@
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
-      <c r="G100" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="G100" s="7"/>
       <c r="H100" s="8"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B101" s="3"/>
-      <c r="C101" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
       <c r="F101" s="3"/>
@@ -2832,63 +2839,71 @@
       <c r="H101" s="8"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A102" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B102" s="3"/>
       <c r="C102" s="3"/>
-      <c r="D102" s="3"/>
+      <c r="D102" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E102" s="3"/>
       <c r="F102" s="3"/>
-      <c r="G102" s="7"/>
+      <c r="G102" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="H102" s="8" t="s">
-        <v>125</v>
+        <v>172</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>161</v>
+      <c r="A103" s="4" t="s">
+        <v>175</v>
       </c>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
-      <c r="D103" s="3"/>
+      <c r="D103" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E103" s="3"/>
       <c r="F103" s="3"/>
-      <c r="G103" s="7"/>
+      <c r="G103" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="H103" s="8" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
-        <v>38</v>
+      <c r="A104" s="4" t="s">
+        <v>170</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C104" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D104" s="3"/>
+      <c r="C104" s="3"/>
+      <c r="D104" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
-      <c r="G104" s="7"/>
-      <c r="H104" s="8"/>
+      <c r="G104" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H104" s="8" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B105" s="3"/>
+      <c r="C105" s="3"/>
       <c r="D105" s="3"/>
-      <c r="E105" s="3"/>
+      <c r="E105" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F105" s="3"/>
       <c r="G105" s="7" t="s">
         <v>55</v>
@@ -2897,14 +2912,12 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
       <c r="D106" s="3"/>
-      <c r="E106" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="E106" s="3"/>
       <c r="F106" s="3"/>
       <c r="G106" s="7" t="s">
         <v>55</v>
@@ -2912,11 +2925,15 @@
       <c r="H106" s="8"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B107" s="3"/>
-      <c r="C107" s="3"/>
+      <c r="A107" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D107" s="3"/>
       <c r="E107" s="3"/>
       <c r="F107" s="3"/>
@@ -2926,15 +2943,11 @@
       <c r="H107" s="8"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A108" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A108" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B108" s="3"/>
+      <c r="C108" s="3"/>
       <c r="D108" s="3"/>
       <c r="E108" s="3"/>
       <c r="F108" s="3"/>
@@ -2944,58 +2957,60 @@
       <c r="H108" s="8"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A109" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="B109" s="3"/>
-      <c r="C109" s="3"/>
+      <c r="A109" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D109" s="3"/>
       <c r="E109" s="3"/>
       <c r="F109" s="3"/>
       <c r="G109" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H109" s="8"/>
+      <c r="H109" s="10" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A110" s="4" t="s">
-        <v>74</v>
+      <c r="A110" s="14" t="s">
+        <v>89</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C110" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C110" s="3"/>
       <c r="D110" s="3"/>
       <c r="E110" s="3"/>
       <c r="F110" s="3"/>
-      <c r="G110" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="G110" s="7"/>
       <c r="H110" s="10" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" s="14" t="s">
-        <v>92</v>
+      <c r="A111" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C111" s="3"/>
+      <c r="C111" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D111" s="3"/>
       <c r="E111" s="3"/>
       <c r="F111" s="3"/>
       <c r="G111" s="7"/>
-      <c r="H111" s="10" t="s">
-        <v>93</v>
-      </c>
+      <c r="H111" s="8"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>55</v>
@@ -3006,19 +3021,17 @@
       <c r="D112" s="3"/>
       <c r="E112" s="3"/>
       <c r="F112" s="3"/>
-      <c r="G112" s="7"/>
+      <c r="G112" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="H112" s="8"/>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B113" s="3"/>
+      <c r="C113" s="3"/>
       <c r="D113" s="3"/>
       <c r="E113" s="3"/>
       <c r="F113" s="3"/>
@@ -3029,7 +3042,7 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
@@ -3043,49 +3056,55 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B115" s="3"/>
-      <c r="C115" s="3"/>
+        <v>46</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D115" s="3"/>
-      <c r="E115" s="3"/>
-      <c r="F115" s="3"/>
+      <c r="E115" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F115" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="G115" s="7" t="s">
         <v>55</v>
       </c>
       <c r="H115" s="8"/>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C116" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A116" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B116" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C116" s="11"/>
       <c r="D116" s="3"/>
-      <c r="E116" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F116" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="E116" s="3"/>
+      <c r="F116" s="3"/>
       <c r="G116" s="7" t="s">
         <v>55</v>
       </c>
       <c r="H116" s="8"/>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A117" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B117" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C117" s="11"/>
-      <c r="D117" s="3"/>
+      <c r="A117" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E117" s="3"/>
       <c r="F117" s="3"/>
       <c r="G117" s="7" t="s">
@@ -3095,17 +3114,11 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B118" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C118" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D118" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="B118" s="3"/>
+      <c r="C118" s="3"/>
+      <c r="D118" s="3"/>
       <c r="E118" s="3"/>
       <c r="F118" s="3"/>
       <c r="G118" s="7" t="s">
@@ -3115,37 +3128,43 @@
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B119" s="3"/>
+        <v>168</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C119" s="3"/>
       <c r="D119" s="3"/>
       <c r="E119" s="3"/>
       <c r="F119" s="3"/>
-      <c r="G119" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H119" s="8"/>
+      <c r="G119" s="7"/>
+      <c r="H119" s="8" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
-        <v>172</v>
+      <c r="A120" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C120" s="3"/>
+      <c r="C120" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D120" s="3"/>
       <c r="E120" s="3"/>
       <c r="F120" s="3"/>
-      <c r="G120" s="7"/>
+      <c r="G120" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="H120" s="8" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A121" s="4" t="s">
-        <v>73</v>
+      <c r="A121" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>55</v>
@@ -3153,19 +3172,23 @@
       <c r="C121" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D121" s="3"/>
-      <c r="E121" s="3"/>
+      <c r="D121" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F121" s="3"/>
       <c r="G121" s="7" t="s">
         <v>55</v>
       </c>
       <c r="H121" s="8" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>55</v>
@@ -3176,20 +3199,16 @@
       <c r="D122" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E122" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="E122" s="3"/>
       <c r="F122" s="3"/>
       <c r="G122" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H122" s="8" t="s">
-        <v>152</v>
-      </c>
+      <c r="H122" s="8"/>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>55</v>
@@ -3197,9 +3216,7 @@
       <c r="C123" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D123" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D123" s="3"/>
       <c r="E123" s="3"/>
       <c r="F123" s="3"/>
       <c r="G123" s="7" t="s">
@@ -3209,14 +3226,10 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B124" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C124" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="B124" s="3"/>
+      <c r="C124" s="3"/>
       <c r="D124" s="3"/>
       <c r="E124" s="3"/>
       <c r="F124" s="3"/>
@@ -3226,50 +3239,52 @@
       <c r="H124" s="8"/>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A125" s="1" t="s">
-        <v>116</v>
+      <c r="A125" s="12" t="s">
+        <v>128</v>
       </c>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
       <c r="D125" s="3"/>
       <c r="E125" s="3"/>
       <c r="F125" s="3"/>
-      <c r="G125" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="G125" s="7"/>
       <c r="H125" s="8"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A126" s="12" t="s">
-        <v>131</v>
+      <c r="A126" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
       <c r="D126" s="3"/>
-      <c r="E126" s="3"/>
+      <c r="E126" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F126" s="3"/>
-      <c r="G126" s="7"/>
+      <c r="G126" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="H126" s="8"/>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A127" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B127" s="3"/>
-      <c r="C127" s="3"/>
+      <c r="A127" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D127" s="3"/>
-      <c r="E127" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="E127" s="3"/>
       <c r="F127" s="3"/>
-      <c r="G127" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="G127" s="7"/>
       <c r="H127" s="8"/>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A128" s="1" t="s">
-        <v>52</v>
+      <c r="A128" s="14" t="s">
+        <v>53</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>55</v>
@@ -3284,61 +3299,45 @@
       <c r="H128" s="8"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A129" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B129" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C129" s="3" t="s">
+      <c r="A129" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B129" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C129" s="11" t="s">
         <v>55</v>
       </c>
       <c r="D129" s="3"/>
       <c r="E129" s="3"/>
-      <c r="F129" s="3"/>
-      <c r="G129" s="7"/>
+      <c r="F129" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G129" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="H129" s="8"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A130" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B130" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C130" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D130" s="3"/>
-      <c r="E130" s="3"/>
-      <c r="F130" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G130" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H130" s="8"/>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A131" s="14" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A132" s="14" t="s">
-        <v>134</v>
+      <c r="A132" s="12" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A133" s="12" t="s">
+      <c r="A133" s="13" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A134" s="13" t="s">
-        <v>133</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:H130" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H129" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="G1" r:id="rId1" display="https://github.com/microsoft/winget-pkgs" xr:uid="{2C434A13-8B1C-492F-95C8-B89737A54984}"/>
-    <hyperlink ref="A47" r:id="rId2" xr:uid="{5AAD9A6E-C562-4737-9662-CEC2B195962E}"/>
+    <hyperlink ref="A44" r:id="rId2" xr:uid="{5AAD9A6E-C562-4737-9662-CEC2B195962E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
do not install eclipse anymore
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\markus\projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3BD939A-AE23-45F4-8BD2-752A2395683F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD340179-C6E2-4CDF-98C1-A4E824D6B3F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="180">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -1100,8 +1100,8 @@
   <dimension ref="A1:H133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H107" sqref="H107"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,13 +1520,9 @@
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="B24" s="3"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="7"/>

</xml_diff>

<commit_message>
remove setpoint from choco
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\markus\projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD340179-C6E2-4CDF-98C1-A4E824D6B3F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC441FA-F045-4E93-BF05-0AE4E311D0AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41970" yWindow="540" windowWidth="11910" windowHeight="19425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="180">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -1100,8 +1100,8 @@
   <dimension ref="A1:H133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2672,9 +2672,7 @@
       <c r="A90" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B90" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="B90" s="3"/>
       <c r="C90" s="3"/>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>

</xml_diff>

<commit_message>
docs: update winget availability
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\markus\projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC441FA-F045-4E93-BF05-0AE4E311D0AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E9F215-C448-4FB2-9423-B4A85A8BCED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41970" yWindow="540" windowWidth="11910" windowHeight="19425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="181">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -588,6 +588,9 @@
   </si>
   <si>
     <t>App wurde eingestellt</t>
+  </si>
+  <si>
+    <t>x (sweethome3d)</t>
   </si>
 </sst>
 </file>
@@ -714,34 +717,24 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="2" applyBorder="1"/>
@@ -1100,8 +1093,8 @@
   <dimension ref="A1:H133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B90" sqref="B90"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,26 +1104,26 @@
     <col min="4" max="4" width="6.5703125" customWidth="1"/>
     <col min="5" max="6" width="7.7109375" customWidth="1"/>
     <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="66.42578125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="66.42578125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>159</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -1141,7 +1134,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1159,10 +1152,10 @@
       <c r="F2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" s="8"/>
+      <c r="G2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1178,10 +1171,10 @@
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="7"/>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1199,10 +1192,10 @@
       <c r="F4" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" s="8"/>
+      <c r="G4" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1213,10 +1206,10 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" s="8"/>
+      <c r="G5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1229,10 +1222,10 @@
         <v>55</v>
       </c>
       <c r="F6" s="3"/>
-      <c r="G6" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" s="8"/>
+      <c r="G6" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1245,8 +1238,8 @@
         <v>55</v>
       </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="8"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1259,11 +1252,11 @@
         <v>55</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="8"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1277,13 +1270,13 @@
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H9" s="8"/>
+      <c r="G9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="10" t="s">
         <v>100</v>
       </c>
       <c r="B10" s="3"/>
@@ -1293,10 +1286,10 @@
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H10" s="8"/>
+      <c r="G10" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1307,11 +1300,11 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="8"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="10" t="s">
         <v>114</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1323,13 +1316,13 @@
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="8" t="s">
+      <c r="G12" s="6"/>
+      <c r="H12" s="7" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="1" t="s">
         <v>124</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1341,13 +1334,13 @@
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="8" t="s">
+      <c r="G13" s="6"/>
+      <c r="H13" s="7" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="1" t="s">
         <v>125</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1361,8 +1354,8 @@
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="8" t="s">
+      <c r="G14" s="6"/>
+      <c r="H14" s="7" t="s">
         <v>177</v>
       </c>
     </row>
@@ -1381,10 +1374,10 @@
         <v>55</v>
       </c>
       <c r="F15" s="3"/>
-      <c r="G15" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H15" s="8" t="s">
+      <c r="G15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="7" t="s">
         <v>154</v>
       </c>
     </row>
@@ -1399,8 +1392,8 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="8" t="s">
+      <c r="G16" s="6"/>
+      <c r="H16" s="7" t="s">
         <v>140</v>
       </c>
     </row>
@@ -1413,8 +1406,8 @@
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="8"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -1425,10 +1418,10 @@
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H18" s="8"/>
+      <c r="G18" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="7"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -1441,10 +1434,10 @@
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H19" s="8"/>
+      <c r="G19" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="7"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -1459,10 +1452,10 @@
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H20" s="8"/>
+      <c r="G20" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20" s="7"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -1475,13 +1468,13 @@
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H21" s="8"/>
+      <c r="G21" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H21" s="7"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="1" t="s">
         <v>175</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1493,15 +1486,15 @@
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H22" s="8" t="s">
+      <c r="G22" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H22" s="7" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -1513,8 +1506,8 @@
         <v>55</v>
       </c>
       <c r="F23" s="3"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="8"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="7"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -1525,42 +1518,42 @@
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="8"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="7"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B25" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="11" t="s">
+      <c r="B25" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H25" s="8"/>
+      <c r="G25" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H25" s="7"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B26" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="11"/>
+      <c r="B26" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H26" s="8" t="s">
+      <c r="G26" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H26" s="7" t="s">
         <v>147</v>
       </c>
     </row>
@@ -1579,10 +1572,10 @@
       <c r="F27" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G27" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H27" s="8"/>
+      <c r="G27" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H27" s="7"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
@@ -1599,13 +1592,13 @@
       <c r="F28" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G28" s="7"/>
-      <c r="H28" s="8" t="s">
+      <c r="G28" s="6"/>
+      <c r="H28" s="7" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="10" t="s">
         <v>116</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -1617,8 +1610,8 @@
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="8" t="s">
+      <c r="G29" s="6"/>
+      <c r="H29" s="7" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1637,8 +1630,8 @@
         <v>55</v>
       </c>
       <c r="F30" s="3"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="8"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="7"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
@@ -1657,13 +1650,13 @@
         <v>55</v>
       </c>
       <c r="F31" s="3"/>
-      <c r="G31" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H31" s="8"/>
+      <c r="G31" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H31" s="7"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B32" s="3"/>
@@ -1671,15 +1664,15 @@
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H32" s="8" t="s">
+      <c r="G32" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H32" s="7" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="10" t="s">
         <v>56</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -1689,13 +1682,13 @@
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="8" t="s">
+      <c r="G33" s="6"/>
+      <c r="H33" s="7" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="10" t="s">
         <v>103</v>
       </c>
       <c r="B34" s="3"/>
@@ -1705,15 +1698,15 @@
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
-      <c r="G34" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H34" s="8" t="s">
+      <c r="G34" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H34" s="7" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -1727,10 +1720,10 @@
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
-      <c r="G35" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H35" s="8"/>
+      <c r="G35" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
@@ -1741,13 +1734,13 @@
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
-      <c r="G36" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H36" s="8"/>
+      <c r="G36" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H36" s="7"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="9" t="s">
         <v>87</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -1759,10 +1752,10 @@
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
-      <c r="G37" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H37" s="15" t="s">
+      <c r="G37" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H37" s="11" t="s">
         <v>133</v>
       </c>
     </row>
@@ -1783,10 +1776,10 @@
         <v>55</v>
       </c>
       <c r="F38" s="3"/>
-      <c r="G38" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H38" s="8"/>
+      <c r="G38" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H38" s="7"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
@@ -1801,10 +1794,10 @@
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
-      <c r="G39" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H39" s="8"/>
+      <c r="G39" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H39" s="7"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
@@ -1817,8 +1810,8 @@
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="8"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="7"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
@@ -1833,15 +1826,15 @@
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
-      <c r="G41" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H41" s="8" t="s">
+      <c r="G41" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H41" s="7" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="14" t="s">
+      <c r="A42" s="10" t="s">
         <v>84</v>
       </c>
       <c r="B42" s="3"/>
@@ -1849,8 +1842,8 @@
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="8" t="s">
+      <c r="G42" s="6"/>
+      <c r="H42" s="7" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1865,13 +1858,13 @@
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
-      <c r="G43" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H43" s="8"/>
+      <c r="G43" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H43" s="7"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="16" t="s">
+      <c r="A44" s="12" t="s">
         <v>150</v>
       </c>
       <c r="B44" s="3"/>
@@ -1883,10 +1876,10 @@
       <c r="F44" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G44" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H44" s="8" t="s">
+      <c r="G44" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H44" s="7" t="s">
         <v>153</v>
       </c>
     </row>
@@ -1905,10 +1898,10 @@
         <v>55</v>
       </c>
       <c r="F45" s="3"/>
-      <c r="G45" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H45" s="8" t="s">
+      <c r="G45" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H45" s="7" t="s">
         <v>154</v>
       </c>
     </row>
@@ -1927,13 +1920,13 @@
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
-      <c r="G46" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H46" s="8"/>
+      <c r="G46" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H46" s="7"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
+      <c r="A47" s="9" t="s">
         <v>96</v>
       </c>
       <c r="B47" s="3" t="s">
@@ -1943,15 +1936,15 @@
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
-      <c r="G47" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H47" s="15" t="s">
+      <c r="G47" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H47" s="11" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B48" s="3" t="s">
@@ -1961,10 +1954,10 @@
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
-      <c r="G48" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H48" s="8" t="s">
+      <c r="G48" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H48" s="7" t="s">
         <v>162</v>
       </c>
     </row>
@@ -1979,10 +1972,10 @@
         <v>55</v>
       </c>
       <c r="F49" s="3"/>
-      <c r="G49" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H49" s="8"/>
+      <c r="G49" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H49" s="7"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
@@ -1997,8 +1990,8 @@
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
-      <c r="G50" s="7"/>
-      <c r="H50" s="8"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="7"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
@@ -2013,13 +2006,13 @@
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
-      <c r="G51" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H51" s="8"/>
+      <c r="G51" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H51" s="7"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="14" t="s">
+      <c r="A52" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B52" s="3"/>
@@ -2029,8 +2022,10 @@
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="8"/>
+      <c r="G52" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H52" s="7"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
@@ -2047,15 +2042,15 @@
         <v>55</v>
       </c>
       <c r="F53" s="3"/>
-      <c r="G53" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H53" s="8" t="s">
+      <c r="G53" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H53" s="7" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B54" s="3" t="s">
@@ -2071,13 +2066,13 @@
       <c r="F54" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G54" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H54" s="8"/>
+      <c r="G54" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H54" s="7"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B55" s="3" t="s">
@@ -2093,10 +2088,10 @@
       <c r="F55" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G55" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H55" s="8"/>
+      <c r="G55" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H55" s="7"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
@@ -2115,13 +2110,13 @@
       <c r="F56" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G56" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H56" s="8"/>
+      <c r="G56" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H56" s="7"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B57" s="3" t="s">
@@ -2133,15 +2128,15 @@
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
-      <c r="G57" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H57" s="8" t="s">
+      <c r="G57" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H57" s="7" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="14" t="s">
+      <c r="A58" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B58" s="3"/>
@@ -2149,8 +2144,8 @@
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
-      <c r="G58" s="7"/>
-      <c r="H58" s="8"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="7"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
@@ -2165,8 +2160,8 @@
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
-      <c r="G59" s="7"/>
-      <c r="H59" s="8" t="s">
+      <c r="G59" s="6"/>
+      <c r="H59" s="7" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2179,15 +2174,15 @@
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
-      <c r="G60" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H60" s="8" t="s">
+      <c r="G60" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H60" s="7" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B61" s="3" t="s">
@@ -2201,17 +2196,19 @@
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
-      <c r="G61" s="7"/>
-      <c r="H61" s="8"/>
+      <c r="G61" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H61" s="7"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B62" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C62" s="11" t="s">
+      <c r="B62" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C62" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D62" s="3"/>
@@ -2219,10 +2216,10 @@
       <c r="F62" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G62" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H62" s="8"/>
+      <c r="G62" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H62" s="7"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
@@ -2237,10 +2234,10 @@
       </c>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
-      <c r="G63" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H63" s="8"/>
+      <c r="G63" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H63" s="7"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
@@ -2251,10 +2248,10 @@
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
-      <c r="G64" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H64" s="8" t="s">
+      <c r="G64" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H64" s="7" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2269,10 +2266,10 @@
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
-      <c r="G65" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H65" s="8" t="s">
+      <c r="G65" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H65" s="7" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2285,8 +2282,8 @@
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
-      <c r="G66" s="7"/>
-      <c r="H66" s="8"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="7"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
@@ -2297,10 +2294,10 @@
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
-      <c r="G67" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H67" s="8"/>
+      <c r="G67" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H67" s="7"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
@@ -2315,10 +2312,10 @@
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
-      <c r="G68" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H68" s="8"/>
+      <c r="G68" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H68" s="7"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
@@ -2331,10 +2328,10 @@
       </c>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
-      <c r="G69" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H69" s="8"/>
+      <c r="G69" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H69" s="7"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
@@ -2349,13 +2346,13 @@
       </c>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
-      <c r="G70" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H70" s="8"/>
+      <c r="G70" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H70" s="7"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
+      <c r="A71" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B71" s="3" t="s">
@@ -2369,11 +2366,13 @@
       <c r="F71" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G71" s="7"/>
-      <c r="H71" s="8"/>
+      <c r="G71" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H71" s="7"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
+      <c r="A72" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B72" s="3"/>
@@ -2381,10 +2380,10 @@
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
-      <c r="G72" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H72" s="8"/>
+      <c r="G72" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H72" s="7"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
@@ -2399,13 +2398,13 @@
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
-      <c r="G73" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H73" s="8"/>
+      <c r="G73" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H73" s="7"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
+      <c r="A74" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B74" s="3" t="s">
@@ -2417,13 +2416,13 @@
       </c>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
-      <c r="G74" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H74" s="8"/>
+      <c r="G74" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H74" s="7"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
+      <c r="A75" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B75" s="3" t="s">
@@ -2441,13 +2440,13 @@
       <c r="F75" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G75" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H75" s="8"/>
+      <c r="G75" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H75" s="7"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
+      <c r="A76" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B76" s="3"/>
@@ -2457,10 +2456,10 @@
         <v>55</v>
       </c>
       <c r="F76" s="3"/>
-      <c r="G76" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H76" s="8" t="s">
+      <c r="G76" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H76" s="7" t="s">
         <v>155</v>
       </c>
     </row>
@@ -2473,10 +2472,10 @@
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
-      <c r="G77" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H77" s="8"/>
+      <c r="G77" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H77" s="7"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
@@ -2489,8 +2488,8 @@
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
-      <c r="G78" s="7"/>
-      <c r="H78" s="8"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="7"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
@@ -2501,10 +2500,10 @@
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
-      <c r="G79" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H79" s="8"/>
+      <c r="G79" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H79" s="7"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
@@ -2515,10 +2514,10 @@
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
-      <c r="G80" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H80" s="8"/>
+      <c r="G80" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H80" s="7"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
@@ -2531,10 +2530,10 @@
       </c>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
-      <c r="G81" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H81" s="8"/>
+      <c r="G81" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H81" s="7"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
@@ -2545,10 +2544,10 @@
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
-      <c r="G82" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H82" s="8"/>
+      <c r="G82" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H82" s="7"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
@@ -2567,10 +2566,10 @@
       <c r="F83" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G83" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H83" s="8"/>
+      <c r="G83" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H83" s="7"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
@@ -2585,8 +2584,10 @@
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
-      <c r="G84" s="7"/>
-      <c r="H84" s="8"/>
+      <c r="G84" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H84" s="7"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
@@ -2601,11 +2602,13 @@
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
-      <c r="G85" s="7"/>
-      <c r="H85" s="8"/>
+      <c r="G85" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H85" s="7"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="4" t="s">
+      <c r="A86" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B86" s="3"/>
@@ -2613,13 +2616,13 @@
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
-      <c r="G86" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H86" s="8"/>
+      <c r="G86" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H86" s="7"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="4" t="s">
+      <c r="A87" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B87" s="3" t="s">
@@ -2629,13 +2632,13 @@
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
       <c r="F87" s="3"/>
-      <c r="G87" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H87" s="8"/>
+      <c r="G87" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H87" s="7"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="14" t="s">
+      <c r="A88" s="10" t="s">
         <v>118</v>
       </c>
       <c r="B88" s="3" t="s">
@@ -2645,13 +2648,13 @@
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
-      <c r="G88" s="7"/>
-      <c r="H88" s="8" t="s">
+      <c r="G88" s="6"/>
+      <c r="H88" s="7" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="4" t="s">
+      <c r="A89" s="1" t="s">
         <v>145</v>
       </c>
       <c r="B89" s="3" t="s">
@@ -2661,15 +2664,15 @@
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
-      <c r="G89" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H89" s="8" t="s">
+      <c r="G89" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H89" s="7" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="4" t="s">
+      <c r="A90" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B90" s="3"/>
@@ -2677,13 +2680,15 @@
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
-      <c r="G90" s="7"/>
-      <c r="H90" s="9" t="s">
+      <c r="G90" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H90" s="7" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="4" t="s">
+      <c r="A91" s="1" t="s">
         <v>165</v>
       </c>
       <c r="B91" s="3" t="s">
@@ -2693,8 +2698,10 @@
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
       <c r="F91" s="3"/>
-      <c r="G91" s="7"/>
-      <c r="H91" s="9" t="s">
+      <c r="G91" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H91" s="7" t="s">
         <v>166</v>
       </c>
     </row>
@@ -2711,10 +2718,10 @@
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
       <c r="F92" s="3"/>
-      <c r="G92" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H92" s="8"/>
+      <c r="G92" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H92" s="7"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
@@ -2725,8 +2732,8 @@
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
-      <c r="G93" s="7"/>
-      <c r="H93" s="8"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="7"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
@@ -2739,10 +2746,10 @@
       </c>
       <c r="E94" s="3"/>
       <c r="F94" s="3"/>
-      <c r="G94" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H94" s="8"/>
+      <c r="G94" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H94" s="7"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
@@ -2753,10 +2760,10 @@
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
       <c r="F95" s="3"/>
-      <c r="G95" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H95" s="8"/>
+      <c r="G95" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H95" s="7"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
@@ -2771,10 +2778,10 @@
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
       <c r="F96" s="3"/>
-      <c r="G96" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H96" s="8"/>
+      <c r="G96" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H96" s="7"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
@@ -2785,13 +2792,13 @@
       <c r="D97" s="3"/>
       <c r="E97" s="3"/>
       <c r="F97" s="3"/>
-      <c r="G97" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H97" s="8"/>
+      <c r="G97" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H97" s="7"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98" s="14" t="s">
+      <c r="A98" s="10" t="s">
         <v>120</v>
       </c>
       <c r="B98" s="3" t="s">
@@ -2801,8 +2808,10 @@
       <c r="D98" s="3"/>
       <c r="E98" s="3"/>
       <c r="F98" s="3"/>
-      <c r="G98" s="7"/>
-      <c r="H98" s="8" t="s">
+      <c r="G98" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H98" s="7" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2815,8 +2824,10 @@
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
-      <c r="G99" s="7"/>
-      <c r="H99" s="8" t="s">
+      <c r="G99" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="H99" s="7" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2833,8 +2844,10 @@
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
-      <c r="G100" s="7"/>
-      <c r="H100" s="8"/>
+      <c r="G100" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H100" s="7"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
@@ -2849,13 +2862,13 @@
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
       <c r="F101" s="3"/>
-      <c r="G101" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H101" s="8"/>
+      <c r="G101" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H101" s="7"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" s="4" t="s">
+      <c r="A102" s="1" t="s">
         <v>173</v>
       </c>
       <c r="B102" s="3"/>
@@ -2865,15 +2878,15 @@
       </c>
       <c r="E102" s="3"/>
       <c r="F102" s="3"/>
-      <c r="G102" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H102" s="8" t="s">
+      <c r="G102" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H102" s="7" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A103" s="4" t="s">
+      <c r="A103" s="1" t="s">
         <v>174</v>
       </c>
       <c r="B103" s="3"/>
@@ -2883,15 +2896,15 @@
       </c>
       <c r="E103" s="3"/>
       <c r="F103" s="3"/>
-      <c r="G103" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H103" s="8" t="s">
+      <c r="G103" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H103" s="7" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A104" s="4" t="s">
+      <c r="A104" s="1" t="s">
         <v>169</v>
       </c>
       <c r="B104" s="3" t="s">
@@ -2903,10 +2916,10 @@
       </c>
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
-      <c r="G104" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H104" s="8" t="s">
+      <c r="G104" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H104" s="7" t="s">
         <v>170</v>
       </c>
     </row>
@@ -2921,10 +2934,10 @@
         <v>55</v>
       </c>
       <c r="F105" s="3"/>
-      <c r="G105" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H105" s="8"/>
+      <c r="G105" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H105" s="7"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
@@ -2935,13 +2948,13 @@
       <c r="D106" s="3"/>
       <c r="E106" s="3"/>
       <c r="F106" s="3"/>
-      <c r="G106" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H106" s="8"/>
+      <c r="G106" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H106" s="7"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A107" s="4" t="s">
+      <c r="A107" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B107" s="3"/>
@@ -2949,13 +2962,13 @@
       <c r="D107" s="3"/>
       <c r="E107" s="3"/>
       <c r="F107" s="3"/>
-      <c r="G107" s="7"/>
-      <c r="H107" s="8" t="s">
+      <c r="G107" s="6"/>
+      <c r="H107" s="7" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A108" s="13" t="s">
+      <c r="A108" s="9" t="s">
         <v>128</v>
       </c>
       <c r="B108" s="3"/>
@@ -2963,13 +2976,13 @@
       <c r="D108" s="3"/>
       <c r="E108" s="3"/>
       <c r="F108" s="3"/>
-      <c r="G108" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H108" s="8"/>
+      <c r="G108" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H108" s="7"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A109" s="4" t="s">
+      <c r="A109" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B109" s="3" t="s">
@@ -2981,15 +2994,15 @@
       <c r="D109" s="3"/>
       <c r="E109" s="3"/>
       <c r="F109" s="3"/>
-      <c r="G109" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H109" s="10" t="s">
+      <c r="G109" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H109" s="7" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A110" s="14" t="s">
+      <c r="A110" s="10" t="s">
         <v>88</v>
       </c>
       <c r="B110" s="3" t="s">
@@ -2999,8 +3012,8 @@
       <c r="D110" s="3"/>
       <c r="E110" s="3"/>
       <c r="F110" s="3"/>
-      <c r="G110" s="7"/>
-      <c r="H110" s="10" t="s">
+      <c r="G110" s="6"/>
+      <c r="H110" s="7" t="s">
         <v>89</v>
       </c>
     </row>
@@ -3017,8 +3030,8 @@
       <c r="D111" s="3"/>
       <c r="E111" s="3"/>
       <c r="F111" s="3"/>
-      <c r="G111" s="7"/>
-      <c r="H111" s="8"/>
+      <c r="G111" s="6"/>
+      <c r="H111" s="7"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
@@ -3033,10 +3046,10 @@
       <c r="D112" s="3"/>
       <c r="E112" s="3"/>
       <c r="F112" s="3"/>
-      <c r="G112" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H112" s="8"/>
+      <c r="G112" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H112" s="7"/>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
@@ -3047,10 +3060,10 @@
       <c r="D113" s="3"/>
       <c r="E113" s="3"/>
       <c r="F113" s="3"/>
-      <c r="G113" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H113" s="8"/>
+      <c r="G113" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H113" s="7"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
@@ -3061,10 +3074,10 @@
       <c r="D114" s="3"/>
       <c r="E114" s="3"/>
       <c r="F114" s="3"/>
-      <c r="G114" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H114" s="8"/>
+      <c r="G114" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H114" s="7"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
@@ -3083,26 +3096,26 @@
       <c r="F115" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G115" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H115" s="8"/>
+      <c r="G115" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H115" s="7"/>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A116" s="4" t="s">
+      <c r="A116" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B116" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C116" s="11"/>
+      <c r="B116" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C116" s="3"/>
       <c r="D116" s="3"/>
       <c r="E116" s="3"/>
       <c r="F116" s="3"/>
-      <c r="G116" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H116" s="8"/>
+      <c r="G116" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H116" s="7"/>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
@@ -3119,10 +3132,10 @@
       </c>
       <c r="E117" s="3"/>
       <c r="F117" s="3"/>
-      <c r="G117" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H117" s="8"/>
+      <c r="G117" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H117" s="7"/>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
@@ -3133,10 +3146,10 @@
       <c r="D118" s="3"/>
       <c r="E118" s="3"/>
       <c r="F118" s="3"/>
-      <c r="G118" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H118" s="8"/>
+      <c r="G118" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H118" s="7"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
@@ -3149,13 +3162,13 @@
       <c r="D119" s="3"/>
       <c r="E119" s="3"/>
       <c r="F119" s="3"/>
-      <c r="G119" s="7"/>
-      <c r="H119" s="8" t="s">
+      <c r="G119" s="6"/>
+      <c r="H119" s="7" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A120" s="4" t="s">
+      <c r="A120" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B120" s="3" t="s">
@@ -3167,10 +3180,10 @@
       <c r="D120" s="3"/>
       <c r="E120" s="3"/>
       <c r="F120" s="3"/>
-      <c r="G120" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H120" s="8" t="s">
+      <c r="G120" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H120" s="7" t="s">
         <v>156</v>
       </c>
     </row>
@@ -3191,10 +3204,10 @@
         <v>55</v>
       </c>
       <c r="F121" s="3"/>
-      <c r="G121" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H121" s="8" t="s">
+      <c r="G121" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H121" s="7" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3213,10 +3226,10 @@
       </c>
       <c r="E122" s="3"/>
       <c r="F122" s="3"/>
-      <c r="G122" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H122" s="8"/>
+      <c r="G122" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H122" s="7"/>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
@@ -3231,10 +3244,10 @@
       <c r="D123" s="3"/>
       <c r="E123" s="3"/>
       <c r="F123" s="3"/>
-      <c r="G123" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H123" s="8"/>
+      <c r="G123" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H123" s="7"/>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
@@ -3245,13 +3258,13 @@
       <c r="D124" s="3"/>
       <c r="E124" s="3"/>
       <c r="F124" s="3"/>
-      <c r="G124" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H124" s="8"/>
+      <c r="G124" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H124" s="7"/>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A125" s="12" t="s">
+      <c r="A125" s="8" t="s">
         <v>127</v>
       </c>
       <c r="B125" s="3"/>
@@ -3259,11 +3272,11 @@
       <c r="D125" s="3"/>
       <c r="E125" s="3"/>
       <c r="F125" s="3"/>
-      <c r="G125" s="7"/>
-      <c r="H125" s="8"/>
+      <c r="G125" s="6"/>
+      <c r="H125" s="7"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A126" s="4" t="s">
+      <c r="A126" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B126" s="3"/>
@@ -3273,10 +3286,10 @@
         <v>55</v>
       </c>
       <c r="F126" s="3"/>
-      <c r="G126" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H126" s="8"/>
+      <c r="G126" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H126" s="7"/>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
@@ -3291,11 +3304,11 @@
       <c r="D127" s="3"/>
       <c r="E127" s="3"/>
       <c r="F127" s="3"/>
-      <c r="G127" s="7"/>
-      <c r="H127" s="8"/>
+      <c r="G127" s="6"/>
+      <c r="H127" s="7"/>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A128" s="14" t="s">
+      <c r="A128" s="10" t="s">
         <v>53</v>
       </c>
       <c r="B128" s="3" t="s">
@@ -3307,17 +3320,19 @@
       <c r="D128" s="3"/>
       <c r="E128" s="3"/>
       <c r="F128" s="3"/>
-      <c r="G128" s="7"/>
-      <c r="H128" s="8"/>
+      <c r="G128" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H128" s="7"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B129" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C129" s="11" t="s">
+      <c r="B129" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C129" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D129" s="3"/>
@@ -3325,23 +3340,23 @@
       <c r="F129" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G129" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H129" s="8"/>
+      <c r="G129" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H129" s="7"/>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A131" s="14" t="s">
+      <c r="A131" s="10" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A132" s="12" t="s">
+      <c r="A132" s="8" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A133" s="13" t="s">
+      <c r="A133" s="9" t="s">
         <v>129</v>
       </c>
     </row>

</xml_diff>

<commit_message>
docs: install neovim, rg and fzf in git-bash
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\markus\projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E9F215-C448-4FB2-9423-B4A85A8BCED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CE58EE-A6C0-4670-8DD5-FB7A454B0611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$129</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$130</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="182">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -591,6 +591,9 @@
   </si>
   <si>
     <t>x (sweethome3d)</t>
+  </si>
+  <si>
+    <t>neovim</t>
   </si>
 </sst>
 </file>
@@ -1090,11 +1093,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H133"/>
+  <dimension ref="A1:H134"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1679,7 +1682,9 @@
         <v>55</v>
       </c>
       <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
+      <c r="D33" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="6"/>
@@ -2387,33 +2392,29 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D73" s="3"/>
+        <v>181</v>
+      </c>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
-      <c r="G73" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="G73" s="6"/>
       <c r="H73" s="7"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C74" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D74" s="3"/>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
       <c r="G74" s="6" t="s">
@@ -2423,23 +2424,17 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C75" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C75" s="3"/>
       <c r="D75" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E75" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F75" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
       <c r="G75" s="6" t="s">
         <v>55</v>
       </c>
@@ -2447,67 +2442,77 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B76" s="3"/>
-      <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E76" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F76" s="3"/>
+      <c r="F76" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="G76" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H76" s="7" t="s">
-        <v>155</v>
-      </c>
+      <c r="H76" s="7"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
-      <c r="E77" s="3"/>
+      <c r="E77" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F77" s="3"/>
       <c r="G77" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H77" s="7"/>
+      <c r="H77" s="7" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B78" s="3"/>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
-      <c r="G78" s="6"/>
+      <c r="G78" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="H78" s="7"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B79" s="3"/>
+        <v>95</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
-      <c r="G79" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="G79" s="6"/>
       <c r="H79" s="7"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>29</v>
+        <v>149</v>
       </c>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -2521,13 +2526,11 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
-      <c r="D81" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D81" s="3"/>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
       <c r="G81" s="6" t="s">
@@ -2537,11 +2540,13 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
+      <c r="D82" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
       <c r="G82" s="6" t="s">
@@ -2551,21 +2556,13 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
       <c r="E83" s="3"/>
-      <c r="F83" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="F83" s="3"/>
       <c r="G83" s="6" t="s">
         <v>55</v>
       </c>
@@ -2573,7 +2570,7 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>32</v>
+        <v>107</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>55</v>
@@ -2581,9 +2578,13 @@
       <c r="C84" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D84" s="3"/>
+      <c r="D84" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E84" s="3"/>
-      <c r="F84" s="3"/>
+      <c r="F84" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="G84" s="6" t="s">
         <v>55</v>
       </c>
@@ -2591,7 +2592,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>55</v>
@@ -2609,10 +2610,14 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B86" s="3"/>
-      <c r="C86" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
@@ -2623,11 +2628,9 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
@@ -2638,8 +2641,8 @@
       <c r="H87" s="7"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="10" t="s">
-        <v>118</v>
+      <c r="A88" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>55</v>
@@ -2648,34 +2651,36 @@
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
-      <c r="G88" s="6"/>
-      <c r="H88" s="7" t="s">
-        <v>119</v>
-      </c>
+      <c r="G88" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H88" s="7"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>145</v>
+      <c r="A89" s="10" t="s">
+        <v>118</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C89" s="3"/>
-      <c r="D89" s="3"/>
+      <c r="D89" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
-      <c r="G89" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="G89" s="6"/>
       <c r="H89" s="7" t="s">
-        <v>146</v>
+        <v>119</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B90" s="3"/>
+        <v>145</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C90" s="3"/>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
@@ -2684,16 +2689,14 @@
         <v>55</v>
       </c>
       <c r="H90" s="7" t="s">
-        <v>79</v>
+        <v>146</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B91" s="3"/>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
@@ -2702,62 +2705,66 @@
         <v>55</v>
       </c>
       <c r="H91" s="7" t="s">
-        <v>166</v>
+        <v>79</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>83</v>
+        <v>165</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C92" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C92" s="3"/>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
       <c r="F92" s="3"/>
       <c r="G92" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H92" s="7"/>
+      <c r="H92" s="7" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B93" s="3"/>
-      <c r="C93" s="3"/>
+        <v>83</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
-      <c r="G93" s="6"/>
+      <c r="G93" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="H93" s="7"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
-      <c r="D94" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D94" s="3"/>
       <c r="E94" s="3"/>
       <c r="F94" s="3"/>
-      <c r="G94" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="G94" s="6"/>
       <c r="H94" s="7"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
-      <c r="D95" s="3"/>
+      <c r="D95" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E95" s="3"/>
       <c r="F95" s="3"/>
       <c r="G95" s="6" t="s">
@@ -2767,14 +2774,10 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
       <c r="F96" s="3"/>
@@ -2785,10 +2788,14 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B97" s="3"/>
-      <c r="C97" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D97" s="3"/>
       <c r="E97" s="3"/>
       <c r="F97" s="3"/>
@@ -2798,12 +2805,10 @@
       <c r="H97" s="7"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A98" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B98" s="3"/>
       <c r="C98" s="3"/>
       <c r="D98" s="3"/>
       <c r="E98" s="3"/>
@@ -2811,47 +2816,45 @@
       <c r="G98" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H98" s="7" t="s">
-        <v>121</v>
-      </c>
+      <c r="H98" s="7"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B99" s="3"/>
+      <c r="A99" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C99" s="3"/>
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
       <c r="G99" s="6" t="s">
-        <v>180</v>
+        <v>55</v>
       </c>
       <c r="H99" s="7" t="s">
-        <v>158</v>
+        <v>121</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="B100" s="3"/>
+      <c r="C100" s="3"/>
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
       <c r="G100" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H100" s="7"/>
+        <v>180</v>
+      </c>
+      <c r="H100" s="7" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>55</v>
@@ -2869,25 +2872,25 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B102" s="3"/>
-      <c r="C102" s="3"/>
-      <c r="D102" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D102" s="3"/>
       <c r="E102" s="3"/>
       <c r="F102" s="3"/>
       <c r="G102" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H102" s="7" t="s">
-        <v>171</v>
-      </c>
+      <c r="H102" s="7"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
@@ -2900,16 +2903,14 @@
         <v>55</v>
       </c>
       <c r="H103" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="B104" s="3"/>
       <c r="C104" s="3"/>
       <c r="D104" s="3" t="s">
         <v>55</v>
@@ -2920,33 +2921,39 @@
         <v>55</v>
       </c>
       <c r="H104" s="7" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B105" s="3"/>
+        <v>169</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C105" s="3"/>
-      <c r="D105" s="3"/>
-      <c r="E105" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D105" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E105" s="3"/>
       <c r="F105" s="3"/>
       <c r="G105" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H105" s="7"/>
+      <c r="H105" s="7" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
       <c r="D106" s="3"/>
-      <c r="E106" s="3"/>
+      <c r="E106" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F106" s="3"/>
       <c r="G106" s="6" t="s">
         <v>55</v>
@@ -2955,87 +2962,85 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
       <c r="D107" s="3"/>
       <c r="E107" s="3"/>
       <c r="F107" s="3"/>
-      <c r="G107" s="6"/>
-      <c r="H107" s="7" t="s">
-        <v>179</v>
-      </c>
+      <c r="G107" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H107" s="7"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A108" s="9" t="s">
-        <v>128</v>
+      <c r="A108" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
       <c r="D108" s="3"/>
       <c r="E108" s="3"/>
       <c r="F108" s="3"/>
-      <c r="G108" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H108" s="7"/>
+      <c r="G108" s="6"/>
+      <c r="H108" s="7" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A109" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B109" s="3"/>
+      <c r="C109" s="3"/>
       <c r="D109" s="3"/>
       <c r="E109" s="3"/>
       <c r="F109" s="3"/>
       <c r="G109" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H109" s="7" t="s">
-        <v>75</v>
-      </c>
+      <c r="H109" s="7"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A110" s="10" t="s">
-        <v>88</v>
+      <c r="A110" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C110" s="3"/>
+      <c r="C110" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D110" s="3"/>
       <c r="E110" s="3"/>
       <c r="F110" s="3"/>
-      <c r="G110" s="6"/>
+      <c r="G110" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="H110" s="7" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
-        <v>42</v>
+      <c r="A111" s="10" t="s">
+        <v>88</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C111" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C111" s="3"/>
       <c r="D111" s="3"/>
       <c r="E111" s="3"/>
       <c r="F111" s="3"/>
       <c r="G111" s="6"/>
-      <c r="H111" s="7"/>
+      <c r="H111" s="7" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>55</v>
@@ -3046,17 +3051,19 @@
       <c r="D112" s="3"/>
       <c r="E112" s="3"/>
       <c r="F112" s="3"/>
-      <c r="G112" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="G112" s="6"/>
       <c r="H112" s="7"/>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B113" s="3"/>
-      <c r="C113" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D113" s="3"/>
       <c r="E113" s="3"/>
       <c r="F113" s="3"/>
@@ -3067,7 +3074,7 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
@@ -3081,21 +3088,13 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B115" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B115" s="3"/>
+      <c r="C115" s="3"/>
       <c r="D115" s="3"/>
-      <c r="E115" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F115" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="E115" s="3"/>
+      <c r="F115" s="3"/>
       <c r="G115" s="6" t="s">
         <v>55</v>
       </c>
@@ -3103,15 +3102,21 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>110</v>
+        <v>46</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C116" s="3"/>
+      <c r="C116" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D116" s="3"/>
-      <c r="E116" s="3"/>
-      <c r="F116" s="3"/>
+      <c r="E116" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="G116" s="6" t="s">
         <v>55</v>
       </c>
@@ -3119,17 +3124,13 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>47</v>
+        <v>110</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C117" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D117" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C117" s="3"/>
+      <c r="D117" s="3"/>
       <c r="E117" s="3"/>
       <c r="F117" s="3"/>
       <c r="G117" s="6" t="s">
@@ -3139,11 +3140,17 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B118" s="3"/>
-      <c r="C118" s="3"/>
-      <c r="D118" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E118" s="3"/>
       <c r="F118" s="3"/>
       <c r="G118" s="6" t="s">
@@ -3153,43 +3160,37 @@
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B119" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="B119" s="3"/>
       <c r="C119" s="3"/>
       <c r="D119" s="3"/>
       <c r="E119" s="3"/>
       <c r="F119" s="3"/>
-      <c r="G119" s="6"/>
-      <c r="H119" s="7" t="s">
-        <v>168</v>
-      </c>
+      <c r="G119" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H119" s="7"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>73</v>
+        <v>167</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C120" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C120" s="3"/>
       <c r="D120" s="3"/>
       <c r="E120" s="3"/>
       <c r="F120" s="3"/>
-      <c r="G120" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="G120" s="6"/>
       <c r="H120" s="7" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>55</v>
@@ -3197,23 +3198,19 @@
       <c r="C121" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D121" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E121" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D121" s="3"/>
+      <c r="E121" s="3"/>
       <c r="F121" s="3"/>
       <c r="G121" s="6" t="s">
         <v>55</v>
       </c>
       <c r="H121" s="7" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>55</v>
@@ -3224,16 +3221,20 @@
       <c r="D122" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E122" s="3"/>
+      <c r="E122" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F122" s="3"/>
       <c r="G122" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H122" s="7"/>
+      <c r="H122" s="7" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>55</v>
@@ -3241,7 +3242,9 @@
       <c r="C123" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D123" s="3"/>
+      <c r="D123" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E123" s="3"/>
       <c r="F123" s="3"/>
       <c r="G123" s="6" t="s">
@@ -3251,10 +3254,14 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B124" s="3"/>
-      <c r="C124" s="3"/>
+        <v>51</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D124" s="3"/>
       <c r="E124" s="3"/>
       <c r="F124" s="3"/>
@@ -3264,52 +3271,50 @@
       <c r="H124" s="7"/>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A125" s="8" t="s">
-        <v>127</v>
+      <c r="A125" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
       <c r="D125" s="3"/>
       <c r="E125" s="3"/>
       <c r="F125" s="3"/>
-      <c r="G125" s="6"/>
+      <c r="G125" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="H125" s="7"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
-        <v>66</v>
+      <c r="A126" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
       <c r="D126" s="3"/>
-      <c r="E126" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="E126" s="3"/>
       <c r="F126" s="3"/>
-      <c r="G126" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="G126" s="6"/>
       <c r="H126" s="7"/>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B127" s="3"/>
+      <c r="C127" s="3"/>
+      <c r="D127" s="3"/>
+      <c r="E127" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F127" s="3"/>
+      <c r="G127" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H127" s="7"/>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C127" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D127" s="3"/>
-      <c r="E127" s="3"/>
-      <c r="F127" s="3"/>
-      <c r="G127" s="6"/>
-      <c r="H127" s="7"/>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A128" s="10" t="s">
-        <v>53</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>55</v>
@@ -3320,14 +3325,12 @@
       <c r="D128" s="3"/>
       <c r="E128" s="3"/>
       <c r="F128" s="3"/>
-      <c r="G128" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="G128" s="6"/>
       <c r="H128" s="7"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A129" s="1" t="s">
-        <v>113</v>
+      <c r="A129" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>55</v>
@@ -3337,31 +3340,49 @@
       </c>
       <c r="D129" s="3"/>
       <c r="E129" s="3"/>
-      <c r="F129" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="F129" s="3"/>
       <c r="G129" s="6" t="s">
         <v>55</v>
       </c>
       <c r="H129" s="7"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A131" s="10" t="s">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D130" s="3"/>
+      <c r="E130" s="3"/>
+      <c r="F130" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G130" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H130" s="7"/>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A132" s="10" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A132" s="8" t="s">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A133" s="8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A133" s="9" t="s">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A134" s="9" t="s">
         <v>129</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H129" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H130" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="G1" r:id="rId1" display="https://github.com/microsoft/winget-pkgs" xr:uid="{2C434A13-8B1C-492F-95C8-B89737A54984}"/>
     <hyperlink ref="A44" r:id="rId2" xr:uid="{5AAD9A6E-C562-4737-9662-CEC2B195962E}"/>

</xml_diff>

<commit_message>
feat: get ready to evaluate winget
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\markus\projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CC880A-57D3-4ACC-B4FA-C739F5E0C510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F16F302-E0D8-43BD-9716-7931ADCAD6B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38295" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,48 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$130</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$131</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Markus Meier</author>
+  </authors>
+  <commentList>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{A5E10DA7-0DFA-42A4-A029-046B2EBA0170}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Markus Meier:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+https://winget.run/</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="186">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -598,12 +632,21 @@
   <si>
     <t>Version in chocolatey (1.15) too old (current: 1.16)</t>
   </si>
+  <si>
+    <t>x (ctags)</t>
+  </si>
+  <si>
+    <t>x (shellexview)</t>
+  </si>
+  <si>
+    <t>powershell-core</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -655,6 +698,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -723,7 +779,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -749,9 +805,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
@@ -1098,12 +1151,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H134"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C133" sqref="C133"/>
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G84" sqref="G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,13 +1387,9 @@
       <c r="A13" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="6"/>
@@ -1352,15 +1401,9 @@
       <c r="A14" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="6"/>
@@ -1570,7 +1613,7 @@
       <c r="A27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -1601,7 +1644,9 @@
       <c r="F28" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G28" s="6"/>
+      <c r="G28" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="H28" s="7" t="s">
         <v>152</v>
       </c>
@@ -1619,7 +1664,9 @@
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="6"/>
+      <c r="G29" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="H29" s="7" t="s">
         <v>117</v>
       </c>
@@ -1639,7 +1686,9 @@
         <v>55</v>
       </c>
       <c r="F30" s="3"/>
-      <c r="G30" s="6"/>
+      <c r="G30" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="H30" s="7"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1693,7 +1742,9 @@
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="6"/>
+      <c r="G33" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="H33" s="7" t="s">
         <v>57</v>
       </c>
@@ -2291,7 +2342,9 @@
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
-      <c r="G66" s="6"/>
+      <c r="G66" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="H66" s="7"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -2398,12 +2451,12 @@
       </c>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
-      <c r="D73" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
-      <c r="G73" s="6"/>
+      <c r="G73" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="H73" s="7"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -2572,21 +2625,17 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B84" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C84" s="3"/>
       <c r="D84" s="3" t="s">
         <v>55</v>
       </c>
       <c r="E84" s="3"/>
-      <c r="F84" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="F84" s="3"/>
       <c r="G84" s="6" t="s">
         <v>55</v>
       </c>
@@ -2594,7 +2643,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>32</v>
+        <v>107</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>55</v>
@@ -2602,9 +2651,13 @@
       <c r="C85" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D85" s="3"/>
+      <c r="D85" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E85" s="3"/>
-      <c r="F85" s="3"/>
+      <c r="F85" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="G85" s="6" t="s">
         <v>55</v>
       </c>
@@ -2612,7 +2665,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>55</v>
@@ -2630,10 +2683,14 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B87" s="3"/>
-      <c r="C87" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
       <c r="F87" s="3"/>
@@ -2644,11 +2701,9 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="B88" s="3"/>
       <c r="C88" s="3"/>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
@@ -2659,46 +2714,48 @@
       <c r="H88" s="7"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="10" t="s">
-        <v>118</v>
+      <c r="A89" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C89" s="3"/>
-      <c r="D89" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D89" s="3"/>
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
-      <c r="G89" s="6"/>
-      <c r="H89" s="7" t="s">
-        <v>119</v>
-      </c>
+      <c r="G89" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H89" s="7"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
-        <v>145</v>
+      <c r="A90" s="10" t="s">
+        <v>118</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C90" s="3"/>
-      <c r="D90" s="3"/>
+      <c r="D90" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
       <c r="G90" s="6" t="s">
         <v>55</v>
       </c>
       <c r="H90" s="7" t="s">
-        <v>146</v>
+        <v>119</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B91" s="3"/>
+        <v>145</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
@@ -2707,16 +2764,14 @@
         <v>55</v>
       </c>
       <c r="H91" s="7" t="s">
-        <v>79</v>
+        <v>146</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B92" s="3"/>
       <c r="C92" s="3"/>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
@@ -2725,62 +2780,66 @@
         <v>55</v>
       </c>
       <c r="H92" s="7" t="s">
-        <v>166</v>
+        <v>79</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>83</v>
+        <v>165</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C93" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C93" s="3"/>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
       <c r="G93" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H93" s="7"/>
+        <v>184</v>
+      </c>
+      <c r="H93" s="7" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B94" s="3"/>
-      <c r="C94" s="3"/>
+        <v>83</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
       <c r="F94" s="3"/>
-      <c r="G94" s="6"/>
+      <c r="G94" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="H94" s="7"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
-      <c r="D95" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D95" s="3"/>
       <c r="E95" s="3"/>
       <c r="F95" s="3"/>
-      <c r="G95" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="G95" s="6"/>
       <c r="H95" s="7"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
-      <c r="D96" s="3"/>
+      <c r="D96" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E96" s="3"/>
       <c r="F96" s="3"/>
       <c r="G96" s="6" t="s">
@@ -2790,14 +2849,10 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B97" s="3"/>
+      <c r="C97" s="3"/>
       <c r="D97" s="3"/>
       <c r="E97" s="3"/>
       <c r="F97" s="3"/>
@@ -2808,10 +2863,14 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B98" s="3"/>
-      <c r="C98" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D98" s="3"/>
       <c r="E98" s="3"/>
       <c r="F98" s="3"/>
@@ -2821,12 +2880,10 @@
       <c r="H98" s="7"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A99" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B99" s="3"/>
       <c r="C99" s="3"/>
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
@@ -2834,47 +2891,45 @@
       <c r="G99" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H99" s="7" t="s">
-        <v>121</v>
-      </c>
+      <c r="H99" s="7"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B100" s="3"/>
+      <c r="A100" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
       <c r="G100" s="6" t="s">
-        <v>180</v>
+        <v>55</v>
       </c>
       <c r="H100" s="7" t="s">
-        <v>158</v>
+        <v>121</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="B101" s="3"/>
+      <c r="C101" s="3"/>
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
       <c r="F101" s="3"/>
       <c r="G101" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H101" s="7"/>
+        <v>180</v>
+      </c>
+      <c r="H101" s="7" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>55</v>
@@ -2892,25 +2947,25 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B103" s="3"/>
-      <c r="C103" s="3"/>
-      <c r="D103" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D103" s="3"/>
       <c r="E103" s="3"/>
       <c r="F103" s="3"/>
       <c r="G103" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H103" s="7" t="s">
-        <v>171</v>
-      </c>
+      <c r="H103" s="7"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
@@ -2923,16 +2978,14 @@
         <v>55</v>
       </c>
       <c r="H104" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="B105" s="3"/>
       <c r="C105" s="3"/>
       <c r="D105" s="3" t="s">
         <v>55</v>
@@ -2943,33 +2996,39 @@
         <v>55</v>
       </c>
       <c r="H105" s="7" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B106" s="3"/>
+        <v>169</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C106" s="3"/>
-      <c r="D106" s="3"/>
-      <c r="E106" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D106" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E106" s="3"/>
       <c r="F106" s="3"/>
       <c r="G106" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H106" s="7"/>
+      <c r="H106" s="7" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
       <c r="D107" s="3"/>
-      <c r="E107" s="3"/>
+      <c r="E107" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F107" s="3"/>
       <c r="G107" s="6" t="s">
         <v>55</v>
@@ -2978,87 +3037,87 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
       <c r="D108" s="3"/>
       <c r="E108" s="3"/>
       <c r="F108" s="3"/>
-      <c r="G108" s="6"/>
-      <c r="H108" s="7" t="s">
-        <v>179</v>
-      </c>
+      <c r="G108" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H108" s="7"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A109" s="9" t="s">
-        <v>128</v>
+      <c r="A109" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
       <c r="D109" s="3"/>
       <c r="E109" s="3"/>
       <c r="F109" s="3"/>
-      <c r="G109" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H109" s="7"/>
+      <c r="G109" s="6"/>
+      <c r="H109" s="7" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B110" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C110" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A110" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B110" s="3"/>
+      <c r="C110" s="3"/>
       <c r="D110" s="3"/>
       <c r="E110" s="3"/>
       <c r="F110" s="3"/>
       <c r="G110" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H110" s="7" t="s">
-        <v>75</v>
-      </c>
+      <c r="H110" s="7"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" s="10" t="s">
-        <v>88</v>
+      <c r="A111" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C111" s="3"/>
+      <c r="C111" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D111" s="3"/>
       <c r="E111" s="3"/>
       <c r="F111" s="3"/>
-      <c r="G111" s="6"/>
+      <c r="G111" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="H111" s="7" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
-        <v>42</v>
+      <c r="A112" s="10" t="s">
+        <v>88</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C112" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C112" s="3"/>
       <c r="D112" s="3"/>
       <c r="E112" s="3"/>
       <c r="F112" s="3"/>
-      <c r="G112" s="6"/>
-      <c r="H112" s="7"/>
+      <c r="G112" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="H112" s="7" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>55</v>
@@ -3069,17 +3128,19 @@
       <c r="D113" s="3"/>
       <c r="E113" s="3"/>
       <c r="F113" s="3"/>
-      <c r="G113" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="G113" s="6"/>
       <c r="H113" s="7"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B114" s="3"/>
-      <c r="C114" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D114" s="3"/>
       <c r="E114" s="3"/>
       <c r="F114" s="3"/>
@@ -3090,7 +3151,7 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
@@ -3104,21 +3165,13 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C116" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B116" s="3"/>
+      <c r="C116" s="3"/>
       <c r="D116" s="3"/>
-      <c r="E116" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F116" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="E116" s="3"/>
+      <c r="F116" s="3"/>
       <c r="G116" s="6" t="s">
         <v>55</v>
       </c>
@@ -3126,15 +3179,21 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>110</v>
+        <v>46</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C117" s="3"/>
+      <c r="C117" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D117" s="3"/>
-      <c r="E117" s="3"/>
-      <c r="F117" s="3"/>
+      <c r="E117" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F117" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="G117" s="6" t="s">
         <v>55</v>
       </c>
@@ -3142,17 +3201,13 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>47</v>
+        <v>110</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C118" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D118" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C118" s="3"/>
+      <c r="D118" s="3"/>
       <c r="E118" s="3"/>
       <c r="F118" s="3"/>
       <c r="G118" s="6" t="s">
@@ -3162,11 +3217,17 @@
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B119" s="3"/>
-      <c r="C119" s="3"/>
-      <c r="D119" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E119" s="3"/>
       <c r="F119" s="3"/>
       <c r="G119" s="6" t="s">
@@ -3176,43 +3237,37 @@
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B120" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="B120" s="3"/>
       <c r="C120" s="3"/>
       <c r="D120" s="3"/>
       <c r="E120" s="3"/>
       <c r="F120" s="3"/>
-      <c r="G120" s="6"/>
-      <c r="H120" s="7" t="s">
-        <v>168</v>
-      </c>
+      <c r="G120" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H120" s="7"/>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>73</v>
+        <v>167</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C121" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C121" s="3"/>
       <c r="D121" s="3"/>
       <c r="E121" s="3"/>
       <c r="F121" s="3"/>
-      <c r="G121" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="G121" s="6"/>
       <c r="H121" s="7" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>55</v>
@@ -3220,23 +3275,19 @@
       <c r="C122" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D122" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E122" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D122" s="3"/>
+      <c r="E122" s="3"/>
       <c r="F122" s="3"/>
       <c r="G122" s="6" t="s">
         <v>55</v>
       </c>
       <c r="H122" s="7" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>55</v>
@@ -3247,16 +3298,20 @@
       <c r="D123" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E123" s="3"/>
+      <c r="E123" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F123" s="3"/>
       <c r="G123" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H123" s="7"/>
+      <c r="H123" s="7" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>55</v>
@@ -3264,7 +3319,9 @@
       <c r="C124" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D124" s="3"/>
+      <c r="D124" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E124" s="3"/>
       <c r="F124" s="3"/>
       <c r="G124" s="6" t="s">
@@ -3274,10 +3331,14 @@
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B125" s="3"/>
-      <c r="C125" s="3"/>
+        <v>51</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D125" s="3"/>
       <c r="E125" s="3"/>
       <c r="F125" s="3"/>
@@ -3287,52 +3348,50 @@
       <c r="H125" s="7"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A126" s="8" t="s">
-        <v>127</v>
+      <c r="A126" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
       <c r="D126" s="3"/>
       <c r="E126" s="3"/>
       <c r="F126" s="3"/>
-      <c r="G126" s="6"/>
+      <c r="G126" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="H126" s="7"/>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
-        <v>66</v>
+      <c r="A127" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
       <c r="D127" s="3"/>
-      <c r="E127" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="E127" s="3"/>
       <c r="F127" s="3"/>
-      <c r="G127" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="G127" s="6"/>
       <c r="H127" s="7"/>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B128" s="3"/>
+      <c r="C128" s="3"/>
+      <c r="D128" s="3"/>
+      <c r="E128" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F128" s="3"/>
+      <c r="G128" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H128" s="7"/>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B128" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C128" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D128" s="3"/>
-      <c r="E128" s="3"/>
-      <c r="F128" s="3"/>
-      <c r="G128" s="6"/>
-      <c r="H128" s="7"/>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A129" s="10" t="s">
-        <v>53</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>55</v>
@@ -3343,14 +3402,12 @@
       <c r="D129" s="3"/>
       <c r="E129" s="3"/>
       <c r="F129" s="3"/>
-      <c r="G129" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="G129" s="6"/>
       <c r="H129" s="7"/>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A130" s="1" t="s">
-        <v>113</v>
+      <c r="A130" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>55</v>
@@ -3360,37 +3417,56 @@
       </c>
       <c r="D130" s="3"/>
       <c r="E130" s="3"/>
-      <c r="F130" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="F130" s="3"/>
       <c r="G130" s="6" t="s">
         <v>55</v>
       </c>
       <c r="H130" s="7"/>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A132" s="10" t="s">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D131" s="3"/>
+      <c r="E131" s="3"/>
+      <c r="F131" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G131" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H131" s="7"/>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A133" s="10" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A133" s="8" t="s">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A134" s="8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A134" s="9" t="s">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A135" s="9" t="s">
         <v>129</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H130" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H131" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="G1" r:id="rId1" display="https://github.com/microsoft/winget-pkgs" xr:uid="{2C434A13-8B1C-492F-95C8-B89737A54984}"/>
     <hyperlink ref="A44" r:id="rId2" xr:uid="{5AAD9A6E-C562-4737-9662-CEC2B195962E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
feat: migrate to winget
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\markus\projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F16F302-E0D8-43BD-9716-7931ADCAD6B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB99B90-B8CF-4F79-85A2-72C4E26D432F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$131</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$133</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="291">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -454,9 +454,6 @@
     <t>git bash / cli related</t>
   </si>
   <si>
-    <t>Not working. Installs to postman's location.</t>
-  </si>
-  <si>
     <t>Secondary</t>
   </si>
   <si>
@@ -515,9 +512,6 @@
   </si>
   <si>
     <t>exiftool</t>
-  </si>
-  <si>
-    <t>Addon for ImageGlass</t>
   </si>
   <si>
     <t>Image Viewer; use with exiftool (https://github.com/d2phap/ImageGlass)</t>
@@ -624,22 +618,343 @@
     <t>App wurde eingestellt</t>
   </si>
   <si>
-    <t>x (sweethome3d)</t>
-  </si>
-  <si>
     <t>neovim</t>
   </si>
   <si>
     <t>Version in chocolatey (1.15) too old (current: 1.16)</t>
   </si>
   <si>
-    <t>x (ctags)</t>
-  </si>
-  <si>
-    <t>x (shellexview)</t>
-  </si>
-  <si>
     <t>powershell-core</t>
+  </si>
+  <si>
+    <t>7zip.7zip</t>
+  </si>
+  <si>
+    <t>Adobe.Acrobat.Reader.64-bit</t>
+  </si>
+  <si>
+    <t>AutoHotkey.AutoHotkey</t>
+  </si>
+  <si>
+    <t>Amazon.AWSCLI</t>
+  </si>
+  <si>
+    <t>dbeaver.dbeaver</t>
+  </si>
+  <si>
+    <t>OliverBetz.ExifTool</t>
+  </si>
+  <si>
+    <t>DuongDieuPhap.ImageGlass</t>
+  </si>
+  <si>
+    <t>Addon for ImageGlass; winget installs to %AppDataLocal%\Programs\ExifTool</t>
+  </si>
+  <si>
+    <t>winget migration todo</t>
+  </si>
+  <si>
+    <t>sharkdp.fd</t>
+  </si>
+  <si>
+    <t>Mozilla.Firefox</t>
+  </si>
+  <si>
+    <t>junegunn.fzf</t>
+  </si>
+  <si>
+    <t>GitHub.cli</t>
+  </si>
+  <si>
+    <t>Git.Git</t>
+  </si>
+  <si>
+    <t>Google.Chrome</t>
+  </si>
+  <si>
+    <t>Hash stimmt nicht</t>
+  </si>
+  <si>
+    <t>Inkscape.Inkscape</t>
+  </si>
+  <si>
+    <t>JetBrains.Toolbox</t>
+  </si>
+  <si>
+    <t>stedolan.jq</t>
+  </si>
+  <si>
+    <t>KeePassXCTeam.KeePassXC</t>
+  </si>
+  <si>
+    <t>KaiKramer.KeyStoreExplorer</t>
+  </si>
+  <si>
+    <t>Microsoft.Teams</t>
+  </si>
+  <si>
+    <t>Microsoft.WindowsTerminal</t>
+  </si>
+  <si>
+    <t>Installieren fehlgeschlagen mit Exitcode: 0x80070002 : Das System kann die angegebene Datei nicht finden.</t>
+  </si>
+  <si>
+    <t>Neovim.Neovim</t>
+  </si>
+  <si>
+    <t>OpenJS.NodeJS.LTS</t>
+  </si>
+  <si>
+    <t>Notepad++.Notepad++</t>
+  </si>
+  <si>
+    <t>Postman.Postman</t>
+  </si>
+  <si>
+    <t>Microsoft.PowerShell</t>
+  </si>
+  <si>
+    <t>Microsoft.PowerToys</t>
+  </si>
+  <si>
+    <t>BurntSushi.ripgrep.MSVC</t>
+  </si>
+  <si>
+    <t>SlackTechnologies.Slack</t>
+  </si>
+  <si>
+    <t>EclipseAdoptium.Temurin.11.JDK</t>
+  </si>
+  <si>
+    <t>EclipseAdoptium.Temurin.17.JDK</t>
+  </si>
+  <si>
+    <t>EclipseAdoptium.Temurin.8.JDK</t>
+  </si>
+  <si>
+    <t>Microsoft.VisualStudioCode</t>
+  </si>
+  <si>
+    <t>WinDirStat.WinDirStat</t>
+  </si>
+  <si>
+    <t>WinMerge.WinMerge</t>
+  </si>
+  <si>
+    <t>Zoom.Zoom</t>
+  </si>
+  <si>
+    <t>youtube-dl.youtube-dl</t>
+  </si>
+  <si>
+    <t>XnSoft.XnView.Classic</t>
+  </si>
+  <si>
+    <t>WinSCP.WinSCP</t>
+  </si>
+  <si>
+    <t>RARLab.WinRAR</t>
+  </si>
+  <si>
+    <t>WhatsApp.WhatsApp</t>
+  </si>
+  <si>
+    <t>StefanMalzner.Franz</t>
+  </si>
+  <si>
+    <t>RealVNC.VNCViewer</t>
+  </si>
+  <si>
+    <t>VideoLAN.VLC</t>
+  </si>
+  <si>
+    <t>ElaborateBytes.VirtualCloneDrive</t>
+  </si>
+  <si>
+    <t>Oracle.VirtualBox</t>
+  </si>
+  <si>
+    <t>Ubisoft.Connect</t>
+  </si>
+  <si>
+    <t>UniversalCtags.Ctags</t>
+  </si>
+  <si>
+    <t>Logitech.UnifyingSoftware</t>
+  </si>
+  <si>
+    <t>Logitech.Options</t>
+  </si>
+  <si>
+    <t>logioptionsplus</t>
+  </si>
+  <si>
+    <t>Logitech.OptionsPlus</t>
+  </si>
+  <si>
+    <t>Logitech.LogiBolt</t>
+  </si>
+  <si>
+    <t>Google.AndroidStudio</t>
+  </si>
+  <si>
+    <t>Audacity.Audacity</t>
+  </si>
+  <si>
+    <t>Canneverbe.CDBurnerXP</t>
+  </si>
+  <si>
+    <t>Maximus5.ConEmu</t>
+  </si>
+  <si>
+    <t>Cryptomator.Cryptomator</t>
+  </si>
+  <si>
+    <t>Discord.Discord</t>
+  </si>
+  <si>
+    <t>Docker.DockerDesktop</t>
+  </si>
+  <si>
+    <t>EpicGames.EpicGamesLauncher</t>
+  </si>
+  <si>
+    <t>Balena.Etcher</t>
+  </si>
+  <si>
+    <t>evernote.evernote</t>
+  </si>
+  <si>
+    <t>FastStone.Viewer</t>
+  </si>
+  <si>
+    <t>GitExtensionsTeam.GitExtensions</t>
+  </si>
+  <si>
+    <t>GOG.Galaxy</t>
+  </si>
+  <si>
+    <t>Google.EarthPro</t>
+  </si>
+  <si>
+    <t>HandBrake.HandBrake</t>
+  </si>
+  <si>
+    <t>HeidiSQL.HeidiSQL</t>
+  </si>
+  <si>
+    <t>LIGHTNINGUK.ImgBurn</t>
+  </si>
+  <si>
+    <t>Insomnia.Insomnia</t>
+  </si>
+  <si>
+    <t>Not working for chocolatey, installs to postman's location.</t>
+  </si>
+  <si>
+    <t>JetBrains.IntelliJIDEA.Ultimate</t>
+  </si>
+  <si>
+    <t>IrfanSkiljan.IrfanView</t>
+  </si>
+  <si>
+    <t>CodecGuide.K-LiteCodecPack.Mega</t>
+  </si>
+  <si>
+    <t>DominikReichl.KeePass</t>
+  </si>
+  <si>
+    <t>Cockos.LICEcap</t>
+  </si>
+  <si>
+    <t>Meld.Meld</t>
+  </si>
+  <si>
+    <t>MoritzBunkus.MKVToolNix</t>
+  </si>
+  <si>
+    <t>Mobatek.MobaXterm</t>
+  </si>
+  <si>
+    <t>Microsoft.MouseWithoutBorders</t>
+  </si>
+  <si>
+    <t>Mp3tag.Mp3tag</t>
+  </si>
+  <si>
+    <t>fjsoft.MyPhoneExplorer</t>
+  </si>
+  <si>
+    <t>Oracle.MySQL</t>
+  </si>
+  <si>
+    <t>Nextcloud.NextcloudDesktop</t>
+  </si>
+  <si>
+    <t>OBSProject.OBSStudio</t>
+  </si>
+  <si>
+    <t>ownCloud.ownCloudDesktop</t>
+  </si>
+  <si>
+    <t>PostgreSQL.pgAdmin</t>
+  </si>
+  <si>
+    <t>PostgreSQL.PostgreSQL</t>
+  </si>
+  <si>
+    <t>PowerSoftware.PowerISO</t>
+  </si>
+  <si>
+    <t>Microsoft.Sysinternals.ProcessExplorer</t>
+  </si>
+  <si>
+    <t>Microsoft.Sysinternals.ProcessMonitor</t>
+  </si>
+  <si>
+    <t>PuTTY.PuTTY</t>
+  </si>
+  <si>
+    <t>Python.Python.3.12</t>
+  </si>
+  <si>
+    <t>Rufus.Rufus</t>
+  </si>
+  <si>
+    <t>Logitech.SetPoint</t>
+  </si>
+  <si>
+    <t>NirSoft.ShellExView</t>
+  </si>
+  <si>
+    <t>Microsoft.Skype</t>
+  </si>
+  <si>
+    <t>Atlassian.Sourcetree</t>
+  </si>
+  <si>
+    <t>Valve.Steam</t>
+  </si>
+  <si>
+    <t>SublimeHQ.SublimeText.3</t>
+  </si>
+  <si>
+    <t>Starship.Starship</t>
+  </si>
+  <si>
+    <t>eTeks.SweetHome3D</t>
+  </si>
+  <si>
+    <t>9P7KNL5RWT25</t>
+  </si>
+  <si>
+    <t>TeamViewer.TeamViewer</t>
+  </si>
+  <si>
+    <t>Mozilla.Thunderbird</t>
+  </si>
+  <si>
+    <t>TortoiseSVN.TortoiseSVN</t>
   </si>
 </sst>
 </file>
@@ -713,7 +1028,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -744,6 +1059,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF002B36"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -779,7 +1106,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -805,6 +1132,24 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
@@ -1152,11 +1497,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H135"/>
+  <dimension ref="A1:I137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G84" sqref="G84"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,11 +1510,12 @@
     <col min="2" max="3" width="6.140625" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" customWidth="1"/>
     <col min="5" max="6" width="7.7109375" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="66.42578125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="70.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>54</v>
       </c>
@@ -1177,7 +1523,7 @@
         <v>70</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>72</v>
@@ -1186,7 +1532,7 @@
         <v>71</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>98</v>
@@ -1194,8 +1540,11 @@
       <c r="H1" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>58</v>
       </c>
@@ -1214,12 +1563,13 @@
       <c r="F2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>55</v>
+      <c r="G2" s="14" t="s">
+        <v>181</v>
       </c>
       <c r="H2" s="7"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1234,8 +1584,9 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>59</v>
       </c>
@@ -1254,12 +1605,13 @@
       <c r="F4" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>55</v>
+      <c r="G4" s="14" t="s">
+        <v>182</v>
       </c>
       <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1268,12 +1620,13 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="6" t="s">
-        <v>55</v>
+      <c r="G5" s="17" t="s">
+        <v>237</v>
       </c>
       <c r="H5" s="7"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>91</v>
       </c>
@@ -1284,12 +1637,13 @@
         <v>55</v>
       </c>
       <c r="F6" s="3"/>
-      <c r="G6" s="6" t="s">
-        <v>55</v>
+      <c r="G6" s="17" t="s">
+        <v>238</v>
       </c>
       <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>92</v>
       </c>
@@ -1302,8 +1656,9 @@
       <c r="F7" s="3"/>
       <c r="G7" s="6"/>
       <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>93</v>
       </c>
@@ -1316,8 +1671,9 @@
       <c r="F8" s="3"/>
       <c r="G8" s="6"/>
       <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>60</v>
       </c>
@@ -1332,12 +1688,13 @@
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="6" t="s">
-        <v>55</v>
+      <c r="G9" s="14" t="s">
+        <v>183</v>
       </c>
       <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>100</v>
       </c>
@@ -1348,12 +1705,13 @@
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="6" t="s">
-        <v>55</v>
+      <c r="G10" s="14" t="s">
+        <v>184</v>
       </c>
       <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -1364,8 +1722,9 @@
       <c r="F11" s="3"/>
       <c r="G11" s="6"/>
       <c r="H11" s="7"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>114</v>
       </c>
@@ -1382,8 +1741,9 @@
       <c r="H12" s="7" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>124</v>
       </c>
@@ -1394,10 +1754,11 @@
       <c r="F13" s="3"/>
       <c r="G13" s="6"/>
       <c r="H13" s="7" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>125</v>
       </c>
@@ -1408,10 +1769,11 @@
       <c r="F14" s="3"/>
       <c r="G14" s="6"/>
       <c r="H14" s="7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -1426,16 +1788,17 @@
         <v>55</v>
       </c>
       <c r="F15" s="3"/>
-      <c r="G15" s="6" t="s">
-        <v>55</v>
+      <c r="G15" s="17" t="s">
+        <v>239</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>55</v>
@@ -1446,10 +1809,11 @@
       <c r="F16" s="3"/>
       <c r="G16" s="6"/>
       <c r="H16" s="7" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
@@ -1460,8 +1824,9 @@
       <c r="F17" s="3"/>
       <c r="G17" s="6"/>
       <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -1470,12 +1835,13 @@
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="6" t="s">
-        <v>55</v>
+      <c r="G18" s="17" t="s">
+        <v>240</v>
       </c>
       <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>101</v>
       </c>
@@ -1486,14 +1852,15 @@
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="6" t="s">
-        <v>55</v>
+      <c r="G19" s="17" t="s">
+        <v>241</v>
       </c>
       <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="7"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>55</v>
@@ -1504,14 +1871,15 @@
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="6" t="s">
-        <v>55</v>
+      <c r="G20" s="14" t="s">
+        <v>185</v>
       </c>
       <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>55</v>
@@ -1520,32 +1888,30 @@
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="6" t="s">
-        <v>55</v>
+      <c r="G21" s="17" t="s">
+        <v>242</v>
       </c>
       <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="6" t="s">
-        <v>55</v>
+      <c r="G22" s="17" t="s">
+        <v>243</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>6</v>
       </c>
@@ -1560,8 +1926,9 @@
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="7"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -1572,8 +1939,9 @@
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="7"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>102</v>
       </c>
@@ -1586,12 +1954,13 @@
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="6" t="s">
-        <v>55</v>
+      <c r="G25" s="17" t="s">
+        <v>244</v>
       </c>
       <c r="H25" s="7"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>99</v>
       </c>
@@ -1602,14 +1971,15 @@
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="6" t="s">
-        <v>55</v>
+      <c r="G26" s="17" t="s">
+        <v>245</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+      <c r="I26" s="7"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>8</v>
       </c>
@@ -1624,14 +1994,15 @@
       <c r="F27" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G27" s="6" t="s">
-        <v>55</v>
+      <c r="G27" s="17" t="s">
+        <v>246</v>
       </c>
       <c r="H27" s="7"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="7"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>55</v>
@@ -1644,14 +2015,15 @@
       <c r="F28" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G28" s="6" t="s">
-        <v>55</v>
+      <c r="G28" s="14" t="s">
+        <v>186</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="I28" s="7"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>116</v>
       </c>
@@ -1664,14 +2036,15 @@
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="6" t="s">
-        <v>55</v>
+      <c r="G29" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="7"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>9</v>
       </c>
@@ -1690,8 +2063,9 @@
         <v>55</v>
       </c>
       <c r="H30" s="7"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" s="7"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>10</v>
       </c>
@@ -1708,12 +2082,13 @@
         <v>55</v>
       </c>
       <c r="F31" s="3"/>
-      <c r="G31" s="6" t="s">
-        <v>55</v>
+      <c r="G31" s="14" t="s">
+        <v>191</v>
       </c>
       <c r="H31" s="7"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" s="7"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>67</v>
       </c>
@@ -1722,14 +2097,15 @@
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="6" t="s">
-        <v>55</v>
+      <c r="G32" s="17" t="s">
+        <v>247</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+      <c r="I32" s="7"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>56</v>
       </c>
@@ -1742,14 +2118,15 @@
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="6" t="s">
-        <v>55</v>
+      <c r="G33" s="14" t="s">
+        <v>192</v>
       </c>
       <c r="H33" s="7" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" s="7"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>103</v>
       </c>
@@ -1760,14 +2137,15 @@
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
-      <c r="G34" s="6" t="s">
-        <v>55</v>
+      <c r="G34" s="14" t="s">
+        <v>193</v>
       </c>
       <c r="H34" s="7" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34" s="7"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>61</v>
       </c>
@@ -1782,12 +2160,13 @@
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
-      <c r="G35" s="6" t="s">
-        <v>55</v>
+      <c r="G35" s="14" t="s">
+        <v>194</v>
       </c>
       <c r="H35" s="7"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" s="7"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>11</v>
       </c>
@@ -1796,12 +2175,13 @@
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
-      <c r="G36" s="6" t="s">
-        <v>55</v>
+      <c r="G36" s="17" t="s">
+        <v>248</v>
       </c>
       <c r="H36" s="7"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" s="7"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>87</v>
       </c>
@@ -1814,14 +2194,15 @@
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
-      <c r="G37" s="6" t="s">
-        <v>55</v>
+      <c r="G37" s="17" t="s">
+        <v>249</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="I37" s="13"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>12</v>
       </c>
@@ -1838,12 +2219,15 @@
         <v>55</v>
       </c>
       <c r="F38" s="3"/>
-      <c r="G38" s="6" t="s">
-        <v>55</v>
+      <c r="G38" s="16" t="s">
+        <v>195</v>
       </c>
       <c r="H38" s="7"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>13</v>
       </c>
@@ -1856,12 +2240,13 @@
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
-      <c r="G39" s="6" t="s">
-        <v>55</v>
+      <c r="G39" s="17" t="s">
+        <v>250</v>
       </c>
       <c r="H39" s="7"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="7"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>14</v>
       </c>
@@ -1872,10 +2257,11 @@
       <c r="F40" s="3"/>
       <c r="G40" s="6"/>
       <c r="H40" s="7"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" s="7"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>55</v>
@@ -1886,14 +2272,15 @@
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
-      <c r="G41" s="6" t="s">
-        <v>55</v>
+      <c r="G41" s="17" t="s">
+        <v>251</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="I41" s="7"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
         <v>84</v>
       </c>
@@ -1906,8 +2293,9 @@
       <c r="H42" s="7" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42" s="7"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>15</v>
       </c>
@@ -1918,14 +2306,15 @@
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
-      <c r="G43" s="6" t="s">
-        <v>55</v>
+      <c r="G43" s="17" t="s">
+        <v>252</v>
       </c>
       <c r="H43" s="7"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" s="7"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1936,14 +2325,15 @@
       <c r="F44" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G44" s="6" t="s">
-        <v>55</v>
+      <c r="G44" s="14" t="s">
+        <v>187</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="I44" s="7"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>16</v>
       </c>
@@ -1958,14 +2348,15 @@
         <v>55</v>
       </c>
       <c r="F45" s="3"/>
-      <c r="G45" s="6" t="s">
-        <v>55</v>
+      <c r="G45" s="17" t="s">
+        <v>253</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="I45" s="7"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>90</v>
       </c>
@@ -1980,12 +2371,13 @@
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
-      <c r="G46" s="6" t="s">
-        <v>55</v>
+      <c r="G46" s="14" t="s">
+        <v>197</v>
       </c>
       <c r="H46" s="7"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46" s="7"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>96</v>
       </c>
@@ -1996,14 +2388,15 @@
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
-      <c r="G47" s="6" t="s">
-        <v>55</v>
+      <c r="G47" s="17" t="s">
+        <v>254</v>
       </c>
       <c r="H47" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+      <c r="I47" s="13"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>80</v>
       </c>
@@ -2014,14 +2407,15 @@
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
-      <c r="G48" s="6" t="s">
-        <v>55</v>
+      <c r="G48" s="17" t="s">
+        <v>256</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="I48" s="7"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>17</v>
       </c>
@@ -2032,12 +2426,13 @@
         <v>55</v>
       </c>
       <c r="F49" s="3"/>
-      <c r="G49" s="6" t="s">
-        <v>55</v>
+      <c r="G49" s="17" t="s">
+        <v>257</v>
       </c>
       <c r="H49" s="7"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49" s="7"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>18</v>
       </c>
@@ -2052,10 +2447,11 @@
       <c r="F50" s="3"/>
       <c r="G50" s="6"/>
       <c r="H50" s="7"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50" s="7"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>55</v>
@@ -2066,12 +2462,13 @@
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
-      <c r="G51" s="6" t="s">
-        <v>55</v>
+      <c r="G51" s="14" t="s">
+        <v>198</v>
       </c>
       <c r="H51" s="7"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51" s="7"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
         <v>19</v>
       </c>
@@ -2082,12 +2479,13 @@
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
-      <c r="G52" s="6" t="s">
-        <v>55</v>
+      <c r="G52" s="14" t="s">
+        <v>199</v>
       </c>
       <c r="H52" s="7"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52" s="7"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>20</v>
       </c>
@@ -2102,14 +2500,15 @@
         <v>55</v>
       </c>
       <c r="F53" s="3"/>
-      <c r="G53" s="6" t="s">
-        <v>55</v>
+      <c r="G53" s="17" t="s">
+        <v>258</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="I53" s="7"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>62</v>
       </c>
@@ -2119,21 +2518,20 @@
       <c r="C54" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D54" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D54" s="3"/>
       <c r="E54" s="3"/>
       <c r="F54" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G54" s="6" t="s">
-        <v>55</v>
+      <c r="G54" s="17" t="s">
+        <v>259</v>
       </c>
       <c r="H54" s="7"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54" s="7"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>55</v>
@@ -2148,12 +2546,13 @@
       <c r="F55" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G55" s="6" t="s">
-        <v>55</v>
+      <c r="G55" s="14" t="s">
+        <v>200</v>
       </c>
       <c r="H55" s="7"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55" s="7"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>21</v>
       </c>
@@ -2163,19 +2562,16 @@
       <c r="C56" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D56" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D56" s="3"/>
       <c r="E56" s="3"/>
       <c r="F56" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G56" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="G56" s="6"/>
       <c r="H56" s="7"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I56" s="7"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>86</v>
       </c>
@@ -2188,14 +2584,15 @@
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
-      <c r="G57" s="6" t="s">
-        <v>55</v>
+      <c r="G57" s="14" t="s">
+        <v>201</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="I57" s="7"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
         <v>22</v>
       </c>
@@ -2206,10 +2603,11 @@
       <c r="F58" s="3"/>
       <c r="G58" s="6"/>
       <c r="H58" s="7"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I58" s="7"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>55</v>
@@ -2222,10 +2620,11 @@
       <c r="F59" s="3"/>
       <c r="G59" s="6"/>
       <c r="H59" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="I59" s="7"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>122</v>
       </c>
@@ -2234,56 +2633,51 @@
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
-      <c r="G60" s="6" t="s">
-        <v>55</v>
+      <c r="G60" s="17" t="s">
+        <v>260</v>
       </c>
       <c r="H60" s="7" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="I60" s="7"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="1"/>
       <c r="B61" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C61" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C61" s="3"/>
       <c r="D61" s="3" t="s">
         <v>55</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
-      <c r="G61" s="6" t="s">
-        <v>55</v>
+      <c r="G61" s="18" t="s">
+        <v>236</v>
       </c>
       <c r="H61" s="7"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61" s="7"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="B62" s="3"/>
       <c r="C62" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
-      <c r="F62" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G62" s="6" t="s">
-        <v>55</v>
+      <c r="F62" s="3"/>
+      <c r="G62" s="17" t="s">
+        <v>233</v>
       </c>
       <c r="H62" s="7"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I62" s="7"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>23</v>
+        <v>234</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>55</v>
@@ -2294,192 +2688,210 @@
       </c>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
-      <c r="G63" s="6" t="s">
-        <v>55</v>
+      <c r="G63" s="18" t="s">
+        <v>235</v>
       </c>
       <c r="H63" s="7"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I63" s="7"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
+        <v>111</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H64" s="7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F64" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G64" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="H64" s="7"/>
+      <c r="I64" s="7"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>142</v>
+        <v>23</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
+      <c r="D65" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
-      <c r="G65" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H65" s="7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G65" s="6"/>
+      <c r="H65" s="7"/>
+      <c r="I65" s="7"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
-      <c r="G66" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H66" s="7"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G66" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="H66" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I66" s="7"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B67" s="3"/>
+        <v>141</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
-      <c r="G67" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H67" s="7"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G67" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="H67" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="I67" s="7"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
-      <c r="G68" s="6" t="s">
-        <v>55</v>
+      <c r="G68" s="17" t="s">
+        <v>263</v>
       </c>
       <c r="H68" s="7"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I68" s="7"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>108</v>
+        <v>25</v>
       </c>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
-      <c r="D69" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D69" s="3"/>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
-      <c r="G69" s="6" t="s">
-        <v>55</v>
+      <c r="G69" s="17" t="s">
+        <v>264</v>
       </c>
       <c r="H69" s="7"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I69" s="7"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D70" s="3"/>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
-      <c r="G70" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H70" s="7" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G70" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="H70" s="7"/>
+      <c r="I70" s="7"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="B71" s="3"/>
-      <c r="C71" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E71" s="3"/>
-      <c r="F71" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G71" s="6" t="s">
-        <v>55</v>
+      <c r="F71" s="3"/>
+      <c r="G71" s="14" t="s">
+        <v>202</v>
       </c>
       <c r="H71" s="7"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I71" s="7"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
+      <c r="D72" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
-      <c r="G72" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H72" s="7"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G72" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="H72" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="I72" s="15" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>181</v>
+        <v>76</v>
       </c>
       <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
+      <c r="C73" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
-      <c r="G73" s="6" t="s">
-        <v>55</v>
+      <c r="F73" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G73" s="17" t="s">
+        <v>266</v>
       </c>
       <c r="H73" s="7"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I73" s="7"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
-      <c r="G74" s="6" t="s">
-        <v>55</v>
+      <c r="G74" s="17" t="s">
+        <v>267</v>
       </c>
       <c r="H74" s="7"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>63</v>
+      <c r="I74" s="7"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="10" t="s">
+        <v>178</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>55</v>
@@ -2490,14 +2902,15 @@
       </c>
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
-      <c r="G75" s="6" t="s">
-        <v>55</v>
+      <c r="G75" s="14" t="s">
+        <v>205</v>
       </c>
       <c r="H75" s="7"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I75" s="7"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>55</v>
@@ -2505,185 +2918,190 @@
       <c r="C76" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D76" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F76" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G76" s="6" t="s">
-        <v>55</v>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="17" t="s">
+        <v>268</v>
       </c>
       <c r="H76" s="7"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I76" s="7"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B77" s="3"/>
+        <v>63</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
-      <c r="E77" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="E77" s="3"/>
       <c r="F77" s="3"/>
-      <c r="G77" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H77" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G77" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="H77" s="7"/>
+      <c r="I77" s="7"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B78" s="3"/>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
-      <c r="G78" s="6" t="s">
-        <v>55</v>
+        <v>64</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G78" s="14" t="s">
+        <v>207</v>
       </c>
       <c r="H78" s="7"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I78" s="7"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="B79" s="3"/>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
-      <c r="E79" s="3"/>
+      <c r="E79" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F79" s="3"/>
-      <c r="G79" s="6"/>
-      <c r="H79" s="7"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G79" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="H79" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="I79" s="7"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>149</v>
+        <v>28</v>
       </c>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
-      <c r="G80" s="6" t="s">
-        <v>55</v>
+      <c r="G80" s="17" t="s">
+        <v>270</v>
       </c>
       <c r="H80" s="7"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I80" s="7"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B81" s="3"/>
+        <v>95</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
-      <c r="G81" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="G81" s="6"/>
       <c r="H81" s="7"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81" s="7"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>30</v>
+        <v>148</v>
       </c>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
-      <c r="D82" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D82" s="3"/>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
-      <c r="G82" s="6" t="s">
-        <v>55</v>
+      <c r="G82" s="17" t="s">
+        <v>271</v>
       </c>
       <c r="H82" s="7"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I82" s="7"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
       <c r="F83" s="3"/>
-      <c r="G83" s="6" t="s">
-        <v>55</v>
+      <c r="G83" s="17" t="s">
+        <v>272</v>
       </c>
       <c r="H83" s="7"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I83" s="7"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B84" s="3"/>
       <c r="C84" s="3"/>
       <c r="D84" s="3" t="s">
         <v>55</v>
       </c>
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
-      <c r="G84" s="6" t="s">
-        <v>55</v>
+      <c r="G84" s="14" t="s">
+        <v>208</v>
       </c>
       <c r="H84" s="7"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I84" s="7"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
       <c r="E85" s="3"/>
-      <c r="F85" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G85" s="6" t="s">
-        <v>55</v>
+      <c r="F85" s="3"/>
+      <c r="G85" s="17" t="s">
+        <v>273</v>
       </c>
       <c r="H85" s="7"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I85" s="7"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>32</v>
+        <v>180</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C86" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
-      <c r="G86" s="6" t="s">
-        <v>55</v>
+      <c r="G86" s="14" t="s">
+        <v>209</v>
       </c>
       <c r="H86" s="7"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I86" s="7"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>33</v>
+        <v>107</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>55</v>
@@ -2691,67 +3109,75 @@
       <c r="C87" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D87" s="3"/>
+      <c r="D87" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E87" s="3"/>
-      <c r="F87" s="3"/>
-      <c r="G87" s="6" t="s">
-        <v>55</v>
+      <c r="F87" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G87" s="14" t="s">
+        <v>210</v>
       </c>
       <c r="H87" s="7"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I87" s="7"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B88" s="3"/>
-      <c r="C88" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
-      <c r="G88" s="6" t="s">
-        <v>55</v>
+      <c r="G88" s="17" t="s">
+        <v>274</v>
       </c>
       <c r="H88" s="7"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I88" s="7"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C89" s="3"/>
+      <c r="C89" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
-      <c r="G89" s="6" t="s">
-        <v>55</v>
+      <c r="G89" s="17" t="s">
+        <v>275</v>
       </c>
       <c r="H89" s="7"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="I89" s="7"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B90" s="3"/>
       <c r="C90" s="3"/>
-      <c r="D90" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D90" s="3"/>
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
-      <c r="G90" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H90" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G90" s="17" t="s">
+        <v>276</v>
+      </c>
+      <c r="H90" s="7"/>
+      <c r="I90" s="7"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>145</v>
+        <v>94</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>55</v>
@@ -2760,32 +3186,36 @@
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
       <c r="F91" s="3"/>
-      <c r="G91" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H91" s="7" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B92" s="3"/>
+      <c r="G91" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="H91" s="7"/>
+      <c r="I91" s="7"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C92" s="3"/>
-      <c r="D92" s="3"/>
+      <c r="D92" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E92" s="3"/>
       <c r="F92" s="3"/>
-      <c r="G92" s="6" t="s">
-        <v>55</v>
+      <c r="G92" s="14" t="s">
+        <v>211</v>
       </c>
       <c r="H92" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="I92" s="7"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>55</v>
@@ -2794,330 +3224,344 @@
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
-      <c r="G93" s="6" t="s">
-        <v>184</v>
+      <c r="G93" s="17" t="s">
+        <v>278</v>
       </c>
       <c r="H93" s="7" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="I93" s="7"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B94" s="3"/>
+      <c r="C94" s="3"/>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
       <c r="F94" s="3"/>
-      <c r="G94" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H94" s="7"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G94" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="H94" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="I94" s="7"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B95" s="3"/>
+        <v>163</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C95" s="3"/>
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
       <c r="F95" s="3"/>
-      <c r="G95" s="6"/>
-      <c r="H95" s="7"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G95" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="H95" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="I95" s="7"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B96" s="3"/>
-      <c r="C96" s="3"/>
-      <c r="D96" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D96" s="3"/>
       <c r="E96" s="3"/>
       <c r="F96" s="3"/>
-      <c r="G96" s="6" t="s">
-        <v>55</v>
+      <c r="G96" s="17" t="s">
+        <v>281</v>
       </c>
       <c r="H96" s="7"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I96" s="7"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
       <c r="D97" s="3"/>
       <c r="E97" s="3"/>
       <c r="F97" s="3"/>
-      <c r="G97" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="G97" s="6"/>
       <c r="H97" s="7"/>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I97" s="7"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D98" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="B98" s="3"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E98" s="3"/>
       <c r="F98" s="3"/>
-      <c r="G98" s="6" t="s">
-        <v>55</v>
+      <c r="G98" s="14" t="s">
+        <v>212</v>
       </c>
       <c r="H98" s="7"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I98" s="7"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
-      <c r="G99" s="6" t="s">
-        <v>55</v>
+      <c r="G99" s="17" t="s">
+        <v>282</v>
       </c>
       <c r="H99" s="7"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" s="10" t="s">
-        <v>120</v>
+      <c r="I99" s="7"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C100" s="3"/>
+      <c r="C100" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
-      <c r="G100" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H100" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G100" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="H100" s="7"/>
+      <c r="I100" s="7"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>157</v>
+        <v>37</v>
       </c>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
       <c r="F101" s="3"/>
-      <c r="G101" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="H101" s="7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>38</v>
+      <c r="G101" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="H101" s="7"/>
+      <c r="I101" s="7"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" s="10" t="s">
+        <v>120</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C102" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C102" s="3"/>
       <c r="D102" s="3"/>
       <c r="E102" s="3"/>
       <c r="F102" s="3"/>
-      <c r="G102" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H102" s="7"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G102" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="H102" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="I102" s="7"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="B103" s="3"/>
+      <c r="C103" s="3"/>
       <c r="D103" s="3"/>
       <c r="E103" s="3"/>
       <c r="F103" s="3"/>
-      <c r="G103" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H103" s="7"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G103" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="H103" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I103" s="7"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B104" s="3"/>
-      <c r="C104" s="3"/>
-      <c r="D104" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D104" s="3"/>
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
-      <c r="G104" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H104" s="7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G104" s="17" t="s">
+        <v>287</v>
+      </c>
+      <c r="H104" s="7"/>
+      <c r="I104" s="7"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B105" s="3"/>
-      <c r="C105" s="3"/>
-      <c r="D105" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D105" s="3"/>
       <c r="E105" s="3"/>
       <c r="F105" s="3"/>
-      <c r="G105" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H105" s="7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G105" s="17" t="s">
+        <v>288</v>
+      </c>
+      <c r="H105" s="7"/>
+      <c r="I105" s="7"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B106" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="B106" s="3"/>
       <c r="C106" s="3"/>
       <c r="D106" s="3" t="s">
         <v>55</v>
       </c>
       <c r="E106" s="3"/>
       <c r="F106" s="3"/>
-      <c r="G106" s="6" t="s">
-        <v>55</v>
+      <c r="G106" s="14" t="s">
+        <v>215</v>
       </c>
       <c r="H106" s="7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="I106" s="7"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>40</v>
+        <v>172</v>
       </c>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
-      <c r="D107" s="3"/>
-      <c r="E107" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D107" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E107" s="3"/>
       <c r="F107" s="3"/>
-      <c r="G107" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H107" s="7"/>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G107" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="H107" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="I107" s="7"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B108" s="3"/>
+        <v>167</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C108" s="3"/>
-      <c r="D108" s="3"/>
+      <c r="D108" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E108" s="3"/>
       <c r="F108" s="3"/>
-      <c r="G108" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H108" s="7"/>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G108" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="H108" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="I108" s="7"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
       <c r="D109" s="3"/>
-      <c r="E109" s="3"/>
+      <c r="E109" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F109" s="3"/>
-      <c r="G109" s="6"/>
-      <c r="H109" s="7" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A110" s="9" t="s">
-        <v>128</v>
+      <c r="G109" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="H109" s="7"/>
+      <c r="I109" s="7"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
       <c r="D110" s="3"/>
       <c r="E110" s="3"/>
       <c r="F110" s="3"/>
-      <c r="G110" s="6" t="s">
-        <v>55</v>
+      <c r="G110" s="17" t="s">
+        <v>290</v>
       </c>
       <c r="H110" s="7"/>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I110" s="7"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="B111" s="3"/>
+      <c r="C111" s="3"/>
       <c r="D111" s="3"/>
       <c r="E111" s="3"/>
       <c r="F111" s="3"/>
-      <c r="G111" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="G111" s="6"/>
       <c r="H111" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B112" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="I111" s="7"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B112" s="3"/>
       <c r="C112" s="3"/>
       <c r="D112" s="3"/>
       <c r="E112" s="3"/>
       <c r="F112" s="3"/>
-      <c r="G112" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="H112" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G112" s="6"/>
+      <c r="H112" s="7"/>
+      <c r="I112" s="7"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>55</v>
@@ -3125,99 +3569,107 @@
       <c r="C113" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D113" s="3"/>
+      <c r="D113" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E113" s="3"/>
       <c r="F113" s="3"/>
-      <c r="G113" s="6"/>
-      <c r="H113" s="7"/>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>43</v>
+      <c r="G113" s="18" t="s">
+        <v>232</v>
+      </c>
+      <c r="H113" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I113" s="7"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" s="10" t="s">
+        <v>88</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C114" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C114" s="3"/>
       <c r="D114" s="3"/>
       <c r="E114" s="3"/>
       <c r="F114" s="3"/>
-      <c r="G114" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H114" s="7"/>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G114" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="H114" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I114" s="7"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B115" s="3"/>
-      <c r="C115" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D115" s="3"/>
       <c r="E115" s="3"/>
       <c r="F115" s="3"/>
-      <c r="G115" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="G115" s="6"/>
       <c r="H115" s="7"/>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I115" s="7"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B116" s="3"/>
-      <c r="C116" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D116" s="3"/>
       <c r="E116" s="3"/>
       <c r="F116" s="3"/>
-      <c r="G116" s="6" t="s">
-        <v>55</v>
+      <c r="G116" s="17" t="s">
+        <v>230</v>
       </c>
       <c r="H116" s="7"/>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I116" s="7"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B117" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C117" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B117" s="3"/>
+      <c r="C117" s="3"/>
       <c r="D117" s="3"/>
-      <c r="E117" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F117" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G117" s="6" t="s">
-        <v>55</v>
+      <c r="E117" s="3"/>
+      <c r="F117" s="3"/>
+      <c r="G117" s="17" t="s">
+        <v>229</v>
       </c>
       <c r="H117" s="7"/>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I117" s="7"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B118" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B118" s="3"/>
       <c r="C118" s="3"/>
       <c r="D118" s="3"/>
       <c r="E118" s="3"/>
       <c r="F118" s="3"/>
-      <c r="G118" s="6" t="s">
-        <v>55</v>
+      <c r="G118" s="17" t="s">
+        <v>228</v>
       </c>
       <c r="H118" s="7"/>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I118" s="7"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>55</v>
@@ -3225,93 +3677,92 @@
       <c r="C119" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D119" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E119" s="3"/>
-      <c r="F119" s="3"/>
-      <c r="G119" s="6" t="s">
-        <v>55</v>
+      <c r="D119" s="3"/>
+      <c r="E119" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F119" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G119" s="17" t="s">
+        <v>227</v>
       </c>
       <c r="H119" s="7"/>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I119" s="7"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B120" s="3"/>
+        <v>110</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C120" s="3"/>
       <c r="D120" s="3"/>
       <c r="E120" s="3"/>
       <c r="F120" s="3"/>
-      <c r="G120" s="6" t="s">
-        <v>55</v>
+      <c r="G120" s="17" t="s">
+        <v>226</v>
       </c>
       <c r="H120" s="7"/>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I120" s="7"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>167</v>
+        <v>47</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C121" s="3"/>
-      <c r="D121" s="3"/>
+      <c r="C121" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E121" s="3"/>
       <c r="F121" s="3"/>
-      <c r="G121" s="6"/>
-      <c r="H121" s="7" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G121" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="H121" s="7"/>
+      <c r="I121" s="7"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B122" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C122" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="B122" s="3"/>
+      <c r="C122" s="3"/>
       <c r="D122" s="3"/>
       <c r="E122" s="3"/>
       <c r="F122" s="3"/>
-      <c r="G122" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H122" s="7" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G122" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="H122" s="7"/>
+      <c r="I122" s="7"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>49</v>
+        <v>165</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C123" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D123" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E123" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C123" s="3"/>
+      <c r="D123" s="3"/>
+      <c r="E123" s="3"/>
       <c r="F123" s="3"/>
-      <c r="G123" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="G123" s="6"/>
       <c r="H123" s="7" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+      <c r="I123" s="7"/>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>55</v>
@@ -3319,19 +3770,18 @@
       <c r="C124" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D124" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D124" s="3"/>
       <c r="E124" s="3"/>
       <c r="F124" s="3"/>
-      <c r="G124" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H124" s="7"/>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G124" s="6"/>
+      <c r="H124" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="I124" s="7"/>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B125" s="3" t="s">
         <v>55</v>
@@ -3339,93 +3789,109 @@
       <c r="C125" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D125" s="3"/>
-      <c r="E125" s="3"/>
+      <c r="D125" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E125" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F125" s="3"/>
-      <c r="G125" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H125" s="7"/>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G125" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="H125" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="I125" s="7"/>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B126" s="3"/>
-      <c r="C126" s="3"/>
-      <c r="D126" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E126" s="3"/>
       <c r="F126" s="3"/>
-      <c r="G126" s="6" t="s">
-        <v>55</v>
+      <c r="G126" s="14" t="s">
+        <v>218</v>
       </c>
       <c r="H126" s="7"/>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A127" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="B127" s="3"/>
-      <c r="C127" s="3"/>
+      <c r="I126" s="7"/>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D127" s="3"/>
       <c r="E127" s="3"/>
       <c r="F127" s="3"/>
-      <c r="G127" s="6"/>
+      <c r="G127" s="17" t="s">
+        <v>223</v>
+      </c>
       <c r="H127" s="7"/>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I127" s="7"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>66</v>
+        <v>112</v>
       </c>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
       <c r="D128" s="3"/>
-      <c r="E128" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="E128" s="3"/>
       <c r="F128" s="3"/>
-      <c r="G128" s="6" t="s">
-        <v>55</v>
+      <c r="G128" s="17" t="s">
+        <v>222</v>
       </c>
       <c r="H128" s="7"/>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A129" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B129" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C129" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="I128" s="7"/>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B129" s="3"/>
+      <c r="C129" s="3"/>
       <c r="D129" s="3"/>
       <c r="E129" s="3"/>
       <c r="F129" s="3"/>
       <c r="G129" s="6"/>
       <c r="H129" s="7"/>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A130" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B130" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C130" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="I129" s="7"/>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B130" s="3"/>
+      <c r="C130" s="3"/>
       <c r="D130" s="3"/>
-      <c r="E130" s="3"/>
+      <c r="E130" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F130" s="3"/>
-      <c r="G130" s="6" t="s">
-        <v>55</v>
+      <c r="G130" s="17" t="s">
+        <v>221</v>
       </c>
       <c r="H130" s="7"/>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I130" s="7"/>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>113</v>
+        <v>52</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>55</v>
@@ -3435,31 +3901,68 @@
       </c>
       <c r="D131" s="3"/>
       <c r="E131" s="3"/>
-      <c r="F131" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G131" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="F131" s="3"/>
+      <c r="G131" s="6"/>
       <c r="H131" s="7"/>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A133" s="10" t="s">
+      <c r="I131" s="7"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A132" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D132" s="3"/>
+      <c r="E132" s="3"/>
+      <c r="F132" s="3"/>
+      <c r="G132" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="H132" s="7"/>
+      <c r="I132" s="7"/>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D133" s="3"/>
+      <c r="E133" s="3"/>
+      <c r="F133" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G133" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="H133" s="7"/>
+      <c r="I133" s="7"/>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A135" s="10" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A134" s="8" t="s">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A136" s="8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A135" s="9" t="s">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A137" s="9" t="s">
         <v>129</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H131" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H133" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="G1" r:id="rId1" display="https://github.com/microsoft/winget-pkgs" xr:uid="{2C434A13-8B1C-492F-95C8-B89737A54984}"/>
     <hyperlink ref="A44" r:id="rId2" xr:uid="{5AAD9A6E-C562-4737-9662-CEC2B195962E}"/>

</xml_diff>

<commit_message>
docs: add chocolatey info
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\markus\projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE5B63B-2544-4CAB-807F-117E04AA4362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821E8E97-E254-427C-A986-67F8FBC84B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="292">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -621,9 +621,6 @@
     <t>neovim</t>
   </si>
   <si>
-    <t>Version in chocolatey (1.15) too old (current: 1.16)</t>
-  </si>
-  <si>
     <t>powershell-core</t>
   </si>
   <si>
@@ -651,9 +648,6 @@
     <t>Addon for ImageGlass; winget installs to %AppDataLocal%\Programs\ExifTool</t>
   </si>
   <si>
-    <t>winget migration todo</t>
-  </si>
-  <si>
     <t>sharkdp.fd</t>
   </si>
   <si>
@@ -693,9 +687,6 @@
     <t>Microsoft.WindowsTerminal</t>
   </si>
   <si>
-    <t>Installieren fehlgeschlagen mit Exitcode: 0x80070002 : Das System kann die angegebene Datei nicht finden.</t>
-  </si>
-  <si>
     <t>Neovim.Neovim</t>
   </si>
   <si>
@@ -960,7 +951,13 @@
     <t>Almico.SpeedFan</t>
   </si>
   <si>
-    <t>Installieren auf Schenker fehlgeschlagen mit Exitcode: 1603 (vermutlich wg. zu altem Acrobat Pro)</t>
+    <t>CD Burner / ISO Tool; Schenker: 404 not found</t>
+  </si>
+  <si>
+    <t>Muss vor Acrobat Pro installiert werden, sonst Konflikt.</t>
+  </si>
+  <si>
+    <t>Version in chocolatey (1.15) too old (current: 1.16) / winget: Installieren fehlgeschlagen mit Exitcode: 0x80070002 : Das System kann die angegebene Datei nicht finden.</t>
   </si>
 </sst>
 </file>
@@ -1106,7 +1103,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1132,16 +1129,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1491,11 +1485,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I138"/>
+  <dimension ref="A1:H138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H72" sqref="H72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1506,10 +1500,9 @@
     <col min="5" max="6" width="7.7109375" customWidth="1"/>
     <col min="7" max="7" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="70.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>54</v>
       </c>
@@ -1534,11 +1527,8 @@
       <c r="H1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>58</v>
       </c>
@@ -1557,13 +1547,12 @@
       <c r="F2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="14" t="s">
-        <v>181</v>
+      <c r="G2" s="13" t="s">
+        <v>180</v>
       </c>
       <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1576,11 +1565,10 @@
         <v>55</v>
       </c>
       <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G3" s="13"/>
+      <c r="H3" s="15"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>59</v>
       </c>
@@ -1599,15 +1587,14 @@
       <c r="F4" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G4" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="11" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G4" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1616,13 +1603,12 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="14" t="s">
-        <v>236</v>
+      <c r="G5" s="13" t="s">
+        <v>233</v>
       </c>
       <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>91</v>
       </c>
@@ -1633,13 +1619,12 @@
         <v>55</v>
       </c>
       <c r="F6" s="3"/>
-      <c r="G6" s="14" t="s">
-        <v>237</v>
+      <c r="G6" s="13" t="s">
+        <v>234</v>
       </c>
       <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>92</v>
       </c>
@@ -1652,9 +1637,8 @@
       <c r="F7" s="3"/>
       <c r="G7" s="6"/>
       <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>93</v>
       </c>
@@ -1667,9 +1651,8 @@
       <c r="F8" s="3"/>
       <c r="G8" s="6"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>60</v>
       </c>
@@ -1684,13 +1667,12 @@
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="14" t="s">
-        <v>183</v>
+      <c r="G9" s="13" t="s">
+        <v>182</v>
       </c>
       <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>100</v>
       </c>
@@ -1701,13 +1683,12 @@
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="14" t="s">
-        <v>184</v>
+      <c r="G10" s="13" t="s">
+        <v>183</v>
       </c>
       <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -1718,9 +1699,8 @@
       <c r="F11" s="3"/>
       <c r="G11" s="6"/>
       <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>114</v>
       </c>
@@ -1737,9 +1717,8 @@
       <c r="H12" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="I12" s="7"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>124</v>
       </c>
@@ -1752,9 +1731,8 @@
       <c r="H13" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="I13" s="7"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>125</v>
       </c>
@@ -1767,32 +1745,24 @@
       <c r="H14" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="14" t="s">
-        <v>238</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="I15" s="7"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G15" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>138</v>
       </c>
@@ -1807,9 +1777,8 @@
       <c r="H16" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="I16" s="7"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
@@ -1820,9 +1789,8 @@
       <c r="F17" s="3"/>
       <c r="G17" s="6"/>
       <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -1831,13 +1799,12 @@
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="14" t="s">
-        <v>239</v>
+      <c r="G18" s="13" t="s">
+        <v>236</v>
       </c>
       <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>101</v>
       </c>
@@ -1848,13 +1815,12 @@
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="14" t="s">
-        <v>240</v>
+      <c r="G19" s="13" t="s">
+        <v>237</v>
       </c>
       <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>140</v>
       </c>
@@ -1867,13 +1833,12 @@
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="14" t="s">
-        <v>185</v>
+      <c r="G20" s="13" t="s">
+        <v>184</v>
       </c>
       <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>133</v>
       </c>
@@ -1884,13 +1849,12 @@
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="14" t="s">
-        <v>241</v>
+      <c r="G21" s="13" t="s">
+        <v>238</v>
       </c>
       <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>173</v>
       </c>
@@ -1899,15 +1863,14 @@
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="14" t="s">
-        <v>242</v>
+      <c r="G22" s="13" t="s">
+        <v>239</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="I22" s="7"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>6</v>
       </c>
@@ -1922,9 +1885,8 @@
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -1935,9 +1897,8 @@
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>102</v>
       </c>
@@ -1950,13 +1911,12 @@
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="14" t="s">
-        <v>243</v>
+      <c r="G25" s="13" t="s">
+        <v>240</v>
       </c>
       <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>99</v>
       </c>
@@ -1967,15 +1927,14 @@
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="14" t="s">
-        <v>244</v>
+      <c r="G26" s="13" t="s">
+        <v>241</v>
       </c>
       <c r="H26" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="I26" s="7"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>8</v>
       </c>
@@ -1990,13 +1949,12 @@
       <c r="F27" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G27" s="14" t="s">
-        <v>245</v>
+      <c r="G27" s="13" t="s">
+        <v>242</v>
       </c>
       <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>150</v>
       </c>
@@ -2011,15 +1969,14 @@
       <c r="F28" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G28" s="14" t="s">
-        <v>186</v>
+      <c r="G28" s="13" t="s">
+        <v>185</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="I28" s="7"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>116</v>
       </c>
@@ -2032,15 +1989,14 @@
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="14" t="s">
-        <v>190</v>
+      <c r="G29" s="13" t="s">
+        <v>188</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="I29" s="7"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>9</v>
       </c>
@@ -2059,9 +2015,8 @@
         <v>55</v>
       </c>
       <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>10</v>
       </c>
@@ -2078,13 +2033,12 @@
         <v>55</v>
       </c>
       <c r="F31" s="3"/>
-      <c r="G31" s="14" t="s">
-        <v>191</v>
+      <c r="G31" s="13" t="s">
+        <v>189</v>
       </c>
       <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>111</v>
       </c>
@@ -2099,13 +2053,12 @@
       <c r="F32" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G32" s="14" t="s">
-        <v>224</v>
+      <c r="G32" s="13" t="s">
+        <v>221</v>
       </c>
       <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>67</v>
       </c>
@@ -2114,15 +2067,14 @@
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="14" t="s">
-        <v>246</v>
+      <c r="G33" s="13" t="s">
+        <v>243</v>
       </c>
       <c r="H33" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="I33" s="7"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>56</v>
       </c>
@@ -2135,15 +2087,14 @@
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
-      <c r="G34" s="14" t="s">
-        <v>192</v>
+      <c r="G34" s="13" t="s">
+        <v>190</v>
       </c>
       <c r="H34" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="I34" s="7"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>103</v>
       </c>
@@ -2154,15 +2105,14 @@
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
-      <c r="G35" s="14" t="s">
-        <v>193</v>
+      <c r="G35" s="13" t="s">
+        <v>191</v>
       </c>
       <c r="H35" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="I35" s="7"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>61</v>
       </c>
@@ -2177,13 +2127,12 @@
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
-      <c r="G36" s="14" t="s">
-        <v>194</v>
+      <c r="G36" s="13" t="s">
+        <v>192</v>
       </c>
       <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>11</v>
       </c>
@@ -2192,13 +2141,12 @@
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
-      <c r="G37" s="14" t="s">
-        <v>247</v>
+      <c r="G37" s="13" t="s">
+        <v>244</v>
       </c>
       <c r="H37" s="7"/>
-      <c r="I37" s="7"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>87</v>
       </c>
@@ -2211,15 +2159,14 @@
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="14" t="s">
-        <v>248</v>
+      <c r="G38" s="13" t="s">
+        <v>245</v>
       </c>
       <c r="H38" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="I38" s="13"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>12</v>
       </c>
@@ -2237,12 +2184,11 @@
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H39" s="7"/>
-      <c r="I39" s="13"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>13</v>
       </c>
@@ -2255,13 +2201,12 @@
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
-      <c r="G40" s="14" t="s">
-        <v>249</v>
+      <c r="G40" s="13" t="s">
+        <v>246</v>
       </c>
       <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
@@ -2272,9 +2217,8 @@
       <c r="F41" s="3"/>
       <c r="G41" s="6"/>
       <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>134</v>
       </c>
@@ -2283,15 +2227,14 @@
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
-      <c r="G42" s="14" t="s">
-        <v>250</v>
+      <c r="G42" s="13" t="s">
+        <v>247</v>
       </c>
       <c r="H42" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="I42" s="7"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>84</v>
       </c>
@@ -2304,9 +2247,8 @@
       <c r="H43" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="I43" s="7"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>15</v>
       </c>
@@ -2317,13 +2259,12 @@
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
-      <c r="G44" s="14" t="s">
-        <v>251</v>
+      <c r="G44" s="13" t="s">
+        <v>248</v>
       </c>
       <c r="H44" s="7"/>
-      <c r="I44" s="7"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
         <v>149</v>
       </c>
@@ -2336,15 +2277,14 @@
       <c r="F45" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G45" s="14" t="s">
-        <v>187</v>
+      <c r="G45" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="H45" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="I45" s="7"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>16</v>
       </c>
@@ -2359,15 +2299,14 @@
         <v>55</v>
       </c>
       <c r="F46" s="3"/>
-      <c r="G46" s="14" t="s">
-        <v>252</v>
+      <c r="G46" s="13" t="s">
+        <v>249</v>
       </c>
       <c r="H46" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="I46" s="7"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>90</v>
       </c>
@@ -2382,13 +2321,12 @@
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
-      <c r="G47" s="14" t="s">
-        <v>196</v>
+      <c r="G47" s="13" t="s">
+        <v>194</v>
       </c>
       <c r="H47" s="7"/>
-      <c r="I47" s="7"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>96</v>
       </c>
@@ -2399,15 +2337,14 @@
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
-      <c r="G48" s="14" t="s">
-        <v>253</v>
+      <c r="G48" s="13" t="s">
+        <v>250</v>
       </c>
       <c r="H48" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="I48" s="13"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>80</v>
       </c>
@@ -2418,15 +2355,14 @@
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
-      <c r="G49" s="14" t="s">
-        <v>255</v>
+      <c r="G49" s="13" t="s">
+        <v>252</v>
       </c>
       <c r="H49" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="I49" s="7"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>17</v>
       </c>
@@ -2437,13 +2373,12 @@
         <v>55</v>
       </c>
       <c r="F50" s="3"/>
-      <c r="G50" s="14" t="s">
-        <v>256</v>
+      <c r="G50" s="13" t="s">
+        <v>253</v>
       </c>
       <c r="H50" s="7"/>
-      <c r="I50" s="7"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>18</v>
       </c>
@@ -2458,9 +2393,8 @@
       <c r="F51" s="3"/>
       <c r="G51" s="6"/>
       <c r="H51" s="7"/>
-      <c r="I51" s="7"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>161</v>
       </c>
@@ -2473,13 +2407,12 @@
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
-      <c r="G52" s="14" t="s">
-        <v>197</v>
+      <c r="G52" s="13" t="s">
+        <v>195</v>
       </c>
       <c r="H52" s="7"/>
-      <c r="I52" s="7"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
         <v>19</v>
       </c>
@@ -2490,13 +2423,12 @@
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
-      <c r="G53" s="14" t="s">
-        <v>198</v>
+      <c r="G53" s="13" t="s">
+        <v>196</v>
       </c>
       <c r="H53" s="7"/>
-      <c r="I53" s="7"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>20</v>
       </c>
@@ -2511,15 +2443,14 @@
         <v>55</v>
       </c>
       <c r="F54" s="3"/>
-      <c r="G54" s="14" t="s">
-        <v>257</v>
+      <c r="G54" s="13" t="s">
+        <v>254</v>
       </c>
       <c r="H54" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="I54" s="7"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>62</v>
       </c>
@@ -2534,13 +2465,12 @@
       <c r="F55" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G55" s="14" t="s">
-        <v>258</v>
+      <c r="G55" s="13" t="s">
+        <v>255</v>
       </c>
       <c r="H55" s="7"/>
-      <c r="I55" s="7"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>162</v>
       </c>
@@ -2557,13 +2487,12 @@
       <c r="F56" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G56" s="14" t="s">
-        <v>199</v>
+      <c r="G56" s="13" t="s">
+        <v>197</v>
       </c>
       <c r="H56" s="7"/>
-      <c r="I56" s="7"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>21</v>
       </c>
@@ -2580,9 +2509,8 @@
       </c>
       <c r="G57" s="6"/>
       <c r="H57" s="7"/>
-      <c r="I57" s="7"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>86</v>
       </c>
@@ -2595,15 +2523,14 @@
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
-      <c r="G58" s="14" t="s">
-        <v>200</v>
+      <c r="G58" s="13" t="s">
+        <v>198</v>
       </c>
       <c r="H58" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="I58" s="7"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
         <v>22</v>
       </c>
@@ -2614,9 +2541,8 @@
       <c r="F59" s="3"/>
       <c r="G59" s="6"/>
       <c r="H59" s="7"/>
-      <c r="I59" s="7"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>136</v>
       </c>
@@ -2629,9 +2555,8 @@
       <c r="H60" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="I60" s="7"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>122</v>
       </c>
@@ -2640,15 +2565,14 @@
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
-      <c r="G61" s="14" t="s">
-        <v>259</v>
+      <c r="G61" s="13" t="s">
+        <v>256</v>
       </c>
       <c r="H61" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="I61" s="7"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="3" t="s">
         <v>55</v>
@@ -2659,13 +2583,12 @@
       </c>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
-      <c r="G62" s="15" t="s">
-        <v>235</v>
+      <c r="G62" s="14" t="s">
+        <v>232</v>
       </c>
       <c r="H62" s="7"/>
-      <c r="I62" s="7"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>77</v>
       </c>
@@ -2676,15 +2599,14 @@
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
-      <c r="G63" s="14" t="s">
-        <v>232</v>
+      <c r="G63" s="13" t="s">
+        <v>229</v>
       </c>
       <c r="H63" s="7"/>
-      <c r="I63" s="7"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>55</v>
@@ -2695,13 +2617,12 @@
       </c>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
-      <c r="G64" s="15" t="s">
-        <v>234</v>
+      <c r="G64" s="14" t="s">
+        <v>231</v>
       </c>
       <c r="H64" s="7"/>
-      <c r="I64" s="7"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>23</v>
       </c>
@@ -2716,9 +2637,8 @@
       <c r="F65" s="3"/>
       <c r="G65" s="6"/>
       <c r="H65" s="7"/>
-      <c r="I65" s="7"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>105</v>
       </c>
@@ -2727,15 +2647,14 @@
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
-      <c r="G66" s="14" t="s">
-        <v>260</v>
+      <c r="G66" s="13" t="s">
+        <v>257</v>
       </c>
       <c r="H66" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="I66" s="7"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>141</v>
       </c>
@@ -2744,15 +2663,14 @@
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
-      <c r="G67" s="14" t="s">
-        <v>261</v>
+      <c r="G67" s="13" t="s">
+        <v>258</v>
       </c>
       <c r="H67" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="I67" s="7"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>24</v>
       </c>
@@ -2761,13 +2679,12 @@
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
-      <c r="G68" s="14" t="s">
-        <v>262</v>
+      <c r="G68" s="13" t="s">
+        <v>259</v>
       </c>
       <c r="H68" s="7"/>
-      <c r="I68" s="7"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>25</v>
       </c>
@@ -2776,13 +2693,12 @@
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
-      <c r="G69" s="14" t="s">
-        <v>263</v>
+      <c r="G69" s="13" t="s">
+        <v>260</v>
       </c>
       <c r="H69" s="7"/>
-      <c r="I69" s="7"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>26</v>
       </c>
@@ -2795,13 +2711,12 @@
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
-      <c r="G70" s="14" t="s">
-        <v>264</v>
+      <c r="G70" s="13" t="s">
+        <v>261</v>
       </c>
       <c r="H70" s="7"/>
-      <c r="I70" s="7"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>108</v>
       </c>
@@ -2812,13 +2727,12 @@
       </c>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
-      <c r="G71" s="14" t="s">
-        <v>201</v>
+      <c r="G71" s="13" t="s">
+        <v>199</v>
       </c>
       <c r="H71" s="7"/>
-      <c r="I71" s="7"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>109</v>
       </c>
@@ -2830,16 +2744,13 @@
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
       <c r="G72" s="11" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H72" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="I72" s="11" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>76</v>
       </c>
@@ -2852,13 +2763,12 @@
       <c r="F73" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G73" s="14" t="s">
-        <v>265</v>
+      <c r="G73" s="13" t="s">
+        <v>262</v>
       </c>
       <c r="H73" s="7"/>
-      <c r="I73" s="7"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>81</v>
       </c>
@@ -2867,13 +2777,12 @@
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
-      <c r="G74" s="14" t="s">
-        <v>266</v>
+      <c r="G74" s="13" t="s">
+        <v>263</v>
       </c>
       <c r="H74" s="7"/>
-      <c r="I74" s="7"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
         <v>178</v>
       </c>
@@ -2886,13 +2795,12 @@
       </c>
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
-      <c r="G75" s="14" t="s">
-        <v>204</v>
+      <c r="G75" s="13" t="s">
+        <v>201</v>
       </c>
       <c r="H75" s="7"/>
-      <c r="I75" s="7"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>27</v>
       </c>
@@ -2905,13 +2813,12 @@
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
-      <c r="G76" s="14" t="s">
-        <v>267</v>
+      <c r="G76" s="13" t="s">
+        <v>264</v>
       </c>
       <c r="H76" s="7"/>
-      <c r="I76" s="7"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>63</v>
       </c>
@@ -2922,13 +2829,12 @@
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
-      <c r="G77" s="14" t="s">
-        <v>205</v>
+      <c r="G77" s="13" t="s">
+        <v>202</v>
       </c>
       <c r="H77" s="7"/>
-      <c r="I77" s="7"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>64</v>
       </c>
@@ -2947,13 +2853,12 @@
       <c r="F78" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G78" s="14" t="s">
-        <v>206</v>
+      <c r="G78" s="13" t="s">
+        <v>203</v>
       </c>
       <c r="H78" s="7"/>
-      <c r="I78" s="7"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>69</v>
       </c>
@@ -2964,15 +2869,14 @@
         <v>55</v>
       </c>
       <c r="F79" s="3"/>
-      <c r="G79" s="14" t="s">
-        <v>268</v>
+      <c r="G79" s="13" t="s">
+        <v>265</v>
       </c>
       <c r="H79" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="I79" s="7"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>28</v>
       </c>
@@ -2981,13 +2885,12 @@
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
-      <c r="G80" s="14" t="s">
-        <v>269</v>
+      <c r="G80" s="13" t="s">
+        <v>266</v>
       </c>
       <c r="H80" s="7"/>
-      <c r="I80" s="7"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>95</v>
       </c>
@@ -3000,9 +2903,8 @@
       <c r="F81" s="3"/>
       <c r="G81" s="6"/>
       <c r="H81" s="7"/>
-      <c r="I81" s="7"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>148</v>
       </c>
@@ -3011,13 +2913,12 @@
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
-      <c r="G82" s="14" t="s">
-        <v>270</v>
+      <c r="G82" s="13" t="s">
+        <v>267</v>
       </c>
       <c r="H82" s="7"/>
-      <c r="I82" s="7"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>29</v>
       </c>
@@ -3026,13 +2927,12 @@
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
       <c r="F83" s="3"/>
-      <c r="G83" s="14" t="s">
-        <v>271</v>
+      <c r="G83" s="13" t="s">
+        <v>268</v>
       </c>
       <c r="H83" s="7"/>
-      <c r="I83" s="7"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>30</v>
       </c>
@@ -3043,13 +2943,12 @@
       </c>
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
-      <c r="G84" s="14" t="s">
-        <v>207</v>
+      <c r="G84" s="13" t="s">
+        <v>204</v>
       </c>
       <c r="H84" s="7"/>
-      <c r="I84" s="7"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>31</v>
       </c>
@@ -3058,15 +2957,14 @@
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
-      <c r="G85" s="14" t="s">
-        <v>272</v>
+      <c r="G85" s="13" t="s">
+        <v>269</v>
       </c>
       <c r="H85" s="7"/>
-      <c r="I85" s="7"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>55</v>
@@ -3077,13 +2975,12 @@
       </c>
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
-      <c r="G86" s="14" t="s">
-        <v>208</v>
+      <c r="G86" s="13" t="s">
+        <v>205</v>
       </c>
       <c r="H86" s="7"/>
-      <c r="I86" s="7"/>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>107</v>
       </c>
@@ -3100,13 +2997,12 @@
       <c r="F87" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G87" s="14" t="s">
-        <v>209</v>
+      <c r="G87" s="13" t="s">
+        <v>206</v>
       </c>
       <c r="H87" s="7"/>
-      <c r="I87" s="7"/>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>32</v>
       </c>
@@ -3119,13 +3015,12 @@
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
-      <c r="G88" s="14" t="s">
-        <v>273</v>
+      <c r="G88" s="13" t="s">
+        <v>270</v>
       </c>
       <c r="H88" s="7"/>
-      <c r="I88" s="7"/>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>33</v>
       </c>
@@ -3138,13 +3033,12 @@
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
-      <c r="G89" s="14" t="s">
-        <v>274</v>
+      <c r="G89" s="13" t="s">
+        <v>271</v>
       </c>
       <c r="H89" s="7"/>
-      <c r="I89" s="7"/>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>65</v>
       </c>
@@ -3153,13 +3047,12 @@
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
-      <c r="G90" s="14" t="s">
-        <v>275</v>
+      <c r="G90" s="13" t="s">
+        <v>272</v>
       </c>
       <c r="H90" s="7"/>
-      <c r="I90" s="7"/>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>94</v>
       </c>
@@ -3170,13 +3063,12 @@
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
       <c r="F91" s="3"/>
-      <c r="G91" s="14" t="s">
-        <v>276</v>
+      <c r="G91" s="13" t="s">
+        <v>273</v>
       </c>
       <c r="H91" s="7"/>
-      <c r="I91" s="7"/>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="10" t="s">
         <v>118</v>
       </c>
@@ -3189,15 +3081,14 @@
       </c>
       <c r="E92" s="3"/>
       <c r="F92" s="3"/>
-      <c r="G92" s="14" t="s">
-        <v>210</v>
+      <c r="G92" s="13" t="s">
+        <v>207</v>
       </c>
       <c r="H92" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="I92" s="7"/>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>144</v>
       </c>
@@ -3208,15 +3099,14 @@
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
-      <c r="G93" s="14" t="s">
-        <v>277</v>
+      <c r="G93" s="13" t="s">
+        <v>274</v>
       </c>
       <c r="H93" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="I93" s="7"/>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>78</v>
       </c>
@@ -3225,15 +3115,14 @@
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
       <c r="F94" s="3"/>
-      <c r="G94" s="14" t="s">
-        <v>278</v>
+      <c r="G94" s="13" t="s">
+        <v>275</v>
       </c>
       <c r="H94" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="I94" s="7"/>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>163</v>
       </c>
@@ -3244,15 +3133,14 @@
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
       <c r="F95" s="3"/>
-      <c r="G95" s="14" t="s">
-        <v>279</v>
+      <c r="G95" s="13" t="s">
+        <v>276</v>
       </c>
       <c r="H95" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="I95" s="7"/>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>83</v>
       </c>
@@ -3261,13 +3149,12 @@
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
       <c r="F96" s="3"/>
-      <c r="G96" s="14" t="s">
-        <v>280</v>
+      <c r="G96" s="13" t="s">
+        <v>277</v>
       </c>
       <c r="H96" s="7"/>
-      <c r="I96" s="7"/>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>82</v>
       </c>
@@ -3278,9 +3165,8 @@
       <c r="F97" s="3"/>
       <c r="G97" s="6"/>
       <c r="H97" s="7"/>
-      <c r="I97" s="7"/>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>34</v>
       </c>
@@ -3291,13 +3177,12 @@
       </c>
       <c r="E98" s="3"/>
       <c r="F98" s="3"/>
-      <c r="G98" s="14" t="s">
-        <v>211</v>
+      <c r="G98" s="13" t="s">
+        <v>208</v>
       </c>
       <c r="H98" s="7"/>
-      <c r="I98" s="7"/>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>35</v>
       </c>
@@ -3306,15 +3191,14 @@
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
-      <c r="G99" s="14" t="s">
-        <v>281</v>
+      <c r="G99" s="13" t="s">
+        <v>278</v>
       </c>
       <c r="H99" s="7"/>
-      <c r="I99" s="7"/>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>55</v>
@@ -3323,13 +3207,12 @@
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
-      <c r="G100" s="14" t="s">
-        <v>291</v>
+      <c r="G100" s="13" t="s">
+        <v>288</v>
       </c>
       <c r="H100" s="7"/>
-      <c r="I100" s="7"/>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="10" t="s">
         <v>120</v>
       </c>
@@ -3340,15 +3223,14 @@
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
       <c r="F101" s="3"/>
-      <c r="G101" s="14" t="s">
-        <v>284</v>
+      <c r="G101" s="13" t="s">
+        <v>281</v>
       </c>
       <c r="H101" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="I101" s="7"/>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>36</v>
       </c>
@@ -3361,13 +3243,12 @@
       <c r="D102" s="3"/>
       <c r="E102" s="3"/>
       <c r="F102" s="3"/>
-      <c r="G102" s="14" t="s">
-        <v>282</v>
+      <c r="G102" s="13" t="s">
+        <v>279</v>
       </c>
       <c r="H102" s="7"/>
-      <c r="I102" s="7"/>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>37</v>
       </c>
@@ -3376,13 +3257,12 @@
       <c r="D103" s="3"/>
       <c r="E103" s="3"/>
       <c r="F103" s="3"/>
-      <c r="G103" s="14" t="s">
-        <v>283</v>
+      <c r="G103" s="13" t="s">
+        <v>280</v>
       </c>
       <c r="H103" s="7"/>
-      <c r="I103" s="7"/>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>155</v>
       </c>
@@ -3391,15 +3271,14 @@
       <c r="D104" s="3"/>
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
-      <c r="G104" s="14" t="s">
-        <v>285</v>
+      <c r="G104" s="13" t="s">
+        <v>282</v>
       </c>
       <c r="H104" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="I104" s="7"/>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>38</v>
       </c>
@@ -3412,13 +3291,12 @@
       <c r="D105" s="3"/>
       <c r="E105" s="3"/>
       <c r="F105" s="3"/>
-      <c r="G105" s="14" t="s">
-        <v>286</v>
+      <c r="G105" s="13" t="s">
+        <v>283</v>
       </c>
       <c r="H105" s="7"/>
-      <c r="I105" s="7"/>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>39</v>
       </c>
@@ -3431,13 +3309,12 @@
       <c r="D106" s="3"/>
       <c r="E106" s="3"/>
       <c r="F106" s="3"/>
-      <c r="G106" s="14" t="s">
-        <v>287</v>
+      <c r="G106" s="13" t="s">
+        <v>284</v>
       </c>
       <c r="H106" s="7"/>
-      <c r="I106" s="7"/>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>171</v>
       </c>
@@ -3448,15 +3325,14 @@
       </c>
       <c r="E107" s="3"/>
       <c r="F107" s="3"/>
-      <c r="G107" s="14" t="s">
-        <v>214</v>
+      <c r="G107" s="13" t="s">
+        <v>211</v>
       </c>
       <c r="H107" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="I107" s="7"/>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>172</v>
       </c>
@@ -3467,15 +3343,14 @@
       </c>
       <c r="E108" s="3"/>
       <c r="F108" s="3"/>
-      <c r="G108" s="14" t="s">
-        <v>212</v>
+      <c r="G108" s="13" t="s">
+        <v>209</v>
       </c>
       <c r="H108" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="I108" s="7"/>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>167</v>
       </c>
@@ -3488,15 +3363,14 @@
       </c>
       <c r="E109" s="3"/>
       <c r="F109" s="3"/>
-      <c r="G109" s="14" t="s">
-        <v>213</v>
+      <c r="G109" s="13" t="s">
+        <v>210</v>
       </c>
       <c r="H109" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="I109" s="7"/>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>40</v>
       </c>
@@ -3507,13 +3381,12 @@
         <v>55</v>
       </c>
       <c r="F110" s="3"/>
-      <c r="G110" s="14" t="s">
-        <v>288</v>
+      <c r="G110" s="13" t="s">
+        <v>285</v>
       </c>
       <c r="H110" s="7"/>
-      <c r="I110" s="7"/>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>41</v>
       </c>
@@ -3522,13 +3395,12 @@
       <c r="D111" s="3"/>
       <c r="E111" s="3"/>
       <c r="F111" s="3"/>
-      <c r="G111" s="14" t="s">
-        <v>289</v>
+      <c r="G111" s="13" t="s">
+        <v>286</v>
       </c>
       <c r="H111" s="7"/>
-      <c r="I111" s="7"/>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>68</v>
       </c>
@@ -3541,9 +3413,8 @@
       <c r="H112" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="I112" s="7"/>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="9" t="s">
         <v>128</v>
       </c>
@@ -3554,9 +3425,8 @@
       <c r="F113" s="3"/>
       <c r="G113" s="6"/>
       <c r="H113" s="7"/>
-      <c r="I113" s="7"/>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>74</v>
       </c>
@@ -3571,15 +3441,14 @@
       </c>
       <c r="E114" s="3"/>
       <c r="F114" s="3"/>
-      <c r="G114" s="15" t="s">
-        <v>231</v>
+      <c r="G114" s="14" t="s">
+        <v>228</v>
       </c>
       <c r="H114" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="I114" s="7"/>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="10" t="s">
         <v>88</v>
       </c>
@@ -3590,15 +3459,14 @@
       <c r="D115" s="3"/>
       <c r="E115" s="3"/>
       <c r="F115" s="3"/>
-      <c r="G115" s="14" t="s">
-        <v>230</v>
+      <c r="G115" s="13" t="s">
+        <v>227</v>
       </c>
       <c r="H115" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="I115" s="7"/>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>42</v>
       </c>
@@ -3613,9 +3481,8 @@
       <c r="F116" s="3"/>
       <c r="G116" s="6"/>
       <c r="H116" s="7"/>
-      <c r="I116" s="7"/>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>43</v>
       </c>
@@ -3628,13 +3495,12 @@
       <c r="D117" s="3"/>
       <c r="E117" s="3"/>
       <c r="F117" s="3"/>
-      <c r="G117" s="14" t="s">
-        <v>229</v>
+      <c r="G117" s="13" t="s">
+        <v>226</v>
       </c>
       <c r="H117" s="7"/>
-      <c r="I117" s="7"/>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>44</v>
       </c>
@@ -3643,13 +3509,12 @@
       <c r="D118" s="3"/>
       <c r="E118" s="3"/>
       <c r="F118" s="3"/>
-      <c r="G118" s="14" t="s">
-        <v>228</v>
+      <c r="G118" s="13" t="s">
+        <v>225</v>
       </c>
       <c r="H118" s="7"/>
-      <c r="I118" s="7"/>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>45</v>
       </c>
@@ -3658,13 +3523,12 @@
       <c r="D119" s="3"/>
       <c r="E119" s="3"/>
       <c r="F119" s="3"/>
-      <c r="G119" s="14" t="s">
-        <v>227</v>
+      <c r="G119" s="13" t="s">
+        <v>224</v>
       </c>
       <c r="H119" s="7"/>
-      <c r="I119" s="7"/>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>46</v>
       </c>
@@ -3681,13 +3545,12 @@
       <c r="F120" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G120" s="14" t="s">
-        <v>226</v>
+      <c r="G120" s="13" t="s">
+        <v>223</v>
       </c>
       <c r="H120" s="7"/>
-      <c r="I120" s="7"/>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>110</v>
       </c>
@@ -3698,13 +3561,12 @@
       <c r="D121" s="3"/>
       <c r="E121" s="3"/>
       <c r="F121" s="3"/>
-      <c r="G121" s="14" t="s">
-        <v>225</v>
+      <c r="G121" s="13" t="s">
+        <v>222</v>
       </c>
       <c r="H121" s="7"/>
-      <c r="I121" s="7"/>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>47</v>
       </c>
@@ -3719,13 +3581,12 @@
       </c>
       <c r="E122" s="3"/>
       <c r="F122" s="3"/>
-      <c r="G122" s="14" t="s">
-        <v>215</v>
+      <c r="G122" s="13" t="s">
+        <v>212</v>
       </c>
       <c r="H122" s="7"/>
-      <c r="I122" s="7"/>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>48</v>
       </c>
@@ -3734,13 +3595,12 @@
       <c r="D123" s="3"/>
       <c r="E123" s="3"/>
       <c r="F123" s="3"/>
-      <c r="G123" s="14" t="s">
-        <v>223</v>
+      <c r="G123" s="13" t="s">
+        <v>220</v>
       </c>
       <c r="H123" s="7"/>
-      <c r="I123" s="7"/>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>165</v>
       </c>
@@ -3755,9 +3615,8 @@
       <c r="H124" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="I124" s="7"/>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>73</v>
       </c>
@@ -3774,9 +3633,8 @@
       <c r="H125" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="I125" s="7"/>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>49</v>
       </c>
@@ -3793,15 +3651,14 @@
         <v>55</v>
       </c>
       <c r="F126" s="3"/>
-      <c r="G126" s="14" t="s">
-        <v>216</v>
+      <c r="G126" s="13" t="s">
+        <v>213</v>
       </c>
       <c r="H126" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="I126" s="7"/>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>50</v>
       </c>
@@ -3816,13 +3673,12 @@
       </c>
       <c r="E127" s="3"/>
       <c r="F127" s="3"/>
-      <c r="G127" s="14" t="s">
-        <v>217</v>
+      <c r="G127" s="13" t="s">
+        <v>214</v>
       </c>
       <c r="H127" s="7"/>
-      <c r="I127" s="7"/>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>51</v>
       </c>
@@ -3835,13 +3691,12 @@
       <c r="D128" s="3"/>
       <c r="E128" s="3"/>
       <c r="F128" s="3"/>
-      <c r="G128" s="14" t="s">
-        <v>222</v>
+      <c r="G128" s="13" t="s">
+        <v>219</v>
       </c>
       <c r="H128" s="7"/>
-      <c r="I128" s="7"/>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>112</v>
       </c>
@@ -3850,13 +3705,12 @@
       <c r="D129" s="3"/>
       <c r="E129" s="3"/>
       <c r="F129" s="3"/>
-      <c r="G129" s="14" t="s">
-        <v>221</v>
+      <c r="G129" s="13" t="s">
+        <v>218</v>
       </c>
       <c r="H129" s="7"/>
-      <c r="I129" s="7"/>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="8" t="s">
         <v>127</v>
       </c>
@@ -3867,9 +3721,8 @@
       <c r="F130" s="3"/>
       <c r="G130" s="6"/>
       <c r="H130" s="7"/>
-      <c r="I130" s="7"/>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>66</v>
       </c>
@@ -3880,13 +3733,12 @@
         <v>55</v>
       </c>
       <c r="F131" s="3"/>
-      <c r="G131" s="14" t="s">
-        <v>220</v>
+      <c r="G131" s="13" t="s">
+        <v>217</v>
       </c>
       <c r="H131" s="7"/>
-      <c r="I131" s="7"/>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>52</v>
       </c>
@@ -3901,9 +3753,8 @@
       <c r="F132" s="3"/>
       <c r="G132" s="6"/>
       <c r="H132" s="7"/>
-      <c r="I132" s="7"/>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="10" t="s">
         <v>53</v>
       </c>
@@ -3916,13 +3767,12 @@
       <c r="D133" s="3"/>
       <c r="E133" s="3"/>
       <c r="F133" s="3"/>
-      <c r="G133" s="14" t="s">
-        <v>219</v>
+      <c r="G133" s="13" t="s">
+        <v>216</v>
       </c>
       <c r="H133" s="7"/>
-      <c r="I133" s="7"/>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>113</v>
       </c>
@@ -3937,23 +3787,22 @@
       <c r="F134" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G134" s="14" t="s">
-        <v>218</v>
+      <c r="G134" s="13" t="s">
+        <v>215</v>
       </c>
       <c r="H134" s="7"/>
-      <c r="I134" s="7"/>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="10" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="9" t="s">
         <v>129</v>
       </c>

</xml_diff>

<commit_message>
feat: update installed software
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markus/Projects/wiki/Settings/Chocolatey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD60FD42-1FE3-C343-AE10-01A8A5A73126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F592440A-CBC7-E44B-8C6F-E560E84CD369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chocolatey" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Chocolatey!$A$1:$H$134</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Mac installed'!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Mac installed'!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="387">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -1201,9 +1201,6 @@
     <t>inkl. Macfuse</t>
   </si>
   <si>
-    <t>AdroidFileTransfer</t>
-  </si>
-  <si>
     <t>Drucker Treiber</t>
   </si>
   <si>
@@ -1235,6 +1232,18 @@
   </si>
   <si>
     <t>qView</t>
+  </si>
+  <si>
+    <t>OpenMTP</t>
+  </si>
+  <si>
+    <t>Alternative zu AndroidFileTransfer</t>
+  </si>
+  <si>
+    <t>AndroidFileTransfer</t>
+  </si>
+  <si>
+    <t>Aktiv</t>
   </si>
 </sst>
 </file>
@@ -4495,273 +4504,382 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F93F60-305A-704A-9194-4387AC0BEE7B}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B30" sqref="B30:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" customWidth="1"/>
-    <col min="3" max="3" width="66.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>365</v>
       </c>
       <c r="B1" s="17" t="s">
+        <v>386</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>366</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="D1" s="17" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>327</v>
       </c>
       <c r="B2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C2" t="s">
         <v>369</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>319</v>
       </c>
       <c r="B3" t="s">
+        <v>292</v>
+      </c>
+      <c r="C3" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>356</v>
       </c>
       <c r="B4" t="s">
+        <v>292</v>
+      </c>
+      <c r="C4" t="s">
         <v>369</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>358</v>
       </c>
       <c r="B5" t="s">
+        <v>292</v>
+      </c>
+      <c r="C5" t="s">
         <v>369</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>348</v>
       </c>
       <c r="B6" t="s">
+        <v>292</v>
+      </c>
+      <c r="C6" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>61</v>
       </c>
       <c r="B7" t="s">
+        <v>292</v>
+      </c>
+      <c r="C7" t="s">
         <v>369</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>361</v>
       </c>
       <c r="B8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C8" t="s">
         <v>369</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>312</v>
       </c>
       <c r="B9" t="s">
+        <v>292</v>
+      </c>
+      <c r="C9" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>363</v>
       </c>
       <c r="B10" t="s">
+        <v>292</v>
+      </c>
+      <c r="C10" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>364</v>
       </c>
       <c r="B11" t="s">
+        <v>292</v>
+      </c>
+      <c r="C11" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>90</v>
       </c>
       <c r="B12" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>52</v>
       </c>
       <c r="B13" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>368</v>
       </c>
       <c r="B14" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>39</v>
       </c>
       <c r="B15" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>133</v>
       </c>
       <c r="B16" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>370</v>
       </c>
       <c r="B17" t="s">
+        <v>292</v>
+      </c>
+      <c r="C17" t="s">
         <v>369</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>372</v>
+        <v>385</v>
       </c>
       <c r="B18" t="s">
+        <v>301</v>
+      </c>
+      <c r="C18" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>350</v>
       </c>
       <c r="B19" t="s">
+        <v>292</v>
+      </c>
+      <c r="C19" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>353</v>
       </c>
       <c r="B20" t="s">
+        <v>292</v>
+      </c>
+      <c r="C20" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>372</v>
+      </c>
+      <c r="B21" t="s">
+        <v>292</v>
+      </c>
+      <c r="C21" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>373</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
+        <v>292</v>
+      </c>
+      <c r="C22" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>375</v>
+      </c>
+      <c r="B23" t="s">
+        <v>292</v>
+      </c>
+      <c r="C23" t="s">
+        <v>369</v>
+      </c>
+      <c r="D23" t="s">
         <v>374</v>
       </c>
-      <c r="B22" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>376</v>
+      </c>
+      <c r="B24" t="s">
+        <v>292</v>
+      </c>
+      <c r="C24" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>376</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>377</v>
+      </c>
+      <c r="B25" t="s">
+        <v>292</v>
+      </c>
+      <c r="C25" t="s">
         <v>369</v>
       </c>
-      <c r="C23" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>377</v>
-      </c>
-      <c r="B24" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="D25" t="s">
         <v>378</v>
       </c>
-      <c r="B25" t="s">
-        <v>369</v>
-      </c>
-      <c r="C25" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>305</v>
       </c>
       <c r="B26" t="s">
+        <v>292</v>
+      </c>
+      <c r="C26" t="s">
         <v>369</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="B27" t="s">
+        <v>292</v>
+      </c>
+      <c r="C27" t="s">
+        <v>301</v>
+      </c>
+      <c r="D27" t="s">
         <v>381</v>
       </c>
-      <c r="B27" t="s">
-        <v>301</v>
-      </c>
-      <c r="C27" t="s">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
+        <v>292</v>
+      </c>
+      <c r="C28" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>383</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
+        <v>292</v>
+      </c>
+      <c r="C29" t="s">
+        <v>292</v>
+      </c>
+      <c r="D29" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" t="s">
+        <v>292</v>
+      </c>
+      <c r="C30" t="s">
         <v>292</v>
       </c>
     </row>

</xml_diff>

<commit_message>
docs: add Affinity as alternative
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markus/Projects/wiki/Settings/Chocolatey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F592440A-CBC7-E44B-8C6F-E560E84CD369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9884DBD4-E96E-074D-96AA-7ABC7BCE74E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chocolatey" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="388">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -982,9 +982,6 @@
     <t>Adobe Creative Suite 4 Design Standard</t>
   </si>
   <si>
-    <t>$$$</t>
-  </si>
-  <si>
     <t>AOMEI Backupper</t>
   </si>
   <si>
@@ -1244,6 +1241,12 @@
   </si>
   <si>
     <t>Aktiv</t>
+  </si>
+  <si>
+    <t>Affinity</t>
+  </si>
+  <si>
+    <t>180€ für Designer (Vektor), Photo (Pixel), Publisher</t>
   </si>
 </sst>
 </file>
@@ -4088,8 +4091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4129,24 +4132,27 @@
       <c r="B3" t="s">
         <v>292</v>
       </c>
+      <c r="C3" t="s">
+        <v>386</v>
+      </c>
       <c r="D3" t="s">
-        <v>299</v>
+        <v>387</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>299</v>
+      </c>
+      <c r="B4" t="s">
         <v>300</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>301</v>
-      </c>
-      <c r="C4" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B5" t="s">
         <v>292</v>
@@ -4154,21 +4160,21 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>303</v>
+      </c>
+      <c r="B6" t="s">
+        <v>300</v>
+      </c>
+      <c r="C6" t="s">
         <v>304</v>
       </c>
-      <c r="B6" t="s">
-        <v>301</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>305</v>
-      </c>
-      <c r="D6" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B7" t="s">
         <v>292</v>
@@ -4176,7 +4182,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B8" t="s">
         <v>292</v>
@@ -4184,7 +4190,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B9" t="s">
         <v>292</v>
@@ -4192,15 +4198,15 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B11" t="s">
         <v>292</v>
@@ -4208,7 +4214,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B12" t="s">
         <v>292</v>
@@ -4216,23 +4222,23 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>312</v>
+      </c>
+      <c r="B13" t="s">
         <v>313</v>
-      </c>
-      <c r="B13" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B14" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B15" t="s">
         <v>292</v>
@@ -4240,7 +4246,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B16" t="s">
         <v>292</v>
@@ -4248,7 +4254,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B17" t="s">
         <v>292</v>
@@ -4256,7 +4262,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B18" t="s">
         <v>292</v>
@@ -4264,26 +4270,26 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>319</v>
+      </c>
+      <c r="B19" t="s">
         <v>320</v>
-      </c>
-      <c r="B19" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>321</v>
+      </c>
+      <c r="B20" t="s">
+        <v>292</v>
+      </c>
+      <c r="D20" t="s">
         <v>322</v>
-      </c>
-      <c r="B20" t="s">
-        <v>292</v>
-      </c>
-      <c r="D20" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B21" t="s">
         <v>292</v>
@@ -4291,7 +4297,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B22" t="s">
         <v>292</v>
@@ -4299,7 +4305,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B23" t="s">
         <v>292</v>
@@ -4307,7 +4313,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B24" t="s">
         <v>292</v>
@@ -4315,7 +4321,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B25" t="s">
         <v>292</v>
@@ -4323,7 +4329,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B26" t="s">
         <v>292</v>
@@ -4331,21 +4337,21 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>329</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>300</v>
+      </c>
+      <c r="C27" t="s">
         <v>330</v>
       </c>
-      <c r="B27" s="16" t="s">
-        <v>301</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>331</v>
-      </c>
-      <c r="D27" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B28" t="s">
         <v>292</v>
@@ -4353,18 +4359,18 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>333</v>
+      </c>
+      <c r="B29" t="s">
+        <v>300</v>
+      </c>
+      <c r="C29" t="s">
         <v>334</v>
-      </c>
-      <c r="B29" t="s">
-        <v>301</v>
-      </c>
-      <c r="C29" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B30" t="s">
         <v>292</v>
@@ -4372,7 +4378,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B31" t="s">
         <v>292</v>
@@ -4380,54 +4386,54 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>337</v>
+      </c>
+      <c r="B32" t="s">
+        <v>300</v>
+      </c>
+      <c r="C32" t="s">
         <v>338</v>
-      </c>
-      <c r="B32" t="s">
-        <v>301</v>
-      </c>
-      <c r="C32" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>339</v>
+      </c>
+      <c r="B33" t="s">
+        <v>300</v>
+      </c>
+      <c r="C33" t="s">
         <v>340</v>
       </c>
-      <c r="B33" t="s">
-        <v>301</v>
-      </c>
-      <c r="C33" t="s">
-        <v>341</v>
-      </c>
       <c r="D33" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>341</v>
+      </c>
+      <c r="B34" t="s">
+        <v>300</v>
+      </c>
+      <c r="C34" t="s">
         <v>342</v>
-      </c>
-      <c r="B34" t="s">
-        <v>301</v>
-      </c>
-      <c r="C34" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>343</v>
+      </c>
+      <c r="B35" t="s">
+        <v>300</v>
+      </c>
+      <c r="C35" t="s">
         <v>344</v>
-      </c>
-      <c r="B35" t="s">
-        <v>301</v>
-      </c>
-      <c r="C35" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B36" t="s">
         <v>292</v>
@@ -4435,7 +4441,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B37" t="s">
         <v>292</v>
@@ -4443,7 +4449,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B38" t="s">
         <v>292</v>
@@ -4451,15 +4457,15 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B39" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B40" t="s">
         <v>292</v>
@@ -4467,7 +4473,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B41" t="s">
         <v>292</v>
@@ -4475,7 +4481,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B42" t="s">
         <v>292</v>
@@ -4483,7 +4489,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B43" t="s">
         <v>292</v>
@@ -4491,10 +4497,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B44" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -4506,8 +4512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F93F60-305A-704A-9194-4387AC0BEE7B}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:C30"/>
+    <sheetView zoomScale="156" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4519,80 +4525,80 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
+        <v>364</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>385</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>365</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>386</v>
-      </c>
-      <c r="C1" s="17" t="s">
+      <c r="D1" s="17" t="s">
         <v>366</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B2" t="s">
         <v>292</v>
       </c>
       <c r="C2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B3" t="s">
         <v>292</v>
       </c>
       <c r="C3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B4" t="s">
+        <v>292</v>
+      </c>
+      <c r="C4" t="s">
+        <v>368</v>
+      </c>
+      <c r="D4" t="s">
         <v>356</v>
-      </c>
-      <c r="B4" t="s">
-        <v>292</v>
-      </c>
-      <c r="C4" t="s">
-        <v>369</v>
-      </c>
-      <c r="D4" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>357</v>
+      </c>
+      <c r="B5" t="s">
+        <v>292</v>
+      </c>
+      <c r="C5" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5" t="s">
         <v>358</v>
-      </c>
-      <c r="B5" t="s">
-        <v>292</v>
-      </c>
-      <c r="C5" t="s">
-        <v>369</v>
-      </c>
-      <c r="D5" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B6" t="s">
         <v>292</v>
       </c>
       <c r="C6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -4603,57 +4609,57 @@
         <v>292</v>
       </c>
       <c r="C7" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D7" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>360</v>
+      </c>
+      <c r="B8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C8" t="s">
+        <v>368</v>
+      </c>
+      <c r="D8" t="s">
         <v>361</v>
-      </c>
-      <c r="B8" t="s">
-        <v>292</v>
-      </c>
-      <c r="C8" t="s">
-        <v>369</v>
-      </c>
-      <c r="D8" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B9" t="s">
         <v>292</v>
       </c>
       <c r="C9" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B10" t="s">
         <v>292</v>
       </c>
       <c r="C10" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B11" t="s">
         <v>292</v>
       </c>
       <c r="C11" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -4680,7 +4686,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B14" t="s">
         <v>292</v>
@@ -4713,143 +4719,143 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>369</v>
+      </c>
+      <c r="B17" t="s">
+        <v>292</v>
+      </c>
+      <c r="C17" t="s">
+        <v>368</v>
+      </c>
+      <c r="D17" t="s">
         <v>370</v>
-      </c>
-      <c r="B17" t="s">
-        <v>292</v>
-      </c>
-      <c r="C17" t="s">
-        <v>369</v>
-      </c>
-      <c r="D17" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B18" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B19" t="s">
         <v>292</v>
       </c>
       <c r="C19" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B20" t="s">
         <v>292</v>
       </c>
       <c r="C20" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B21" t="s">
         <v>292</v>
       </c>
       <c r="C21" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B22" t="s">
         <v>292</v>
       </c>
       <c r="C22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B23" t="s">
         <v>292</v>
       </c>
       <c r="C23" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D23" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B24" t="s">
         <v>292</v>
       </c>
       <c r="C24" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>376</v>
+      </c>
+      <c r="B25" t="s">
+        <v>292</v>
+      </c>
+      <c r="C25" t="s">
+        <v>368</v>
+      </c>
+      <c r="D25" t="s">
         <v>377</v>
-      </c>
-      <c r="B25" t="s">
-        <v>292</v>
-      </c>
-      <c r="C25" t="s">
-        <v>369</v>
-      </c>
-      <c r="D25" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B26" t="s">
         <v>292</v>
       </c>
       <c r="C26" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D26" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>379</v>
+      </c>
+      <c r="B27" t="s">
+        <v>292</v>
+      </c>
+      <c r="C27" t="s">
+        <v>300</v>
+      </c>
+      <c r="D27" t="s">
         <v>380</v>
-      </c>
-      <c r="B27" t="s">
-        <v>292</v>
-      </c>
-      <c r="C27" t="s">
-        <v>301</v>
-      </c>
-      <c r="D27" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B28" t="s">
         <v>292</v>
@@ -4860,16 +4866,16 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>382</v>
+      </c>
+      <c r="B29" t="s">
+        <v>292</v>
+      </c>
+      <c r="C29" t="s">
+        <v>292</v>
+      </c>
+      <c r="D29" t="s">
         <v>383</v>
-      </c>
-      <c r="B29" t="s">
-        <v>292</v>
-      </c>
-      <c r="C29" t="s">
-        <v>292</v>
-      </c>
-      <c r="D29" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
feat: add Maccy settings
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markus/Projects/wiki/Settings/Chocolatey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9884DBD4-E96E-074D-96AA-7ABC7BCE74E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7735A8D8-C386-3D49-B985-826B8F508C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="25600" windowHeight="25380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chocolatey" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="390">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -1247,6 +1247,12 @@
   </si>
   <si>
     <t>180€ für Designer (Vektor), Photo (Pixel), Publisher</t>
+  </si>
+  <si>
+    <t>maccy</t>
+  </si>
+  <si>
+    <t>Multiclipboard</t>
   </si>
 </sst>
 </file>
@@ -4091,7 +4097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -4510,10 +4516,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F93F60-305A-704A-9194-4387AC0BEE7B}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView zoomScale="156" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4889,7 +4895,22 @@
         <v>292</v>
       </c>
     </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>388</v>
+      </c>
+      <c r="B31" t="s">
+        <v>292</v>
+      </c>
+      <c r="C31" t="s">
+        <v>292</v>
+      </c>
+      <c r="D31" t="s">
+        <v>389</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: update MacOs installation
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markus/Projects/wiki/Settings/Chocolatey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7735A8D8-C386-3D49-B985-826B8F508C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93194602-8700-8A40-9B44-AA93B299914D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="25600" windowHeight="25380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-17280" yWindow="15860" windowWidth="17280" windowHeight="21580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chocolatey" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="399">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -1253,6 +1253,33 @@
   </si>
   <si>
     <t>Multiclipboard</t>
+  </si>
+  <si>
+    <t>htop</t>
+  </si>
+  <si>
+    <t>whisky</t>
+  </si>
+  <si>
+    <t>Heroic Games Launcher</t>
+  </si>
+  <si>
+    <t>https://heroicgameslauncher.com/downloads (Epic, GOG, Amazon)</t>
+  </si>
+  <si>
+    <t>Wine UI (Steam)</t>
+  </si>
+  <si>
+    <t>https://www.golem.de/news/tools-fuer-das-game-porting-toolkit-windows-games-auf-dem-mac-spielen-2401-180913-3.html</t>
+  </si>
+  <si>
+    <t>Snap</t>
+  </si>
+  <si>
+    <t>App Store</t>
+  </si>
+  <si>
+    <t>pcloud</t>
   </si>
 </sst>
 </file>
@@ -1411,7 +1438,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1446,6 +1473,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
@@ -4516,10 +4544,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F93F60-305A-704A-9194-4387AC0BEE7B}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="156" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4909,7 +4937,82 @@
         <v>389</v>
       </c>
     </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>391</v>
+      </c>
+      <c r="B32" t="s">
+        <v>292</v>
+      </c>
+      <c r="C32" t="s">
+        <v>292</v>
+      </c>
+      <c r="D32" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>392</v>
+      </c>
+      <c r="B33" t="s">
+        <v>292</v>
+      </c>
+      <c r="C33" t="s">
+        <v>368</v>
+      </c>
+      <c r="D33" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>396</v>
+      </c>
+      <c r="B34" t="s">
+        <v>292</v>
+      </c>
+      <c r="C34" t="s">
+        <v>368</v>
+      </c>
+      <c r="D34" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>390</v>
+      </c>
+      <c r="B35" t="s">
+        <v>292</v>
+      </c>
+      <c r="C35" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>398</v>
+      </c>
+      <c r="B36" t="s">
+        <v>292</v>
+      </c>
+      <c r="C36" t="s">
+        <v>300</v>
+      </c>
+      <c r="D36" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="18" t="s">
+        <v>395</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A38" r:id="rId1" xr:uid="{15511904-BAF9-6A4E-AF89-D7B8BAEF100F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: update MacOs apps
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markus/Projects/wiki/Settings/Chocolatey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93194602-8700-8A40-9B44-AA93B299914D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E98881-70E0-2D40-BC1C-FB2AA48CC511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-17280" yWindow="15860" windowWidth="17280" windowHeight="21580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,19 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Chocolatey!$A$1:$H$134</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Mac installed'!$A$1:$D$1</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -4125,7 +4137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="150" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat: unify deletion shortcuts
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markus/Projects/wiki/Settings/Chocolatey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC1085C-7668-7544-9F22-3C10A8353788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F76868C-FB9E-E242-BF99-A29251E53681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="401">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -1292,6 +1292,12 @@
   </si>
   <si>
     <t>App Store (Progamme im Dock mit Shortcuts starten)</t>
+  </si>
+  <si>
+    <t>npm</t>
+  </si>
+  <si>
+    <t>WhatsApp</t>
   </si>
 </sst>
 </file>
@@ -4556,10 +4562,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F93F60-305A-704A-9194-4387AC0BEE7B}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="B38" sqref="B38:C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5016,14 +5022,36 @@
         <v>380</v>
       </c>
     </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>399</v>
+      </c>
+      <c r="B37" t="s">
+        <v>292</v>
+      </c>
+      <c r="C37" t="s">
+        <v>292</v>
+      </c>
+    </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="18" t="s">
+      <c r="A38" t="s">
+        <v>400</v>
+      </c>
+      <c r="B38" t="s">
+        <v>292</v>
+      </c>
+      <c r="C38" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="18" t="s">
         <v>395</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A38" r:id="rId1" xr:uid="{15511904-BAF9-6A4E-AF89-D7B8BAEF100F}"/>
+    <hyperlink ref="A40" r:id="rId1" xr:uid="{15511904-BAF9-6A4E-AF89-D7B8BAEF100F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
feat: install openssh on macOS
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markus/Projects/wiki/Settings/Chocolatey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F76868C-FB9E-E242-BF99-A29251E53681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACDAED8-92A4-3E40-B26E-81F7D7A04D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="404">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -1298,6 +1298,15 @@
   </si>
   <si>
     <t>WhatsApp</t>
+  </si>
+  <si>
+    <t>rsync</t>
+  </si>
+  <si>
+    <t>openssh</t>
+  </si>
+  <si>
+    <t>necessary for checking the return value in sync job</t>
   </si>
 </sst>
 </file>
@@ -4562,10 +4571,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F93F60-305A-704A-9194-4387AC0BEE7B}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38:C38"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5044,14 +5053,39 @@
         <v>292</v>
       </c>
     </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>401</v>
+      </c>
+      <c r="B39" t="s">
+        <v>292</v>
+      </c>
+      <c r="C39" t="s">
+        <v>292</v>
+      </c>
+    </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="18" t="s">
+      <c r="A40" t="s">
+        <v>402</v>
+      </c>
+      <c r="B40" t="s">
+        <v>292</v>
+      </c>
+      <c r="C40" t="s">
+        <v>292</v>
+      </c>
+      <c r="D40" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="18" t="s">
         <v>395</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A40" r:id="rId1" xr:uid="{15511904-BAF9-6A4E-AF89-D7B8BAEF100F}"/>
+    <hyperlink ref="A42" r:id="rId1" xr:uid="{15511904-BAF9-6A4E-AF89-D7B8BAEF100F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
docs: update brew installed software
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markus/Projects/wiki/Settings/Chocolatey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACDAED8-92A4-3E40-B26E-81F7D7A04D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A2C3CD-23C8-6946-9E07-92E265406B93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chocolatey" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="409">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -1177,18 +1177,12 @@
     <t>Durch Aufruf im Terminal</t>
   </si>
   <si>
-    <t>VS Code</t>
-  </si>
-  <si>
     <t>https://code.visualstudio.com/docs/setup/mac#_launching-from-the-command-line</t>
   </si>
   <si>
     <t>iTerm2</t>
   </si>
   <si>
-    <t>Acrobat Reader</t>
-  </si>
-  <si>
     <t>Package</t>
   </si>
   <si>
@@ -1201,15 +1195,9 @@
     <t>nextcloud</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>VeraCrypt</t>
   </si>
   <si>
-    <t>inkl. Macfuse</t>
-  </si>
-  <si>
     <t>Drucker Treiber</t>
   </si>
   <si>
@@ -1222,9 +1210,6 @@
     <t>IJ Scan Utility</t>
   </si>
   <si>
-    <t>Logi Options+</t>
-  </si>
-  <si>
     <t>Ukelele</t>
   </si>
   <si>
@@ -1249,9 +1234,6 @@
     <t>Alternative zu AndroidFileTransfer</t>
   </si>
   <si>
-    <t>AndroidFileTransfer</t>
-  </si>
-  <si>
     <t>Aktiv</t>
   </si>
   <si>
@@ -1307,6 +1289,39 @@
   </si>
   <si>
     <t>necessary for checking the return value in sync job</t>
+  </si>
+  <si>
+    <t>visual-studio-code</t>
+  </si>
+  <si>
+    <t>google-chrome</t>
+  </si>
+  <si>
+    <t>adobe-acrobat-reader</t>
+  </si>
+  <si>
+    <t>zus. Macfuse</t>
+  </si>
+  <si>
+    <t>OpenMTP ist besser und wird gepflegt</t>
+  </si>
+  <si>
+    <t>epic-games</t>
+  </si>
+  <si>
+    <t>android-file-transfer</t>
+  </si>
+  <si>
+    <t>logi-options-plus</t>
+  </si>
+  <si>
+    <t>(✅)</t>
+  </si>
+  <si>
+    <t>05.04.2024: brew installation currently broken; installed manually</t>
+  </si>
+  <si>
+    <t>karabiner-elements</t>
   </si>
 </sst>
 </file>
@@ -4152,8 +4167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4194,10 +4209,10 @@
         <v>292</v>
       </c>
       <c r="C3" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="D3" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4574,7 +4589,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4586,16 +4601,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>379</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>363</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>364</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>385</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>365</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4606,7 +4621,7 @@
         <v>292</v>
       </c>
       <c r="C2" t="s">
-        <v>368</v>
+        <v>292</v>
       </c>
       <c r="D2" t="s">
         <v>354</v>
@@ -4620,7 +4635,7 @@
         <v>292</v>
       </c>
       <c r="C3" t="s">
-        <v>368</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4631,7 +4646,7 @@
         <v>292</v>
       </c>
       <c r="C4" t="s">
-        <v>368</v>
+        <v>300</v>
       </c>
       <c r="D4" t="s">
         <v>356</v>
@@ -4645,7 +4660,7 @@
         <v>292</v>
       </c>
       <c r="C5" t="s">
-        <v>368</v>
+        <v>292</v>
       </c>
       <c r="D5" t="s">
         <v>358</v>
@@ -4659,7 +4674,7 @@
         <v>292</v>
       </c>
       <c r="C6" t="s">
-        <v>368</v>
+        <v>292</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -4670,7 +4685,7 @@
         <v>292</v>
       </c>
       <c r="C7" t="s">
-        <v>368</v>
+        <v>292</v>
       </c>
       <c r="D7" t="s">
         <v>359</v>
@@ -4678,49 +4693,49 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>398</v>
+      </c>
+      <c r="B8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C8" t="s">
+        <v>292</v>
+      </c>
+      <c r="D8" t="s">
         <v>360</v>
-      </c>
-      <c r="B8" t="s">
-        <v>292</v>
-      </c>
-      <c r="C8" t="s">
-        <v>368</v>
-      </c>
-      <c r="D8" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>311</v>
+        <v>399</v>
       </c>
       <c r="B9" t="s">
         <v>292</v>
       </c>
       <c r="C9" t="s">
-        <v>368</v>
+        <v>292</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B10" t="s">
         <v>292</v>
       </c>
       <c r="C10" t="s">
-        <v>368</v>
+        <v>292</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>363</v>
+        <v>400</v>
       </c>
       <c r="B11" t="s">
         <v>292</v>
       </c>
       <c r="C11" t="s">
-        <v>368</v>
+        <v>292</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -4747,7 +4762,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B14" t="s">
         <v>292</v>
@@ -4780,38 +4795,41 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B17" t="s">
         <v>292</v>
       </c>
       <c r="C17" t="s">
-        <v>368</v>
+        <v>292</v>
       </c>
       <c r="D17" t="s">
-        <v>370</v>
+        <v>401</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>384</v>
+        <v>404</v>
       </c>
       <c r="B18" t="s">
         <v>300</v>
       </c>
       <c r="C18" t="s">
-        <v>368</v>
+        <v>292</v>
+      </c>
+      <c r="D18" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>349</v>
+        <v>403</v>
       </c>
       <c r="B19" t="s">
         <v>292</v>
       </c>
       <c r="C19" t="s">
-        <v>368</v>
+        <v>292</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -4822,87 +4840,90 @@
         <v>292</v>
       </c>
       <c r="C20" t="s">
-        <v>368</v>
+        <v>292</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B21" t="s">
         <v>292</v>
       </c>
       <c r="C21" t="s">
-        <v>368</v>
+        <v>300</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B22" t="s">
         <v>292</v>
       </c>
       <c r="C22" t="s">
-        <v>368</v>
+        <v>300</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B23" t="s">
         <v>292</v>
       </c>
       <c r="C23" t="s">
-        <v>368</v>
+        <v>300</v>
       </c>
       <c r="D23" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>375</v>
+        <v>405</v>
       </c>
       <c r="B24" t="s">
         <v>292</v>
       </c>
       <c r="C24" t="s">
-        <v>368</v>
+        <v>406</v>
+      </c>
+      <c r="D24" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="B25" t="s">
         <v>292</v>
       </c>
       <c r="C25" t="s">
-        <v>368</v>
+        <v>292</v>
       </c>
       <c r="D25" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>304</v>
+        <v>408</v>
       </c>
       <c r="B26" t="s">
         <v>292</v>
       </c>
       <c r="C26" t="s">
-        <v>368</v>
+        <v>292</v>
       </c>
       <c r="D26" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="B27" t="s">
         <v>292</v>
@@ -4911,12 +4932,12 @@
         <v>300</v>
       </c>
       <c r="D27" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="B28" t="s">
         <v>292</v>
@@ -4927,7 +4948,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="B29" t="s">
         <v>292</v>
@@ -4936,7 +4957,7 @@
         <v>292</v>
       </c>
       <c r="D29" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -4952,7 +4973,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="B31" t="s">
         <v>292</v>
@@ -4961,12 +4982,12 @@
         <v>292</v>
       </c>
       <c r="D31" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="B32" t="s">
         <v>292</v>
@@ -4975,40 +4996,40 @@
         <v>292</v>
       </c>
       <c r="D32" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="B33" t="s">
         <v>292</v>
       </c>
       <c r="C33" t="s">
-        <v>368</v>
+        <v>292</v>
       </c>
       <c r="D33" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B34" t="s">
         <v>292</v>
       </c>
       <c r="C34" t="s">
-        <v>368</v>
+        <v>300</v>
       </c>
       <c r="D34" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="B35" t="s">
         <v>292</v>
@@ -5019,7 +5040,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="B36" t="s">
         <v>292</v>
@@ -5028,12 +5049,12 @@
         <v>300</v>
       </c>
       <c r="D36" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="B37" t="s">
         <v>292</v>
@@ -5044,7 +5065,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="B38" t="s">
         <v>292</v>
@@ -5055,7 +5076,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="B39" t="s">
         <v>292</v>
@@ -5066,7 +5087,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B40" t="s">
         <v>292</v>
@@ -5075,12 +5096,12 @@
         <v>292</v>
       </c>
       <c r="D40" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="18" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: document Dev tools for macOS
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markus/Projects/wiki/Settings/Chocolatey/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/work/Projects/wiki/Settings/Chocolatey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A2C3CD-23C8-6946-9E07-92E265406B93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9343F546-094D-ED46-9AB5-9B1453F352D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="76800" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chocolatey" sheetId="1" r:id="rId1"/>
     <sheet name="Mac availability" sheetId="2" r:id="rId2"/>
     <sheet name="Mac installed" sheetId="3" r:id="rId3"/>
+    <sheet name="Mac@Work" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Chocolatey!$A$1:$H$134</definedName>
@@ -72,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="412">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -1322,6 +1323,15 @@
   </si>
   <si>
     <t>karabiner-elements</t>
+  </si>
+  <si>
+    <t>kubectl</t>
+  </si>
+  <si>
+    <t>hashicorp/tap/terraform</t>
+  </si>
+  <si>
+    <t>https://developer.hashicorp.com/terraform/tutorials/aws-get-started/install-cli</t>
   </si>
 </sst>
 </file>
@@ -4589,7 +4599,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5111,4 +5121,46 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{065AFD5E-E7C4-4344-BCB5-48CFA86F7E2C}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>410</v>
+      </c>
+      <c r="B2" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>409</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: update brew apps
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/work/Projects/wiki/Settings/Chocolatey/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markus/Projects/wiki/Settings/Chocolatey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9343F546-094D-ED46-9AB5-9B1453F352D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8026852C-3028-304A-A15D-9AC64FCEC451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="76800" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chocolatey" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="412">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -1160,9 +1160,6 @@
     <t>Uplay</t>
   </si>
   <si>
-    <t>Achtung: Tray nicht installieren, führt zu Problemen</t>
-  </si>
-  <si>
     <t>CascadiaCode</t>
   </si>
   <si>
@@ -1332,13 +1329,16 @@
   </si>
   <si>
     <t>https://developer.hashicorp.com/terraform/tutorials/aws-get-started/install-cli</t>
+  </si>
+  <si>
+    <t>Ly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1407,6 +1407,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1490,7 +1497,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1526,6 +1533,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
@@ -4219,10 +4227,10 @@
         <v>292</v>
       </c>
       <c r="C3" t="s">
+        <v>379</v>
+      </c>
+      <c r="D3" t="s">
         <v>380</v>
-      </c>
-      <c r="D3" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4596,10 +4604,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F93F60-305A-704A-9194-4387AC0BEE7B}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4609,21 +4617,24 @@
     <col min="4" max="4" width="66.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>378</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>362</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>379</v>
-      </c>
-      <c r="C1" s="17" t="s">
+      <c r="D1" s="17" t="s">
         <v>363</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="17" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>326</v>
       </c>
@@ -4633,11 +4644,8 @@
       <c r="C2" t="s">
         <v>292</v>
       </c>
-      <c r="D2" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>318</v>
       </c>
@@ -4647,10 +4655,13 @@
       <c r="C3" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B4" t="s">
         <v>292</v>
@@ -4659,24 +4670,24 @@
         <v>300</v>
       </c>
       <c r="D4" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>292</v>
+      </c>
+      <c r="C5" t="s">
+        <v>292</v>
+      </c>
+      <c r="D5" t="s">
         <v>357</v>
       </c>
-      <c r="B5" t="s">
-        <v>292</v>
-      </c>
-      <c r="C5" t="s">
-        <v>292</v>
-      </c>
-      <c r="D5" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>347</v>
       </c>
@@ -4686,8 +4697,11 @@
       <c r="C6" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -4698,57 +4712,63 @@
         <v>292</v>
       </c>
       <c r="D7" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>397</v>
+      </c>
+      <c r="B8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C8" t="s">
+        <v>292</v>
+      </c>
+      <c r="D8" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>398</v>
       </c>
-      <c r="B8" t="s">
-        <v>292</v>
-      </c>
-      <c r="C8" t="s">
-        <v>292</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B9" t="s">
+        <v>292</v>
+      </c>
+      <c r="C9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B10" t="s">
+        <v>292</v>
+      </c>
+      <c r="C10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>399</v>
       </c>
-      <c r="B9" t="s">
-        <v>292</v>
-      </c>
-      <c r="C9" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>361</v>
-      </c>
-      <c r="B10" t="s">
-        <v>292</v>
-      </c>
-      <c r="C10" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>400</v>
-      </c>
       <c r="B11" t="s">
         <v>292</v>
       </c>
       <c r="C11" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>90</v>
       </c>
@@ -4759,7 +4779,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -4770,9 +4790,9 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B14" t="s">
         <v>292</v>
@@ -4781,7 +4801,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -4792,7 +4812,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>133</v>
       </c>
@@ -4803,9 +4823,9 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B17" t="s">
         <v>292</v>
@@ -4814,12 +4834,12 @@
         <v>292</v>
       </c>
       <c r="D17" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B18" t="s">
         <v>300</v>
@@ -4828,13 +4848,13 @@
         <v>292</v>
       </c>
       <c r="D18" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>403</v>
-      </c>
       <c r="B19" t="s">
         <v>292</v>
       </c>
@@ -4842,7 +4862,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>352</v>
       </c>
@@ -4853,9 +4873,9 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B21" t="s">
         <v>292</v>
@@ -4863,10 +4883,13 @@
       <c r="C21" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B22" t="s">
         <v>292</v>
@@ -4874,10 +4897,13 @@
       <c r="C22" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" s="19" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B23" t="s">
         <v>292</v>
@@ -4886,54 +4912,57 @@
         <v>300</v>
       </c>
       <c r="D23" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>368</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>404</v>
+      </c>
+      <c r="B24" t="s">
+        <v>292</v>
+      </c>
+      <c r="C24" t="s">
         <v>405</v>
       </c>
-      <c r="B24" t="s">
-        <v>292</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>406</v>
       </c>
-      <c r="D24" t="s">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>370</v>
+      </c>
+      <c r="B25" t="s">
+        <v>292</v>
+      </c>
+      <c r="C25" t="s">
+        <v>292</v>
+      </c>
+      <c r="D25" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>371</v>
-      </c>
-      <c r="B25" t="s">
-        <v>292</v>
-      </c>
-      <c r="C25" t="s">
-        <v>292</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="B26" t="s">
+        <v>292</v>
+      </c>
+      <c r="C26" t="s">
+        <v>292</v>
+      </c>
+      <c r="D26" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>408</v>
-      </c>
-      <c r="B26" t="s">
-        <v>292</v>
-      </c>
-      <c r="C26" t="s">
-        <v>292</v>
-      </c>
-      <c r="D26" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>373</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>374</v>
       </c>
       <c r="B27" t="s">
         <v>292</v>
@@ -4942,35 +4971,38 @@
         <v>300</v>
       </c>
       <c r="D27" t="s">
+        <v>374</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
+        <v>292</v>
+      </c>
+      <c r="C28" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>376</v>
       </c>
-      <c r="B28" t="s">
-        <v>292</v>
-      </c>
-      <c r="C28" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
+        <v>292</v>
+      </c>
+      <c r="C29" t="s">
+        <v>292</v>
+      </c>
+      <c r="D29" t="s">
         <v>377</v>
       </c>
-      <c r="B29" t="s">
-        <v>292</v>
-      </c>
-      <c r="C29" t="s">
-        <v>292</v>
-      </c>
-      <c r="D29" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -4981,51 +5013,51 @@
         <v>292</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>381</v>
+      </c>
+      <c r="B31" t="s">
+        <v>292</v>
+      </c>
+      <c r="C31" t="s">
+        <v>292</v>
+      </c>
+      <c r="D31" t="s">
         <v>382</v>
       </c>
-      <c r="B31" t="s">
-        <v>292</v>
-      </c>
-      <c r="C31" t="s">
-        <v>292</v>
-      </c>
-      <c r="D31" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>384</v>
+      </c>
+      <c r="B32" t="s">
+        <v>292</v>
+      </c>
+      <c r="C32" t="s">
+        <v>292</v>
+      </c>
+      <c r="D32" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>385</v>
       </c>
-      <c r="B32" t="s">
-        <v>292</v>
-      </c>
-      <c r="C32" t="s">
-        <v>292</v>
-      </c>
-      <c r="D32" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="B33" t="s">
+        <v>292</v>
+      </c>
+      <c r="C33" t="s">
+        <v>292</v>
+      </c>
+      <c r="D33" t="s">
         <v>386</v>
       </c>
-      <c r="B33" t="s">
-        <v>292</v>
-      </c>
-      <c r="C33" t="s">
-        <v>292</v>
-      </c>
-      <c r="D33" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B34" t="s">
         <v>292</v>
@@ -5034,12 +5066,12 @@
         <v>300</v>
       </c>
       <c r="D34" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B35" t="s">
         <v>292</v>
@@ -5048,9 +5080,9 @@
         <v>292</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B36" t="s">
         <v>292</v>
@@ -5059,59 +5091,62 @@
         <v>300</v>
       </c>
       <c r="D36" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>392</v>
+      </c>
+      <c r="B37" t="s">
+        <v>292</v>
+      </c>
+      <c r="C37" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>393</v>
       </c>
-      <c r="B37" t="s">
-        <v>292</v>
-      </c>
-      <c r="C37" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="B38" t="s">
+        <v>292</v>
+      </c>
+      <c r="C38" t="s">
+        <v>292</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>394</v>
       </c>
-      <c r="B38" t="s">
-        <v>292</v>
-      </c>
-      <c r="C38" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="B39" t="s">
+        <v>292</v>
+      </c>
+      <c r="C39" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>395</v>
       </c>
-      <c r="B39" t="s">
-        <v>292</v>
-      </c>
-      <c r="C39" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="B40" t="s">
+        <v>292</v>
+      </c>
+      <c r="C40" t="s">
+        <v>292</v>
+      </c>
+      <c r="D40" t="s">
         <v>396</v>
       </c>
-      <c r="B40" t="s">
-        <v>292</v>
-      </c>
-      <c r="C40" t="s">
-        <v>292</v>
-      </c>
-      <c r="D40" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="18" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -5144,10 +5179,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>409</v>
+      </c>
+      <c r="B2" t="s">
         <v>410</v>
-      </c>
-      <c r="B2" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -5157,7 +5192,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs: install helm via brew
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markus/Projects/wiki/Settings/Chocolatey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8026852C-3028-304A-A15D-9AC64FCEC451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50AB39AF-3479-0640-A935-0C9BB0BCCF68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9960" yWindow="2640" windowWidth="34560" windowHeight="21580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chocolatey" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="413">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -1332,6 +1332,9 @@
   </si>
   <si>
     <t>Ly</t>
+  </si>
+  <si>
+    <t>helm</t>
   </si>
 </sst>
 </file>
@@ -4606,7 +4609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F93F60-305A-704A-9194-4387AC0BEE7B}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="135" workbookViewId="0">
+    <sheetView zoomScale="156" zoomScaleNormal="135" workbookViewId="0">
       <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
@@ -5160,10 +5163,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{065AFD5E-E7C4-4344-BCB5-48CFA86F7E2C}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5195,6 +5198,11 @@
         <v>408</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>412</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: update mac apps
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markus/Projects/wiki/Settings/Chocolatey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69EB1643-74CF-E348-9CBD-7CA0F9BEEFA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53DBC133-089E-1744-BBE5-D21EF3E3AC02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chocolatey" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="420">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -1344,6 +1344,18 @@
   </si>
   <si>
     <t>hstracker</t>
+  </si>
+  <si>
+    <t>localsend</t>
+  </si>
+  <si>
+    <t>neardrop</t>
+  </si>
+  <si>
+    <t>Android file transfer / https://github.com/localsend/homebrew-localsend</t>
+  </si>
+  <si>
+    <t>Android file transfer / https://github.com/grishka/NearDrop</t>
   </si>
 </sst>
 </file>
@@ -4617,11 +4629,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F93F60-305A-704A-9194-4387AC0BEE7B}">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="135" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B43" sqref="B43:C43"/>
+      <selection pane="topRight" activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5195,16 +5207,44 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="18"/>
+      <c r="A44" t="s">
+        <v>417</v>
+      </c>
+      <c r="B44" t="s">
+        <v>292</v>
+      </c>
+      <c r="C44" t="s">
+        <v>292</v>
+      </c>
+      <c r="D44" t="s">
+        <v>419</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="18" t="s">
+      <c r="A45" t="s">
+        <v>416</v>
+      </c>
+      <c r="B45" t="s">
+        <v>292</v>
+      </c>
+      <c r="C45" t="s">
+        <v>292</v>
+      </c>
+      <c r="D45" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="18"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="18" t="s">
         <v>388</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A45" r:id="rId1" xr:uid="{65CB6B51-C990-C94E-8E20-9886EFDBDD52}"/>
+    <hyperlink ref="A47" r:id="rId1" xr:uid="{65CB6B51-C990-C94E-8E20-9886EFDBDD52}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
feat: document usage of FileMerge
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markus/Projects/wiki/Settings/Chocolatey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53DBC133-089E-1744-BBE5-D21EF3E3AC02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F43BC24-8057-1642-B390-D3AC59E06B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="422">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -1118,9 +1118,6 @@
     <t>WinMerge</t>
   </si>
   <si>
-    <t>BeyondCompare</t>
-  </si>
-  <si>
     <t>WinRAR / 7-Zip</t>
   </si>
   <si>
@@ -1356,6 +1353,15 @@
   </si>
   <si>
     <t>Android file transfer / https://github.com/grishka/NearDrop</t>
+  </si>
+  <si>
+    <t>BeyondCompare ($) / FileMerge (via Xcode)</t>
+  </si>
+  <si>
+    <t>Xcode</t>
+  </si>
+  <si>
+    <t>App Store (bringt FileMerge)</t>
   </si>
 </sst>
 </file>
@@ -4211,7 +4217,7 @@
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C9" sqref="C9"/>
+      <selection pane="topRight" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4252,10 +4258,10 @@
         <v>292</v>
       </c>
       <c r="C3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D3" t="s">
         <v>379</v>
-      </c>
-      <c r="D3" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4514,7 +4520,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>339</v>
       </c>
@@ -4522,101 +4528,98 @@
         <v>300</v>
       </c>
       <c r="C33" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>340</v>
-      </c>
-      <c r="D33" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>341</v>
       </c>
       <c r="B34" t="s">
         <v>300</v>
       </c>
       <c r="C34" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>342</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>343</v>
       </c>
       <c r="B35" t="s">
         <v>300</v>
       </c>
       <c r="C35" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="B36" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>345</v>
       </c>
-      <c r="B36" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="B37" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>346</v>
       </c>
-      <c r="B37" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="B38" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>347</v>
-      </c>
-      <c r="B38" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>348</v>
       </c>
       <c r="B39" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>348</v>
+      </c>
+      <c r="B40" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>349</v>
       </c>
-      <c r="B40" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="B41" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>350</v>
       </c>
-      <c r="B41" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="B42" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>351</v>
       </c>
-      <c r="B42" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="B43" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>352</v>
-      </c>
-      <c r="B43" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>353</v>
       </c>
       <c r="B44" t="s">
         <v>300</v>
@@ -4629,11 +4632,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F93F60-305A-704A-9194-4387AC0BEE7B}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="135" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D45" sqref="D45"/>
+      <selection pane="topRight" activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4645,19 +4648,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
+        <v>360</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>377</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>361</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>378</v>
-      </c>
-      <c r="C1" s="17" t="s">
+      <c r="D1" s="17" t="s">
         <v>362</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>363</v>
-      </c>
       <c r="E1" s="17" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -4687,7 +4690,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B4" t="s">
         <v>292</v>
@@ -4696,26 +4699,26 @@
         <v>300</v>
       </c>
       <c r="D4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>355</v>
+      </c>
+      <c r="B5" t="s">
+        <v>292</v>
+      </c>
+      <c r="C5" t="s">
+        <v>292</v>
+      </c>
+      <c r="D5" t="s">
         <v>356</v>
-      </c>
-      <c r="B5" t="s">
-        <v>292</v>
-      </c>
-      <c r="C5" t="s">
-        <v>292</v>
-      </c>
-      <c r="D5" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B6" t="s">
         <v>292</v>
@@ -4738,12 +4741,12 @@
         <v>292</v>
       </c>
       <c r="D7" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B8" t="s">
         <v>292</v>
@@ -4752,12 +4755,12 @@
         <v>292</v>
       </c>
       <c r="D8" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B9" t="s">
         <v>292</v>
@@ -4771,7 +4774,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B10" t="s">
         <v>292</v>
@@ -4782,7 +4785,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B11" t="s">
         <v>292</v>
@@ -4818,7 +4821,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B14" t="s">
         <v>292</v>
@@ -4851,7 +4854,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B17" t="s">
         <v>292</v>
@@ -4860,12 +4863,12 @@
         <v>292</v>
       </c>
       <c r="D17" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B18" t="s">
         <v>300</v>
@@ -4874,12 +4877,12 @@
         <v>292</v>
       </c>
       <c r="D18" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B19" t="s">
         <v>292</v>
@@ -4890,7 +4893,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B20" t="s">
         <v>292</v>
@@ -4901,7 +4904,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B21" t="s">
         <v>292</v>
@@ -4915,7 +4918,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B22" t="s">
         <v>292</v>
@@ -4929,7 +4932,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B23" t="s">
         <v>292</v>
@@ -4938,7 +4941,7 @@
         <v>300</v>
       </c>
       <c r="D23" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E23" s="19" t="s">
         <v>292</v>
@@ -4946,35 +4949,35 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>403</v>
+      </c>
+      <c r="B24" t="s">
+        <v>292</v>
+      </c>
+      <c r="C24" t="s">
         <v>404</v>
       </c>
-      <c r="B24" t="s">
-        <v>292</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>405</v>
-      </c>
-      <c r="D24" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>369</v>
+      </c>
+      <c r="B25" t="s">
+        <v>292</v>
+      </c>
+      <c r="C25" t="s">
+        <v>292</v>
+      </c>
+      <c r="D25" t="s">
         <v>370</v>
-      </c>
-      <c r="B25" t="s">
-        <v>292</v>
-      </c>
-      <c r="C25" t="s">
-        <v>292</v>
-      </c>
-      <c r="D25" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B26" t="s">
         <v>292</v>
@@ -4983,12 +4986,12 @@
         <v>292</v>
       </c>
       <c r="D26" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B27" t="s">
         <v>292</v>
@@ -4997,7 +5000,7 @@
         <v>300</v>
       </c>
       <c r="D27" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E27" s="19" t="s">
         <v>292</v>
@@ -5005,7 +5008,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B28" t="s">
         <v>292</v>
@@ -5016,16 +5019,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>375</v>
+      </c>
+      <c r="B29" t="s">
+        <v>292</v>
+      </c>
+      <c r="C29" t="s">
+        <v>292</v>
+      </c>
+      <c r="D29" t="s">
         <v>376</v>
-      </c>
-      <c r="B29" t="s">
-        <v>292</v>
-      </c>
-      <c r="C29" t="s">
-        <v>292</v>
-      </c>
-      <c r="D29" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -5041,21 +5044,21 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>380</v>
+      </c>
+      <c r="B31" t="s">
+        <v>292</v>
+      </c>
+      <c r="C31" t="s">
+        <v>292</v>
+      </c>
+      <c r="D31" t="s">
         <v>381</v>
-      </c>
-      <c r="B31" t="s">
-        <v>292</v>
-      </c>
-      <c r="C31" t="s">
-        <v>292</v>
-      </c>
-      <c r="D31" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B32" t="s">
         <v>292</v>
@@ -5064,26 +5067,26 @@
         <v>292</v>
       </c>
       <c r="D32" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>384</v>
+      </c>
+      <c r="B33" t="s">
+        <v>292</v>
+      </c>
+      <c r="C33" t="s">
+        <v>292</v>
+      </c>
+      <c r="D33" t="s">
         <v>385</v>
-      </c>
-      <c r="B33" t="s">
-        <v>292</v>
-      </c>
-      <c r="C33" t="s">
-        <v>292</v>
-      </c>
-      <c r="D33" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B34" t="s">
         <v>292</v>
@@ -5092,12 +5095,12 @@
         <v>300</v>
       </c>
       <c r="D34" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B35" t="s">
         <v>292</v>
@@ -5108,7 +5111,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B36" t="s">
         <v>292</v>
@@ -5117,12 +5120,12 @@
         <v>300</v>
       </c>
       <c r="D36" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B37" t="s">
         <v>292</v>
@@ -5133,7 +5136,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B38" t="s">
         <v>292</v>
@@ -5147,7 +5150,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B39" t="s">
         <v>292</v>
@@ -5158,21 +5161,21 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>394</v>
+      </c>
+      <c r="B40" t="s">
+        <v>292</v>
+      </c>
+      <c r="C40" t="s">
+        <v>292</v>
+      </c>
+      <c r="D40" t="s">
         <v>395</v>
-      </c>
-      <c r="B40" t="s">
-        <v>292</v>
-      </c>
-      <c r="C40" t="s">
-        <v>292</v>
-      </c>
-      <c r="D40" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B41" t="s">
         <v>292</v>
@@ -5181,12 +5184,12 @@
         <v>300</v>
       </c>
       <c r="D41" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B42" t="s">
         <v>292</v>
@@ -5197,7 +5200,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B43" t="s">
         <v>292</v>
@@ -5208,7 +5211,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B44" t="s">
         <v>292</v>
@@ -5217,12 +5220,12 @@
         <v>292</v>
       </c>
       <c r="D44" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B45" t="s">
         <v>292</v>
@@ -5231,20 +5234,34 @@
         <v>292</v>
       </c>
       <c r="D45" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="18"/>
+      <c r="A46" t="s">
+        <v>420</v>
+      </c>
+      <c r="B46" t="s">
+        <v>292</v>
+      </c>
+      <c r="C46" t="s">
+        <v>300</v>
+      </c>
+      <c r="D46" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="18" t="s">
-        <v>388</v>
+      <c r="A47" s="18"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="18" t="s">
+        <v>387</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A47" r:id="rId1" xr:uid="{65CB6B51-C990-C94E-8E20-9886EFDBDD52}"/>
+    <hyperlink ref="A48" r:id="rId1" xr:uid="{65CB6B51-C990-C94E-8E20-9886EFDBDD52}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -5272,10 +5289,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B2" t="s">
         <v>409</v>
-      </c>
-      <c r="B2" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -5285,12 +5302,12 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs: update winget packages for work
</commit_message>
<xml_diff>
--- a/Settings/Chocolatey/Chocolatey.xlsx
+++ b/Settings/Chocolatey/Chocolatey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markus/Projects/wiki/Settings/Chocolatey/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\markus\projects\wiki\Settings\Chocolatey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A972B3-2778-2D4D-970B-9CAE95EE0A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0599A668-A925-462F-961A-AFA385865243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="-5960" windowWidth="51200" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38310" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chocolatey" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Mac@Work" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Chocolatey!$A$1:$H$134</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Chocolatey!$A$1:$H$135</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Mac installed'!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="425">
   <si>
     <t>adblockpluschrome</t>
   </si>
@@ -971,9 +971,6 @@
     <t>Muss vor Acrobat Pro installiert werden, sonst Konflikt.</t>
   </si>
   <si>
-    <t>Version in chocolatey (1.15) too old (current: 1.16) / winget: Installieren fehlgeschlagen mit Exitcode: 0x80070002 : Das System kann die angegebene Datei nicht finden.</t>
-  </si>
-  <si>
     <t>✅</t>
   </si>
   <si>
@@ -1368,6 +1365,12 @@
   </si>
   <si>
     <t>Alternative: Affinity</t>
+  </si>
+  <si>
+    <t>Already installed in newer versions of Windows</t>
+  </si>
+  <si>
+    <t>Obsidian.Obsidian</t>
   </si>
 </sst>
 </file>
@@ -1883,24 +1886,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H138"/>
+  <dimension ref="A1:H139"/>
   <sheetViews>
-    <sheetView zoomScale="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H39" sqref="H39"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="6.1640625" customWidth="1"/>
-    <col min="4" max="4" width="6.5" customWidth="1"/>
-    <col min="5" max="6" width="7.6640625" customWidth="1"/>
-    <col min="7" max="7" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="70.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="6.1796875" customWidth="1"/>
+    <col min="4" max="4" width="6.453125" customWidth="1"/>
+    <col min="5" max="6" width="7.6328125" customWidth="1"/>
+    <col min="7" max="7" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="70.6328125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>54</v>
       </c>
@@ -1926,7 +1929,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>58</v>
       </c>
@@ -1950,7 +1953,7 @@
       </c>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1966,7 +1969,7 @@
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>59</v>
       </c>
@@ -1992,7 +1995,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -2006,7 +2009,7 @@
       </c>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>91</v>
       </c>
@@ -2022,7 +2025,7 @@
       </c>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>92</v>
       </c>
@@ -2036,7 +2039,7 @@
       <c r="G7" s="6"/>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>93</v>
       </c>
@@ -2050,7 +2053,7 @@
       <c r="G8" s="6"/>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>60</v>
       </c>
@@ -2070,15 +2073,13 @@
       </c>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>100</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="13" t="s">
@@ -2086,7 +2087,7 @@
       </c>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -2098,7 +2099,7 @@
       <c r="G11" s="6"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>114</v>
       </c>
@@ -2106,9 +2107,7 @@
         <v>55</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="6"/>
@@ -2116,7 +2115,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>124</v>
       </c>
@@ -2130,7 +2129,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>125</v>
       </c>
@@ -2144,7 +2143,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>3</v>
       </c>
@@ -2160,7 +2159,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>138</v>
       </c>
@@ -2176,7 +2175,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
@@ -2188,7 +2187,7 @@
       <c r="G17" s="6"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -2202,7 +2201,7 @@
       </c>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>101</v>
       </c>
@@ -2218,7 +2217,7 @@
       </c>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>140</v>
       </c>
@@ -2236,7 +2235,7 @@
       </c>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>133</v>
       </c>
@@ -2252,13 +2251,15 @@
       </c>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>173</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="13" t="s">
@@ -2268,7 +2269,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
         <v>6</v>
       </c>
@@ -2284,7 +2285,7 @@
       <c r="G23" s="6"/>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -2296,7 +2297,7 @@
       <c r="G24" s="6"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>102</v>
       </c>
@@ -2314,7 +2315,7 @@
       </c>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>99</v>
       </c>
@@ -2332,7 +2333,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>8</v>
       </c>
@@ -2352,7 +2353,7 @@
       </c>
       <c r="H27" s="7"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>150</v>
       </c>
@@ -2374,7 +2375,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
         <v>116</v>
       </c>
@@ -2382,9 +2383,7 @@
         <v>55</v>
       </c>
       <c r="C29" s="3"/>
-      <c r="D29" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="13" t="s">
@@ -2394,7 +2393,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>9</v>
       </c>
@@ -2414,7 +2413,7 @@
       </c>
       <c r="H30" s="7"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>10</v>
       </c>
@@ -2436,7 +2435,7 @@
       </c>
       <c r="H31" s="7"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>111</v>
       </c>
@@ -2456,7 +2455,7 @@
       </c>
       <c r="H32" s="7"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>67</v>
       </c>
@@ -2472,7 +2471,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="10" t="s">
         <v>56</v>
       </c>
@@ -2480,9 +2479,7 @@
         <v>55</v>
       </c>
       <c r="C34" s="3"/>
-      <c r="D34" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="13" t="s">
@@ -2492,15 +2489,13 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="10" t="s">
         <v>103</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
-      <c r="D35" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="13" t="s">
@@ -2510,7 +2505,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>61</v>
       </c>
@@ -2520,9 +2515,7 @@
       <c r="C36" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="13" t="s">
@@ -2530,7 +2523,7 @@
       </c>
       <c r="H36" s="7"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>11</v>
       </c>
@@ -2544,7 +2537,7 @@
       </c>
       <c r="H37" s="7"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
         <v>87</v>
       </c>
@@ -2564,7 +2557,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>12</v>
       </c>
@@ -2586,7 +2579,7 @@
       </c>
       <c r="H39" s="7"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>13</v>
       </c>
@@ -2604,7 +2597,7 @@
       </c>
       <c r="H40" s="7"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
@@ -2616,7 +2609,7 @@
       <c r="G41" s="6"/>
       <c r="H41" s="7"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>134</v>
       </c>
@@ -2632,7 +2625,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="10" t="s">
         <v>84</v>
       </c>
@@ -2646,7 +2639,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>15</v>
       </c>
@@ -2662,7 +2655,7 @@
       </c>
       <c r="H44" s="7"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="12" t="s">
         <v>149</v>
       </c>
@@ -2682,7 +2675,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>16</v>
       </c>
@@ -2704,7 +2697,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>90</v>
       </c>
@@ -2724,7 +2717,7 @@
       </c>
       <c r="H47" s="7"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
         <v>96</v>
       </c>
@@ -2742,7 +2735,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>80</v>
       </c>
@@ -2760,7 +2753,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>17</v>
       </c>
@@ -2776,7 +2769,7 @@
       </c>
       <c r="H50" s="7"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>18</v>
       </c>
@@ -2792,7 +2785,7 @@
       <c r="G51" s="6"/>
       <c r="H51" s="7"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>161</v>
       </c>
@@ -2810,15 +2803,13 @@
       </c>
       <c r="H52" s="7"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
-      <c r="D53" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D53" s="3"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="13" t="s">
@@ -2826,7 +2817,7 @@
       </c>
       <c r="H53" s="7"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>20</v>
       </c>
@@ -2848,7 +2839,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>62</v>
       </c>
@@ -2868,7 +2859,7 @@
       </c>
       <c r="H55" s="7"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>162</v>
       </c>
@@ -2890,7 +2881,7 @@
       </c>
       <c r="H56" s="7"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>21</v>
       </c>
@@ -2908,7 +2899,7 @@
       <c r="G57" s="6"/>
       <c r="H57" s="7"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>86</v>
       </c>
@@ -2928,7 +2919,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="10" t="s">
         <v>22</v>
       </c>
@@ -2940,7 +2931,7 @@
       <c r="G59" s="6"/>
       <c r="H59" s="7"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>136</v>
       </c>
@@ -2954,7 +2945,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>122</v>
       </c>
@@ -2970,7 +2961,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="1"/>
       <c r="B62" s="3" t="s">
         <v>55</v>
@@ -2986,7 +2977,7 @@
       </c>
       <c r="H62" s="7"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>77</v>
       </c>
@@ -3002,7 +2993,7 @@
       </c>
       <c r="H63" s="7"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>230</v>
       </c>
@@ -3020,7 +3011,7 @@
       </c>
       <c r="H64" s="7"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>23</v>
       </c>
@@ -3028,15 +3019,13 @@
         <v>55</v>
       </c>
       <c r="C65" s="3"/>
-      <c r="D65" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D65" s="3"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
       <c r="G65" s="6"/>
       <c r="H65" s="7"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>105</v>
       </c>
@@ -3052,7 +3041,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>141</v>
       </c>
@@ -3068,7 +3057,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>24</v>
       </c>
@@ -3082,7 +3071,7 @@
       </c>
       <c r="H68" s="7"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>25</v>
       </c>
@@ -3096,7 +3085,7 @@
       </c>
       <c r="H69" s="7"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>26</v>
       </c>
@@ -3114,7 +3103,7 @@
       </c>
       <c r="H70" s="7"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>108</v>
       </c>
@@ -3130,25 +3119,23 @@
       </c>
       <c r="H71" s="7"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
-      <c r="D72" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D72" s="3"/>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
       <c r="G72" s="11" t="s">
         <v>200</v>
       </c>
       <c r="H72" s="7" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>76</v>
       </c>
@@ -3166,7 +3153,7 @@
       </c>
       <c r="H73" s="7"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>81</v>
       </c>
@@ -3180,7 +3167,7 @@
       </c>
       <c r="H74" s="7"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" s="10" t="s">
         <v>178</v>
       </c>
@@ -3188,9 +3175,7 @@
         <v>55</v>
       </c>
       <c r="C75" s="3"/>
-      <c r="D75" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D75" s="3"/>
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
       <c r="G75" s="13" t="s">
@@ -3198,7 +3183,7 @@
       </c>
       <c r="H75" s="7"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>27</v>
       </c>
@@ -3216,7 +3201,7 @@
       </c>
       <c r="H76" s="7"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>63</v>
       </c>
@@ -3232,7 +3217,7 @@
       </c>
       <c r="H77" s="7"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>64</v>
       </c>
@@ -3256,7 +3241,7 @@
       </c>
       <c r="H78" s="7"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>69</v>
       </c>
@@ -3274,51 +3259,51 @@
         <v>153</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
-        <v>28</v>
-      </c>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A80" s="1"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
+      <c r="D80" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
       <c r="G80" s="13" t="s">
-        <v>266</v>
+        <v>424</v>
       </c>
       <c r="H80" s="7"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B81" s="3"/>
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
-      <c r="G81" s="6"/>
+      <c r="G81" s="13" t="s">
+        <v>266</v>
+      </c>
       <c r="H81" s="7"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B82" s="3"/>
+        <v>95</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
-      <c r="G82" s="13" t="s">
-        <v>267</v>
-      </c>
+      <c r="G82" s="6"/>
       <c r="H82" s="7"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>29</v>
+        <v>148</v>
       </c>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -3326,101 +3311,97 @@
       <c r="E83" s="3"/>
       <c r="F83" s="3"/>
       <c r="G83" s="13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H83" s="7"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
-      <c r="D84" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D84" s="3"/>
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
       <c r="G84" s="13" t="s">
-        <v>204</v>
+        <v>268</v>
       </c>
       <c r="H84" s="7"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
-      <c r="D85" s="3"/>
+      <c r="D85" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
       <c r="G85" s="13" t="s">
-        <v>269</v>
+        <v>204</v>
       </c>
       <c r="H85" s="7"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B86" s="3"/>
       <c r="C86" s="3"/>
-      <c r="D86" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D86" s="3"/>
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
       <c r="G86" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="H86" s="7"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A87" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+      <c r="G87" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="H86" s="7"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="s">
+      <c r="H87" s="7"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A88" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B87" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E87" s="3"/>
-      <c r="F87" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G87" s="13" t="s">
+      <c r="B88" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G88" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="H87" s="7"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A88" s="1" t="s">
+      <c r="H88" s="7"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D88" s="3"/>
-      <c r="E88" s="3"/>
-      <c r="F88" s="3"/>
-      <c r="G88" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="H88" s="7"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>55</v>
@@ -3432,63 +3413,61 @@
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
       <c r="G89" s="13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H89" s="7"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B90" s="3"/>
-      <c r="C90" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
       <c r="G90" s="13" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H90" s="7"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="B91" s="3"/>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
       <c r="F91" s="3"/>
       <c r="G91" s="13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H91" s="7"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A92" s="10" t="s">
-        <v>118</v>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A92" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C92" s="3"/>
-      <c r="D92" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D92" s="3"/>
       <c r="E92" s="3"/>
       <c r="F92" s="3"/>
       <c r="G92" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="H92" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" s="1" t="s">
-        <v>144</v>
+        <v>273</v>
+      </c>
+      <c r="H92" s="7"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A93" s="10" t="s">
+        <v>118</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>55</v>
@@ -3498,121 +3477,123 @@
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
       <c r="G93" s="13" t="s">
-        <v>274</v>
+        <v>207</v>
       </c>
       <c r="H93" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B94" s="3"/>
+        <v>144</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C94" s="3"/>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
       <c r="F94" s="3"/>
       <c r="G94" s="13" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H94" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B95" s="3"/>
       <c r="C95" s="3"/>
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
       <c r="F95" s="3"/>
       <c r="G95" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H95" s="7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B96" s="3"/>
+        <v>163</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C96" s="3"/>
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
       <c r="F96" s="3"/>
       <c r="G96" s="13" t="s">
-        <v>277</v>
-      </c>
-      <c r="H96" s="7"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+        <v>276</v>
+      </c>
+      <c r="H96" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
       <c r="D97" s="3"/>
       <c r="E97" s="3"/>
       <c r="F97" s="3"/>
-      <c r="G97" s="6"/>
+      <c r="G97" s="13" t="s">
+        <v>277</v>
+      </c>
       <c r="H97" s="7"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
-      <c r="D98" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D98" s="3"/>
       <c r="E98" s="3"/>
       <c r="F98" s="3"/>
-      <c r="G98" s="13" t="s">
-        <v>208</v>
-      </c>
+      <c r="G98" s="6"/>
       <c r="H98" s="7"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
-      <c r="D99" s="3"/>
+      <c r="D99" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
       <c r="G99" s="13" t="s">
-        <v>278</v>
+        <v>208</v>
       </c>
       <c r="H99" s="7"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B100" s="3"/>
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
       <c r="G100" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H100" s="7"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A101" s="10" t="s">
-        <v>120</v>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A101" s="1" t="s">
+        <v>287</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>55</v>
@@ -3622,47 +3603,49 @@
       <c r="E101" s="3"/>
       <c r="F101" s="3"/>
       <c r="G101" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="H101" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A102" s="1" t="s">
-        <v>36</v>
+        <v>288</v>
+      </c>
+      <c r="H101" s="7"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A102" s="10" t="s">
+        <v>120</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C102" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C102" s="3"/>
       <c r="D102" s="3"/>
       <c r="E102" s="3"/>
       <c r="F102" s="3"/>
       <c r="G102" s="13" t="s">
-        <v>279</v>
-      </c>
-      <c r="H102" s="7"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+        <v>281</v>
+      </c>
+      <c r="H102" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B103" s="3"/>
-      <c r="C103" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D103" s="3"/>
       <c r="E103" s="3"/>
       <c r="F103" s="3"/>
       <c r="G103" s="13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H103" s="7"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>155</v>
+        <v>37</v>
       </c>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
@@ -3670,33 +3653,29 @@
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
       <c r="G104" s="13" t="s">
-        <v>282</v>
-      </c>
-      <c r="H104" s="7" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+        <v>280</v>
+      </c>
+      <c r="H104" s="7"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="B105" s="3"/>
+      <c r="C105" s="3"/>
       <c r="D105" s="3"/>
       <c r="E105" s="3"/>
       <c r="F105" s="3"/>
       <c r="G105" s="13" t="s">
-        <v>283</v>
-      </c>
-      <c r="H105" s="7"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+        <v>282</v>
+      </c>
+      <c r="H105" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>55</v>
@@ -3708,31 +3687,31 @@
       <c r="E106" s="3"/>
       <c r="F106" s="3"/>
       <c r="G106" s="13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H106" s="7"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B107" s="3"/>
-      <c r="C107" s="3"/>
-      <c r="D107" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D107" s="3"/>
       <c r="E107" s="3"/>
       <c r="F107" s="3"/>
       <c r="G107" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="H107" s="7" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+        <v>284</v>
+      </c>
+      <c r="H107" s="7"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
@@ -3742,19 +3721,17 @@
       <c r="E108" s="3"/>
       <c r="F108" s="3"/>
       <c r="G108" s="13" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="H108" s="7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="B109" s="3"/>
       <c r="C109" s="3"/>
       <c r="D109" s="3" t="s">
         <v>55</v>
@@ -3762,59 +3739,65 @@
       <c r="E109" s="3"/>
       <c r="F109" s="3"/>
       <c r="G109" s="13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H109" s="7" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B110" s="3"/>
+        <v>167</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="C110" s="3"/>
-      <c r="D110" s="3"/>
-      <c r="E110" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="D110" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E110" s="3"/>
       <c r="F110" s="3"/>
       <c r="G110" s="13" t="s">
-        <v>285</v>
-      </c>
-      <c r="H110" s="7"/>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+      <c r="H110" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
       <c r="D111" s="3"/>
-      <c r="E111" s="3"/>
+      <c r="E111" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F111" s="3"/>
       <c r="G111" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H111" s="7"/>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
       <c r="D112" s="3"/>
       <c r="E112" s="3"/>
       <c r="F112" s="3"/>
-      <c r="G112" s="6"/>
-      <c r="H112" s="7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A113" s="9" t="s">
-        <v>128</v>
+      <c r="G112" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="H112" s="7"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A113" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
@@ -3822,67 +3805,65 @@
       <c r="E113" s="3"/>
       <c r="F113" s="3"/>
       <c r="G113" s="6"/>
-      <c r="H113" s="7"/>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A114" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D114" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="H113" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A114" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B114" s="3"/>
+      <c r="C114" s="3"/>
+      <c r="D114" s="3"/>
       <c r="E114" s="3"/>
       <c r="F114" s="3"/>
-      <c r="G114" s="14" t="s">
-        <v>228</v>
-      </c>
-      <c r="H114" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A115" s="10" t="s">
-        <v>88</v>
+      <c r="G114" s="6"/>
+      <c r="H114" s="7"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A115" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C115" s="3"/>
-      <c r="D115" s="3"/>
+      <c r="C115" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E115" s="3"/>
       <c r="F115" s="3"/>
-      <c r="G115" s="13" t="s">
-        <v>227</v>
+      <c r="G115" s="14" t="s">
+        <v>228</v>
       </c>
       <c r="H115" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A116" s="1" t="s">
-        <v>42</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A116" s="10" t="s">
+        <v>88</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C116" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C116" s="3"/>
       <c r="D116" s="3"/>
       <c r="E116" s="3"/>
       <c r="F116" s="3"/>
-      <c r="G116" s="6"/>
-      <c r="H116" s="7"/>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G116" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="H116" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>55</v>
@@ -3893,28 +3874,30 @@
       <c r="D117" s="3"/>
       <c r="E117" s="3"/>
       <c r="F117" s="3"/>
-      <c r="G117" s="13" t="s">
-        <v>226</v>
-      </c>
+      <c r="G117" s="6"/>
       <c r="H117" s="7"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B118" s="3"/>
-      <c r="C118" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D118" s="3"/>
       <c r="E118" s="3"/>
       <c r="F118" s="3"/>
       <c r="G118" s="13" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H118" s="7"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
@@ -3922,144 +3905,134 @@
       <c r="E119" s="3"/>
       <c r="F119" s="3"/>
       <c r="G119" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="H119" s="7"/>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A120" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B120" s="3"/>
+      <c r="C120" s="3"/>
+      <c r="D120" s="3"/>
+      <c r="E120" s="3"/>
+      <c r="F120" s="3"/>
+      <c r="G120" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="H119" s="7"/>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A120" s="1" t="s">
+      <c r="H120" s="7"/>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A121" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B120" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C120" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D120" s="3"/>
-      <c r="E120" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F120" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G120" s="13" t="s">
+      <c r="B121" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D121" s="3"/>
+      <c r="E121" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G121" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="H120" s="7"/>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A121" s="1" t="s">
+      <c r="H121" s="7"/>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A122" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B121" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C121" s="3"/>
-      <c r="D121" s="3"/>
-      <c r="E121" s="3"/>
-      <c r="F121" s="3"/>
-      <c r="G121" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="H121" s="7"/>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A122" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="B122" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C122" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D122" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C122" s="3"/>
+      <c r="D122" s="3"/>
       <c r="E122" s="3"/>
       <c r="F122" s="3"/>
       <c r="G122" s="13" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="H122" s="7"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B123" s="3"/>
-      <c r="C123" s="3"/>
-      <c r="D123" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E123" s="3"/>
       <c r="F123" s="3"/>
       <c r="G123" s="13" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="H123" s="7"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B124" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="B124" s="3"/>
       <c r="C124" s="3"/>
       <c r="D124" s="3"/>
       <c r="E124" s="3"/>
       <c r="F124" s="3"/>
-      <c r="G124" s="6"/>
-      <c r="H124" s="7" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G124" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="H124" s="7"/>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
-        <v>73</v>
+        <v>165</v>
       </c>
       <c r="B125" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C125" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C125" s="3"/>
       <c r="D125" s="3"/>
       <c r="E125" s="3"/>
       <c r="F125" s="3"/>
       <c r="G125" s="6"/>
       <c r="H125" s="7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A126" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D126" s="3"/>
+      <c r="E126" s="3"/>
+      <c r="F126" s="3"/>
+      <c r="G126" s="6"/>
+      <c r="H126" s="7" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A126" s="1" t="s">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A127" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B126" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C126" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D126" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E126" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F126" s="3"/>
-      <c r="G126" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="H126" s="7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A127" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="B127" s="3" t="s">
         <v>55</v>
       </c>
@@ -4069,16 +4042,20 @@
       <c r="D127" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E127" s="3"/>
+      <c r="E127" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="F127" s="3"/>
       <c r="G127" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="H127" s="7"/>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+        <v>213</v>
+      </c>
+      <c r="H127" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>55</v>
@@ -4086,75 +4063,79 @@
       <c r="C128" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D128" s="3"/>
+      <c r="D128" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E128" s="3"/>
       <c r="F128" s="3"/>
       <c r="G128" s="13" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="H128" s="7"/>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B129" s="3"/>
-      <c r="C129" s="3"/>
+        <v>51</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D129" s="3"/>
       <c r="E129" s="3"/>
       <c r="F129" s="3"/>
       <c r="G129" s="13" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H129" s="7"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A130" s="8" t="s">
-        <v>127</v>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A130" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
       <c r="D130" s="3"/>
       <c r="E130" s="3"/>
       <c r="F130" s="3"/>
-      <c r="G130" s="6"/>
+      <c r="G130" s="13" t="s">
+        <v>218</v>
+      </c>
       <c r="H130" s="7"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A131" s="1" t="s">
-        <v>66</v>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A131" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
       <c r="D131" s="3"/>
-      <c r="E131" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="E131" s="3"/>
       <c r="F131" s="3"/>
-      <c r="G131" s="13" t="s">
+      <c r="G131" s="6"/>
+      <c r="H131" s="7"/>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A132" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B132" s="3"/>
+      <c r="C132" s="3"/>
+      <c r="D132" s="3"/>
+      <c r="E132" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F132" s="3"/>
+      <c r="G132" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="H131" s="7"/>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A132" s="1" t="s">
+      <c r="H132" s="7"/>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A133" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C132" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D132" s="3"/>
-      <c r="E132" s="3"/>
-      <c r="F132" s="3"/>
-      <c r="G132" s="6"/>
-      <c r="H132" s="7"/>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A133" s="10" t="s">
-        <v>53</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>55</v>
@@ -4165,14 +4146,12 @@
       <c r="D133" s="3"/>
       <c r="E133" s="3"/>
       <c r="F133" s="3"/>
-      <c r="G133" s="13" t="s">
-        <v>216</v>
-      </c>
+      <c r="G133" s="6"/>
       <c r="H133" s="7"/>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A134" s="1" t="s">
-        <v>113</v>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A134" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>55</v>
@@ -4182,31 +4161,49 @@
       </c>
       <c r="D134" s="3"/>
       <c r="E134" s="3"/>
-      <c r="F134" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="F134" s="3"/>
       <c r="G134" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="H134" s="7"/>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A135" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D135" s="3"/>
+      <c r="E135" s="3"/>
+      <c r="F135" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G135" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="H134" s="7"/>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A136" s="10" t="s">
+      <c r="H135" s="7"/>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A137" s="10" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A137" s="8" t="s">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A138" s="8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A138" s="9" t="s">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A139" s="9" t="s">
         <v>129</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H134" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H135" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="G1" r:id="rId1" display="https://github.com/microsoft/winget-pkgs" xr:uid="{2C434A13-8B1C-492F-95C8-B89737A54984}"/>
     <hyperlink ref="A45" r:id="rId2" xr:uid="{5AAD9A6E-C562-4737-9662-CEC2B195962E}"/>
@@ -4226,409 +4223,409 @@
       <selection pane="topRight" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>293</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="15" t="s">
         <v>294</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>295</v>
       </c>
-      <c r="D1" s="15" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>297</v>
       </c>
-      <c r="B2" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>291</v>
+      </c>
+      <c r="C3" t="s">
+        <v>376</v>
+      </c>
+      <c r="D3" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>298</v>
       </c>
-      <c r="B3" t="s">
-        <v>292</v>
-      </c>
-      <c r="C3" t="s">
-        <v>377</v>
-      </c>
-      <c r="D3" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>299</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>300</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>302</v>
       </c>
-      <c r="B5" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>299</v>
+      </c>
+      <c r="C6" t="s">
         <v>303</v>
       </c>
-      <c r="B6" t="s">
-        <v>300</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>304</v>
       </c>
-      <c r="D6" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>306</v>
       </c>
-      <c r="B7" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>307</v>
       </c>
-      <c r="B8" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>308</v>
       </c>
-      <c r="B9" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>309</v>
       </c>
-      <c r="B10" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>310</v>
       </c>
-      <c r="B11" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>311</v>
       </c>
-      <c r="B12" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>312</v>
       </c>
-      <c r="B13" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>314</v>
       </c>
-      <c r="B14" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>315</v>
       </c>
-      <c r="B15" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>316</v>
       </c>
-      <c r="B16" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>317</v>
       </c>
-      <c r="B17" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>318</v>
       </c>
-      <c r="B18" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
         <v>319</v>
       </c>
-      <c r="B19" t="s">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
+        <v>291</v>
+      </c>
+      <c r="D20" t="s">
         <v>321</v>
       </c>
-      <c r="B20" t="s">
-        <v>292</v>
-      </c>
-      <c r="D20" t="s">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>323</v>
       </c>
-      <c r="B21" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>324</v>
       </c>
-      <c r="B22" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>325</v>
       </c>
-      <c r="B23" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>326</v>
       </c>
-      <c r="B24" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>327</v>
       </c>
-      <c r="B25" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>328</v>
       </c>
-      <c r="B26" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="B27" s="16" t="s">
+        <v>299</v>
+      </c>
+      <c r="C27" t="s">
         <v>329</v>
       </c>
-      <c r="B27" s="16" t="s">
-        <v>300</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>330</v>
       </c>
-      <c r="D27" t="s">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>332</v>
       </c>
-      <c r="B28" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
+        <v>299</v>
+      </c>
+      <c r="C29" t="s">
         <v>333</v>
       </c>
-      <c r="B29" t="s">
-        <v>300</v>
-      </c>
-      <c r="C29" t="s">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="B30" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>335</v>
       </c>
-      <c r="B30" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="B31" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>336</v>
       </c>
-      <c r="B31" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="B32" t="s">
+        <v>299</v>
+      </c>
+      <c r="C32" t="s">
         <v>337</v>
       </c>
-      <c r="B32" t="s">
-        <v>300</v>
-      </c>
-      <c r="C32" t="s">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="B33" t="s">
+        <v>299</v>
+      </c>
+      <c r="C33" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>339</v>
       </c>
-      <c r="B33" t="s">
-        <v>300</v>
-      </c>
-      <c r="C33" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="B34" t="s">
+        <v>299</v>
+      </c>
+      <c r="C34" t="s">
         <v>340</v>
       </c>
-      <c r="B34" t="s">
-        <v>300</v>
-      </c>
-      <c r="C34" t="s">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="B35" t="s">
+        <v>299</v>
+      </c>
+      <c r="C35" t="s">
         <v>342</v>
       </c>
-      <c r="B35" t="s">
-        <v>300</v>
-      </c>
-      <c r="C35" t="s">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="B36" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>344</v>
       </c>
-      <c r="B36" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="B37" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>345</v>
       </c>
-      <c r="B37" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="B38" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>346</v>
       </c>
-      <c r="B38" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="B39" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>347</v>
       </c>
-      <c r="B39" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="B40" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>348</v>
       </c>
-      <c r="B40" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="B41" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>349</v>
       </c>
-      <c r="B41" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="B42" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>350</v>
       </c>
-      <c r="B42" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="B43" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>351</v>
       </c>
-      <c r="B43" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>352</v>
-      </c>
       <c r="B44" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -4640,646 +4637,646 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F93F60-305A-704A-9194-4387AC0BEE7B}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="135" workbookViewId="0">
+    <sheetView zoomScale="156" zoomScaleNormal="135" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D13" sqref="D13"/>
+      <selection pane="topRight" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
+        <v>359</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>375</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>360</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>376</v>
-      </c>
-      <c r="C1" s="17" t="s">
+      <c r="D1" s="17" t="s">
         <v>361</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>362</v>
-      </c>
       <c r="E1" s="17" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C2" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E3" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>352</v>
+      </c>
+      <c r="B4" t="s">
+        <v>291</v>
+      </c>
+      <c r="C4" t="s">
+        <v>299</v>
+      </c>
+      <c r="D4" t="s">
         <v>353</v>
       </c>
-      <c r="B4" t="s">
-        <v>292</v>
-      </c>
-      <c r="C4" t="s">
-        <v>300</v>
-      </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C5" t="s">
+        <v>291</v>
+      </c>
+      <c r="D5" t="s">
         <v>355</v>
       </c>
-      <c r="B5" t="s">
-        <v>292</v>
-      </c>
-      <c r="C5" t="s">
-        <v>292</v>
-      </c>
-      <c r="D5" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E6" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D7" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>394</v>
+      </c>
+      <c r="B8" t="s">
+        <v>291</v>
+      </c>
+      <c r="C8" t="s">
+        <v>291</v>
+      </c>
+      <c r="D8" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>395</v>
       </c>
-      <c r="B8" t="s">
-        <v>292</v>
-      </c>
-      <c r="C8" t="s">
-        <v>292</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B9" t="s">
+        <v>291</v>
+      </c>
+      <c r="C9" t="s">
+        <v>291</v>
+      </c>
+      <c r="E9" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B10" t="s">
+        <v>291</v>
+      </c>
+      <c r="C10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>396</v>
       </c>
-      <c r="B9" t="s">
-        <v>292</v>
-      </c>
-      <c r="C9" t="s">
-        <v>292</v>
-      </c>
-      <c r="E9" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>359</v>
-      </c>
-      <c r="B10" t="s">
-        <v>292</v>
-      </c>
-      <c r="C10" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>397</v>
-      </c>
       <c r="B11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E11" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>421</v>
+      </c>
+      <c r="B12" t="s">
+        <v>299</v>
+      </c>
+      <c r="C12" t="s">
+        <v>291</v>
+      </c>
+      <c r="D12" t="s">
         <v>422</v>
       </c>
-      <c r="B12" t="s">
-        <v>300</v>
-      </c>
-      <c r="C12" t="s">
-        <v>292</v>
-      </c>
-      <c r="D12" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>90</v>
       </c>
       <c r="B13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D13" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C14" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B15" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C15" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C16" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>133</v>
       </c>
       <c r="B17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C17" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>363</v>
+      </c>
+      <c r="B18" t="s">
+        <v>291</v>
+      </c>
+      <c r="C18" t="s">
+        <v>291</v>
+      </c>
+      <c r="D18" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>399</v>
+      </c>
+      <c r="B19" t="s">
+        <v>299</v>
+      </c>
+      <c r="C19" t="s">
+        <v>291</v>
+      </c>
+      <c r="D19" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>398</v>
+      </c>
+      <c r="B20" t="s">
+        <v>291</v>
+      </c>
+      <c r="C20" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>350</v>
+      </c>
+      <c r="B21" t="s">
+        <v>291</v>
+      </c>
+      <c r="C21" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>364</v>
       </c>
-      <c r="B18" t="s">
-        <v>292</v>
-      </c>
-      <c r="C18" t="s">
-        <v>292</v>
-      </c>
-      <c r="D18" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="B22" t="s">
+        <v>291</v>
+      </c>
+      <c r="C22" t="s">
+        <v>299</v>
+      </c>
+      <c r="E22" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>365</v>
+      </c>
+      <c r="B23" t="s">
+        <v>291</v>
+      </c>
+      <c r="C23" t="s">
+        <v>299</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>367</v>
+      </c>
+      <c r="B24" t="s">
+        <v>291</v>
+      </c>
+      <c r="C24" t="s">
+        <v>299</v>
+      </c>
+      <c r="D24" t="s">
+        <v>366</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>400</v>
       </c>
-      <c r="B19" t="s">
-        <v>300</v>
-      </c>
-      <c r="C19" t="s">
-        <v>292</v>
-      </c>
-      <c r="D19" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>399</v>
-      </c>
-      <c r="B20" t="s">
-        <v>292</v>
-      </c>
-      <c r="C20" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>351</v>
-      </c>
-      <c r="B21" t="s">
-        <v>292</v>
-      </c>
-      <c r="C21" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>365</v>
-      </c>
-      <c r="B22" t="s">
-        <v>292</v>
-      </c>
-      <c r="C22" t="s">
-        <v>300</v>
-      </c>
-      <c r="E22" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>366</v>
-      </c>
-      <c r="B23" t="s">
-        <v>292</v>
-      </c>
-      <c r="C23" t="s">
-        <v>300</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="B25" t="s">
+        <v>291</v>
+      </c>
+      <c r="C25" t="s">
+        <v>401</v>
+      </c>
+      <c r="D25" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>368</v>
       </c>
-      <c r="B24" t="s">
-        <v>292</v>
-      </c>
-      <c r="C24" t="s">
-        <v>300</v>
-      </c>
-      <c r="D24" t="s">
-        <v>367</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>401</v>
-      </c>
-      <c r="B25" t="s">
-        <v>292</v>
-      </c>
-      <c r="C25" t="s">
-        <v>402</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="B26" t="s">
+        <v>291</v>
+      </c>
+      <c r="C26" t="s">
+        <v>291</v>
+      </c>
+      <c r="D26" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>369</v>
-      </c>
-      <c r="B26" t="s">
-        <v>292</v>
-      </c>
-      <c r="C26" t="s">
-        <v>292</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="B27" t="s">
+        <v>291</v>
+      </c>
+      <c r="C27" t="s">
+        <v>291</v>
+      </c>
+      <c r="D27" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>404</v>
-      </c>
-      <c r="B27" t="s">
-        <v>292</v>
-      </c>
-      <c r="C27" t="s">
-        <v>292</v>
-      </c>
-      <c r="D27" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
+        <v>291</v>
+      </c>
+      <c r="C28" t="s">
+        <v>299</v>
+      </c>
+      <c r="D28" t="s">
         <v>372</v>
       </c>
-      <c r="B28" t="s">
-        <v>292</v>
-      </c>
-      <c r="C28" t="s">
-        <v>300</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="E28" s="19" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>373</v>
       </c>
-      <c r="E28" s="19" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
+        <v>291</v>
+      </c>
+      <c r="C29" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>374</v>
       </c>
-      <c r="B29" t="s">
-        <v>292</v>
-      </c>
-      <c r="C29" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>375</v>
-      </c>
       <c r="B30" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C30" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D30" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>46</v>
       </c>
       <c r="B31" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C31" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
+        <v>378</v>
+      </c>
+      <c r="B32" t="s">
+        <v>291</v>
+      </c>
+      <c r="C32" t="s">
+        <v>291</v>
+      </c>
+      <c r="D32" t="s">
         <v>379</v>
       </c>
-      <c r="B32" t="s">
-        <v>292</v>
-      </c>
-      <c r="C32" t="s">
-        <v>292</v>
-      </c>
-      <c r="D32" t="s">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>381</v>
+      </c>
+      <c r="B33" t="s">
+        <v>291</v>
+      </c>
+      <c r="C33" t="s">
+        <v>291</v>
+      </c>
+      <c r="D33" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>382</v>
+      </c>
+      <c r="B34" t="s">
+        <v>291</v>
+      </c>
+      <c r="C34" t="s">
+        <v>291</v>
+      </c>
+      <c r="D34" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>386</v>
+      </c>
+      <c r="B35" t="s">
+        <v>291</v>
+      </c>
+      <c r="C35" t="s">
+        <v>299</v>
+      </c>
+      <c r="D35" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>382</v>
-      </c>
-      <c r="B33" t="s">
-        <v>292</v>
-      </c>
-      <c r="C33" t="s">
-        <v>292</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="B36" t="s">
+        <v>291</v>
+      </c>
+      <c r="C36" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>387</v>
+      </c>
+      <c r="B37" t="s">
+        <v>291</v>
+      </c>
+      <c r="C37" t="s">
+        <v>299</v>
+      </c>
+      <c r="D37" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>389</v>
+      </c>
+      <c r="B38" t="s">
+        <v>291</v>
+      </c>
+      <c r="C38" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>390</v>
+      </c>
+      <c r="B39" t="s">
+        <v>291</v>
+      </c>
+      <c r="C39" t="s">
+        <v>291</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>391</v>
+      </c>
+      <c r="B40" t="s">
+        <v>291</v>
+      </c>
+      <c r="C40" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>392</v>
+      </c>
+      <c r="B41" t="s">
+        <v>291</v>
+      </c>
+      <c r="C41" t="s">
+        <v>291</v>
+      </c>
+      <c r="D41" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>409</v>
+      </c>
+      <c r="B42" t="s">
+        <v>291</v>
+      </c>
+      <c r="C42" t="s">
+        <v>299</v>
+      </c>
+      <c r="D42" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>410</v>
+      </c>
+      <c r="B43" t="s">
+        <v>291</v>
+      </c>
+      <c r="C43" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>411</v>
+      </c>
+      <c r="B44" t="s">
+        <v>291</v>
+      </c>
+      <c r="C44" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>413</v>
+      </c>
+      <c r="B45" t="s">
+        <v>299</v>
+      </c>
+      <c r="C45" t="s">
+        <v>291</v>
+      </c>
+      <c r="D45" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>412</v>
+      </c>
+      <c r="B46" t="s">
+        <v>291</v>
+      </c>
+      <c r="C46" t="s">
+        <v>291</v>
+      </c>
+      <c r="D46" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>417</v>
+      </c>
+      <c r="B47" t="s">
+        <v>291</v>
+      </c>
+      <c r="C47" t="s">
+        <v>299</v>
+      </c>
+      <c r="D47" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" s="18"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" s="18" t="s">
         <v>385</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>383</v>
-      </c>
-      <c r="B34" t="s">
-        <v>292</v>
-      </c>
-      <c r="C34" t="s">
-        <v>292</v>
-      </c>
-      <c r="D34" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>387</v>
-      </c>
-      <c r="B35" t="s">
-        <v>292</v>
-      </c>
-      <c r="C35" t="s">
-        <v>300</v>
-      </c>
-      <c r="D35" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>381</v>
-      </c>
-      <c r="B36" t="s">
-        <v>292</v>
-      </c>
-      <c r="C36" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>388</v>
-      </c>
-      <c r="B37" t="s">
-        <v>292</v>
-      </c>
-      <c r="C37" t="s">
-        <v>300</v>
-      </c>
-      <c r="D37" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>390</v>
-      </c>
-      <c r="B38" t="s">
-        <v>292</v>
-      </c>
-      <c r="C38" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>391</v>
-      </c>
-      <c r="B39" t="s">
-        <v>292</v>
-      </c>
-      <c r="C39" t="s">
-        <v>292</v>
-      </c>
-      <c r="E39" s="19" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>392</v>
-      </c>
-      <c r="B40" t="s">
-        <v>292</v>
-      </c>
-      <c r="C40" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>393</v>
-      </c>
-      <c r="B41" t="s">
-        <v>292</v>
-      </c>
-      <c r="C41" t="s">
-        <v>292</v>
-      </c>
-      <c r="D41" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>410</v>
-      </c>
-      <c r="B42" t="s">
-        <v>292</v>
-      </c>
-      <c r="C42" t="s">
-        <v>300</v>
-      </c>
-      <c r="D42" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>411</v>
-      </c>
-      <c r="B43" t="s">
-        <v>292</v>
-      </c>
-      <c r="C43" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>412</v>
-      </c>
-      <c r="B44" t="s">
-        <v>292</v>
-      </c>
-      <c r="C44" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>414</v>
-      </c>
-      <c r="B45" t="s">
-        <v>300</v>
-      </c>
-      <c r="C45" t="s">
-        <v>292</v>
-      </c>
-      <c r="D45" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>413</v>
-      </c>
-      <c r="B46" t="s">
-        <v>292</v>
-      </c>
-      <c r="C46" t="s">
-        <v>292</v>
-      </c>
-      <c r="D46" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>418</v>
-      </c>
-      <c r="B47" t="s">
-        <v>292</v>
-      </c>
-      <c r="C47" t="s">
-        <v>300</v>
-      </c>
-      <c r="D47" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="18"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="18" t="s">
-        <v>386</v>
       </c>
     </row>
   </sheetData>
@@ -5299,38 +5296,38 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="63" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>405</v>
+      </c>
+      <c r="B2" t="s">
         <v>406</v>
       </c>
-      <c r="B2" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>